<commit_message>
Minor update of census, collection and environment files
</commit_message>
<xml_diff>
--- a/docs/Census_Wsc_Services.xlsx
+++ b/docs/Census_Wsc_Services.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian.catelli/Google Drive (christian.catelli@kineton.it)/Sky/Automation IT CI:CD WSC/Repository/PostmanCollection_AutomationAPI/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8887EB5-6942-8B46-97BF-AF308DBC6ED1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B78D343-9B7C-C148-A9E2-29EA2D7FEF6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{8656BBE8-7E17-AC42-8AF4-F6E9122F8590}"/>
   </bookViews>
@@ -696,7 +696,7 @@
     <t>Err 422</t>
   </si>
   <si>
-    <t>Err 406</t>
+    <t>Err 406, check application/pdf - json</t>
   </si>
 </sst>
 </file>
@@ -1226,7 +1226,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N183"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" workbookViewId="0">
       <selection activeCell="D124" sqref="D124"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Data file added. Collection, environment and census updated
</commit_message>
<xml_diff>
--- a/docs/Census_Wsc_Services.xlsx
+++ b/docs/Census_Wsc_Services.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian.catelli/Google Drive (christian.catelli@kineton.it)/Sky/Automation IT CI:CD WSC/Repository/PostmanCollection_AutomationAPI/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1680D0B9-C494-DE44-898B-65B7ECB6BA86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488686B8-735E-AC49-AA57-CB71BE74B752}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{8656BBE8-7E17-AC42-8AF4-F6E9122F8590}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8656BBE8-7E17-AC42-8AF4-F6E9122F8590}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="232">
   <si>
     <t>Service Category</t>
   </si>
@@ -715,13 +715,28 @@
   </si>
   <si>
     <t>Err 404, check in progress by QA. Check URL</t>
+  </si>
+  <si>
+    <t>Monocontratto</t>
+  </si>
+  <si>
+    <t>Utenza</t>
+  </si>
+  <si>
+    <t>Caratteristiche</t>
+  </si>
+  <si>
+    <t>Attivo, monocontratto, DTH, smc censita. Consistenza: sky famiglia, go, kids, on demand e almeno un canale opzione. Eleggibile Sky Sport. Consistenza ulteriore: sky q black.</t>
+  </si>
+  <si>
+    <t>Attivo, Sky via Fibra in preattivazione, completo.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -790,6 +805,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -847,7 +868,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -925,15 +946,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -951,6 +963,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1270,7 +1292,7 @@
   <dimension ref="A1:O183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+      <selection activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1286,25 +1308,27 @@
     <col min="9" max="9" width="40" style="5" customWidth="1"/>
     <col min="10" max="10" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="35.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="10.83203125" style="5"/>
+    <col min="12" max="12" width="7.83203125" style="33" customWidth="1"/>
+    <col min="13" max="13" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="146" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="27" t="s">
         <v>220</v>
       </c>
       <c r="F1" s="8" t="s">
@@ -1316,25 +1340,40 @@
       <c r="H1" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="31" t="s">
         <v>205</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="31" t="s">
         <v>208</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="O1" s="35"/>
-    </row>
-    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L1" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="O1" s="32"/>
+    </row>
+    <row r="2" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="F2" s="10"/>
       <c r="G2" s="17"/>
       <c r="H2" s="10"/>
+      <c r="M2" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>230</v>
+      </c>
       <c r="O2" s="9"/>
     </row>
-    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -1347,20 +1386,26 @@
       <c r="G3" s="19" t="s">
         <v>200</v>
       </c>
+      <c r="M3" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="O3" s="22"/>
     </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="O4" s="22"/>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
       <c r="D5" s="16" t="s">
         <v>5</v>
       </c>
@@ -1375,10 +1420,10 @@
       </c>
       <c r="O5" s="22"/>
     </row>
-    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="29"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
+    <row r="6" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="16" t="s">
         <v>6</v>
       </c>
@@ -1393,10 +1438,10 @@
       </c>
       <c r="O6" s="22"/>
     </row>
-    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="29"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
+    <row r="7" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="16" t="s">
         <v>7</v>
       </c>
@@ -1411,10 +1456,10 @@
       </c>
       <c r="O7" s="22"/>
     </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
+    <row r="8" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="34"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="16" t="s">
         <v>8</v>
       </c>
@@ -1429,10 +1474,10 @@
       </c>
       <c r="O8" s="22"/>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="29"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
+    <row r="9" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="16" t="s">
         <v>9</v>
       </c>
@@ -1446,10 +1491,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="29"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
+    <row r="10" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="16" t="s">
         <v>10</v>
       </c>
@@ -1463,10 +1508,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="29"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
+    <row r="11" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
       <c r="D11" s="16" t="s">
         <v>11</v>
       </c>
@@ -1480,10 +1525,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="29"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
+    <row r="12" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
       <c r="D12" s="16" t="s">
         <v>12</v>
       </c>
@@ -1497,10 +1542,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="29"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
+    <row r="13" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="16" t="s">
         <v>13</v>
       </c>
@@ -1514,10 +1559,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="29"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
+    <row r="14" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
       <c r="D14" s="16" t="s">
         <v>14</v>
       </c>
@@ -1531,10 +1576,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="29"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
+    <row r="15" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
       <c r="D15" s="16" t="s">
         <v>15</v>
       </c>
@@ -1548,10 +1593,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="29"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
+    <row r="16" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="16" t="s">
         <v>16</v>
       </c>
@@ -1565,10 +1610,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
+    <row r="17" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="34"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
       <c r="D17" s="16" t="s">
         <v>17</v>
       </c>
@@ -1582,10 +1627,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
+    <row r="18" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="34"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
       <c r="D18" s="16" t="s">
         <v>18</v>
       </c>
@@ -1599,10 +1644,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="29"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
+    <row r="19" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
       <c r="D19" s="16" t="s">
         <v>19</v>
       </c>
@@ -1616,17 +1661,17 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="29" t="s">
+    <row r="21" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
       <c r="D21" s="16" t="s">
         <v>21</v>
       </c>
@@ -1638,10 +1683,10 @@
       </c>
       <c r="G21" s="12"/>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="29"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
+    <row r="22" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
       <c r="D22" s="16" t="s">
         <v>24</v>
       </c>
@@ -1653,10 +1698,10 @@
       </c>
       <c r="G22" s="12"/>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="29"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
+    <row r="23" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
       <c r="D23" s="16" t="s">
         <v>25</v>
       </c>
@@ -1668,10 +1713,10 @@
       </c>
       <c r="G23" s="12"/>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="29"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
+    <row r="24" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
       <c r="D24" s="16" t="s">
         <v>26</v>
       </c>
@@ -1683,10 +1728,10 @@
       </c>
       <c r="G24" s="12"/>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="29"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
+    <row r="25" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
       <c r="D25" s="16" t="s">
         <v>27</v>
       </c>
@@ -1698,17 +1743,17 @@
       </c>
       <c r="G25" s="12"/>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
       <c r="D27" s="16" t="s">
         <v>30</v>
       </c>
@@ -1731,10 +1776,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="29"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
+    <row r="28" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="34"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
       <c r="D28" s="16" t="s">
         <v>31</v>
       </c>
@@ -1746,17 +1791,17 @@
       </c>
       <c r="G28" s="13"/>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="29" t="s">
+    <row r="30" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
       <c r="D30" s="16" t="s">
         <v>34</v>
       </c>
@@ -1779,10 +1824,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="29"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
+    <row r="31" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
       <c r="D31" s="16" t="s">
         <v>35</v>
       </c>
@@ -1808,10 +1853,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="29"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
+    <row r="32" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="34"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
       <c r="D32" s="16" t="s">
         <v>36</v>
       </c>
@@ -1823,10 +1868,10 @@
       </c>
       <c r="G32" s="14"/>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="29"/>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
+    <row r="33" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
       <c r="D33" s="16" t="s">
         <v>37</v>
       </c>
@@ -1838,17 +1883,17 @@
       </c>
       <c r="G33" s="14"/>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="29" t="s">
+    <row r="35" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
       <c r="D35" s="16" t="s">
         <v>40</v>
       </c>
@@ -1860,10 +1905,10 @@
       </c>
       <c r="G35" s="13"/>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="29"/>
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
+    <row r="36" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="34"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
       <c r="D36" s="16" t="s">
         <v>41</v>
       </c>
@@ -1883,10 +1928,10 @@
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="29"/>
-      <c r="B37" s="29"/>
-      <c r="C37" s="29"/>
+    <row r="37" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="34"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
       <c r="D37" s="16" t="s">
         <v>42</v>
       </c>
@@ -1906,12 +1951,12 @@
         <v>206</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="24" t="s">
         <v>43</v>
       </c>
@@ -1934,17 +1979,17 @@
         <v>214</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="29" t="s">
+    <row r="41" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="29"/>
-      <c r="C41" s="29"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
       <c r="D41" s="16" t="s">
         <v>46</v>
       </c>
@@ -1956,10 +2001,10 @@
       </c>
       <c r="G41" s="12"/>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="29"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
+    <row r="42" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="34"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="34"/>
       <c r="D42" s="16" t="s">
         <v>47</v>
       </c>
@@ -1971,23 +2016,23 @@
       </c>
       <c r="G42" s="12"/>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="29" t="s">
+    <row r="44" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="29" t="s">
+      <c r="B44" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="29"/>
+      <c r="C44" s="34"/>
       <c r="D44" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E44" s="31" t="s">
+      <c r="E44" s="28" t="s">
         <v>223</v>
       </c>
       <c r="F44" s="12" t="s">
@@ -1995,14 +2040,14 @@
       </c>
       <c r="G44" s="12"/>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="29"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
+    <row r="45" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="34"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
       <c r="D45" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="31" t="s">
+      <c r="E45" s="28" t="s">
         <v>223</v>
       </c>
       <c r="F45" s="12" t="s">
@@ -2011,13 +2056,13 @@
       <c r="G45" s="12"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="34"/>
       <c r="D46" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E46" s="31" t="s">
+      <c r="E46" s="28" t="s">
         <v>223</v>
       </c>
       <c r="F46" s="11" t="s">
@@ -2037,13 +2082,13 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="29"/>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
+      <c r="A47" s="34"/>
+      <c r="B47" s="34"/>
+      <c r="C47" s="34"/>
       <c r="D47" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E47" s="31" t="s">
+      <c r="E47" s="28" t="s">
         <v>223</v>
       </c>
       <c r="F47" s="11" t="s">
@@ -2065,12 +2110,12 @@
         <v>214</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="29"/>
-      <c r="B48" s="29" t="s">
+    <row r="48" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="34"/>
+      <c r="B48" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="C48" s="29"/>
+      <c r="C48" s="34"/>
       <c r="D48" s="16" t="s">
         <v>56</v>
       </c>
@@ -2079,10 +2124,10 @@
       </c>
       <c r="G48" s="12"/>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="29"/>
-      <c r="B49" s="29"/>
-      <c r="C49" s="29"/>
+    <row r="49" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="34"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="34"/>
       <c r="D49" s="16" t="s">
         <v>57</v>
       </c>
@@ -2092,11 +2137,11 @@
       <c r="G49" s="12"/>
     </row>
     <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="29"/>
-      <c r="B50" s="29" t="s">
+      <c r="A50" s="34"/>
+      <c r="B50" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C50" s="29"/>
+      <c r="C50" s="34"/>
       <c r="D50" s="16" t="s">
         <v>59</v>
       </c>
@@ -2111,9 +2156,9 @@
       </c>
     </row>
     <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="29"/>
-      <c r="B51" s="29"/>
-      <c r="C51" s="29"/>
+      <c r="A51" s="34"/>
+      <c r="B51" s="34"/>
+      <c r="C51" s="34"/>
       <c r="D51" s="16" t="s">
         <v>60</v>
       </c>
@@ -2128,15 +2173,15 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" s="29"/>
-      <c r="B52" s="29" t="s">
+      <c r="A52" s="34"/>
+      <c r="B52" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="C52" s="29"/>
+      <c r="C52" s="34"/>
       <c r="D52" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E52" s="31" t="s">
+      <c r="E52" s="28" t="s">
         <v>223</v>
       </c>
       <c r="F52" s="11" t="s">
@@ -2156,13 +2201,13 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" s="29"/>
-      <c r="B53" s="29"/>
-      <c r="C53" s="29"/>
+      <c r="A53" s="34"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="34"/>
       <c r="D53" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E53" s="31" t="s">
+      <c r="E53" s="28" t="s">
         <v>223</v>
       </c>
       <c r="F53" s="11" t="s">
@@ -2184,8 +2229,8 @@
         <v>212</v>
       </c>
     </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="29"/>
+    <row r="54" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="34"/>
       <c r="B54" s="7" t="s">
         <v>64</v>
       </c>
@@ -2199,8 +2244,8 @@
         <v>202</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="29"/>
+    <row r="55" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="34"/>
       <c r="B55" s="7" t="s">
         <v>66</v>
       </c>
@@ -2215,11 +2260,11 @@
       </c>
     </row>
     <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="29"/>
-      <c r="B56" s="29" t="s">
+      <c r="A56" s="34"/>
+      <c r="B56" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="C56" s="29" t="s">
+      <c r="C56" s="34" t="s">
         <v>68</v>
       </c>
       <c r="D56" s="16" t="s">
@@ -2236,9 +2281,9 @@
       </c>
     </row>
     <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="29"/>
-      <c r="B57" s="29"/>
-      <c r="C57" s="29"/>
+      <c r="A57" s="34"/>
+      <c r="B57" s="34"/>
+      <c r="C57" s="34"/>
       <c r="D57" s="16" t="s">
         <v>70</v>
       </c>
@@ -2253,9 +2298,9 @@
       </c>
     </row>
     <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="29"/>
-      <c r="B58" s="29"/>
-      <c r="C58" s="29"/>
+      <c r="A58" s="34"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="34"/>
       <c r="D58" s="16" t="s">
         <v>73</v>
       </c>
@@ -2270,9 +2315,9 @@
       </c>
     </row>
     <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="29"/>
-      <c r="B59" s="29"/>
-      <c r="C59" s="29"/>
+      <c r="A59" s="34"/>
+      <c r="B59" s="34"/>
+      <c r="C59" s="34"/>
       <c r="D59" s="16" t="s">
         <v>74</v>
       </c>
@@ -2287,9 +2332,9 @@
       </c>
     </row>
     <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="29"/>
-      <c r="B60" s="29"/>
-      <c r="C60" s="29"/>
+      <c r="A60" s="34"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="34"/>
       <c r="D60" s="16" t="s">
         <v>75</v>
       </c>
@@ -2303,12 +2348,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="29"/>
-      <c r="B61" s="29" t="s">
+    <row r="61" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="34"/>
+      <c r="B61" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="C61" s="29"/>
+      <c r="C61" s="34"/>
       <c r="D61" s="16" t="s">
         <v>77</v>
       </c>
@@ -2320,10 +2365,10 @@
       </c>
       <c r="G61" s="12"/>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="29"/>
-      <c r="B62" s="29"/>
-      <c r="C62" s="29"/>
+    <row r="62" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="34"/>
+      <c r="B62" s="34"/>
+      <c r="C62" s="34"/>
       <c r="D62" s="16" t="s">
         <v>78</v>
       </c>
@@ -2335,10 +2380,10 @@
       </c>
       <c r="G62" s="12"/>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="29"/>
-      <c r="B63" s="29"/>
-      <c r="C63" s="29"/>
+    <row r="63" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="34"/>
+      <c r="B63" s="34"/>
+      <c r="C63" s="34"/>
       <c r="D63" s="16" t="s">
         <v>79</v>
       </c>
@@ -2350,12 +2395,12 @@
       </c>
       <c r="G63" s="12"/>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="29"/>
-      <c r="B64" s="29" t="s">
+    <row r="64" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="34"/>
+      <c r="B64" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="C64" s="29"/>
+      <c r="C64" s="34"/>
       <c r="D64" s="16" t="s">
         <v>81</v>
       </c>
@@ -2367,10 +2412,10 @@
       </c>
       <c r="G64" s="12"/>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="29"/>
-      <c r="B65" s="29"/>
-      <c r="C65" s="29"/>
+    <row r="65" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="34"/>
+      <c r="B65" s="34"/>
+      <c r="C65" s="34"/>
       <c r="D65" s="16" t="s">
         <v>82</v>
       </c>
@@ -2382,10 +2427,10 @@
       </c>
       <c r="G65" s="12"/>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="29"/>
-      <c r="B66" s="29"/>
-      <c r="C66" s="29"/>
+    <row r="66" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="34"/>
+      <c r="B66" s="34"/>
+      <c r="C66" s="34"/>
       <c r="D66" s="16" t="s">
         <v>83</v>
       </c>
@@ -2398,9 +2443,9 @@
       <c r="G66" s="12"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A67" s="29"/>
-      <c r="B67" s="29"/>
-      <c r="C67" s="29"/>
+      <c r="A67" s="34"/>
+      <c r="B67" s="34"/>
+      <c r="C67" s="34"/>
       <c r="D67" s="16" t="s">
         <v>84</v>
       </c>
@@ -2423,10 +2468,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="29"/>
-      <c r="B68" s="29"/>
-      <c r="C68" s="29"/>
+    <row r="68" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="34"/>
+      <c r="B68" s="34"/>
+      <c r="C68" s="34"/>
       <c r="D68" s="16" t="s">
         <v>85</v>
       </c>
@@ -2447,9 +2492,9 @@
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69" s="29"/>
-      <c r="B69" s="29"/>
-      <c r="C69" s="29"/>
+      <c r="A69" s="34"/>
+      <c r="B69" s="34"/>
+      <c r="C69" s="34"/>
       <c r="D69" s="16" t="s">
         <v>86</v>
       </c>
@@ -2473,9 +2518,9 @@
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A70" s="29"/>
-      <c r="B70" s="29"/>
-      <c r="C70" s="29"/>
+      <c r="A70" s="34"/>
+      <c r="B70" s="34"/>
+      <c r="C70" s="34"/>
       <c r="D70" s="16" t="s">
         <v>87</v>
       </c>
@@ -2499,9 +2544,9 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A71" s="29"/>
-      <c r="B71" s="29"/>
-      <c r="C71" s="29"/>
+      <c r="A71" s="34"/>
+      <c r="B71" s="34"/>
+      <c r="C71" s="34"/>
       <c r="D71" s="16" t="s">
         <v>88</v>
       </c>
@@ -2525,9 +2570,9 @@
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A72" s="29"/>
-      <c r="B72" s="29"/>
-      <c r="C72" s="29"/>
+      <c r="A72" s="34"/>
+      <c r="B72" s="34"/>
+      <c r="C72" s="34"/>
       <c r="D72" s="16" t="s">
         <v>89</v>
       </c>
@@ -2551,9 +2596,9 @@
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A73" s="29"/>
-      <c r="B73" s="29"/>
-      <c r="C73" s="29"/>
+      <c r="A73" s="34"/>
+      <c r="B73" s="34"/>
+      <c r="C73" s="34"/>
       <c r="D73" s="16" t="s">
         <v>90</v>
       </c>
@@ -2580,9 +2625,9 @@
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A74" s="29"/>
-      <c r="B74" s="29"/>
-      <c r="C74" s="29"/>
+      <c r="A74" s="34"/>
+      <c r="B74" s="34"/>
+      <c r="C74" s="34"/>
       <c r="D74" s="16" t="s">
         <v>91</v>
       </c>
@@ -2609,9 +2654,9 @@
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A75" s="29"/>
-      <c r="B75" s="29"/>
-      <c r="C75" s="29"/>
+      <c r="A75" s="34"/>
+      <c r="B75" s="34"/>
+      <c r="C75" s="34"/>
       <c r="D75" s="16" t="s">
         <v>92</v>
       </c>
@@ -2634,10 +2679,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="29"/>
-      <c r="B76" s="29"/>
-      <c r="C76" s="29"/>
+    <row r="76" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="34"/>
+      <c r="B76" s="34"/>
+      <c r="C76" s="34"/>
       <c r="D76" s="16" t="s">
         <v>93</v>
       </c>
@@ -2660,10 +2705,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="29"/>
-      <c r="B77" s="29"/>
-      <c r="C77" s="29"/>
+    <row r="77" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="34"/>
+      <c r="B77" s="34"/>
+      <c r="C77" s="34"/>
       <c r="D77" s="16" t="s">
         <v>94</v>
       </c>
@@ -2684,9 +2729,9 @@
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A78" s="29"/>
-      <c r="B78" s="29"/>
-      <c r="C78" s="29"/>
+      <c r="A78" s="34"/>
+      <c r="B78" s="34"/>
+      <c r="C78" s="34"/>
       <c r="D78" s="16" t="s">
         <v>95</v>
       </c>
@@ -2709,10 +2754,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="29"/>
-      <c r="B79" s="29"/>
-      <c r="C79" s="29"/>
+    <row r="79" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="34"/>
+      <c r="B79" s="34"/>
+      <c r="C79" s="34"/>
       <c r="D79" s="24" t="s">
         <v>96</v>
       </c>
@@ -2735,10 +2780,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="29"/>
-      <c r="B80" s="29"/>
-      <c r="C80" s="29"/>
+    <row r="80" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="34"/>
+      <c r="B80" s="34"/>
+      <c r="C80" s="34"/>
       <c r="D80" s="24" t="s">
         <v>97</v>
       </c>
@@ -2758,10 +2803,10 @@
         <v>215</v>
       </c>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="29"/>
-      <c r="B81" s="29"/>
-      <c r="C81" s="29"/>
+    <row r="81" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="34"/>
+      <c r="B81" s="34"/>
+      <c r="C81" s="34"/>
       <c r="D81" s="16" t="s">
         <v>98</v>
       </c>
@@ -2774,9 +2819,9 @@
       <c r="G81" s="13"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A82" s="29"/>
-      <c r="B82" s="29"/>
-      <c r="C82" s="29"/>
+      <c r="A82" s="34"/>
+      <c r="B82" s="34"/>
+      <c r="C82" s="34"/>
       <c r="D82" s="24" t="s">
         <v>99</v>
       </c>
@@ -2802,10 +2847,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="29"/>
-      <c r="B83" s="29"/>
-      <c r="C83" s="29"/>
+    <row r="83" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="34"/>
+      <c r="B83" s="34"/>
+      <c r="C83" s="34"/>
       <c r="D83" s="24" t="s">
         <v>100</v>
       </c>
@@ -2831,10 +2876,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="29"/>
-      <c r="B84" s="29"/>
-      <c r="C84" s="29"/>
+    <row r="84" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="34"/>
+      <c r="B84" s="34"/>
+      <c r="C84" s="34"/>
       <c r="D84" s="24" t="s">
         <v>101</v>
       </c>
@@ -2860,10 +2905,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="29"/>
-      <c r="B85" s="29"/>
-      <c r="C85" s="29"/>
+    <row r="85" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="34"/>
+      <c r="B85" s="34"/>
+      <c r="C85" s="34"/>
       <c r="D85" s="24" t="s">
         <v>102</v>
       </c>
@@ -2889,10 +2934,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="29"/>
-      <c r="B86" s="29"/>
-      <c r="C86" s="29"/>
+    <row r="86" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="34"/>
+      <c r="B86" s="34"/>
+      <c r="C86" s="34"/>
       <c r="D86" s="24" t="s">
         <v>103</v>
       </c>
@@ -2918,10 +2963,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="29"/>
-      <c r="B87" s="29"/>
-      <c r="C87" s="29"/>
+    <row r="87" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="34"/>
+      <c r="B87" s="34"/>
+      <c r="C87" s="34"/>
       <c r="D87" s="16" t="s">
         <v>104</v>
       </c>
@@ -2933,10 +2978,10 @@
       </c>
       <c r="G87" s="13"/>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="29"/>
-      <c r="B88" s="29"/>
-      <c r="C88" s="29"/>
+    <row r="88" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="34"/>
+      <c r="B88" s="34"/>
+      <c r="C88" s="34"/>
       <c r="D88" s="16" t="s">
         <v>105</v>
       </c>
@@ -2948,10 +2993,10 @@
       </c>
       <c r="G88" s="13"/>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="29"/>
-      <c r="B89" s="29"/>
-      <c r="C89" s="29"/>
+    <row r="89" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="34"/>
+      <c r="B89" s="34"/>
+      <c r="C89" s="34"/>
       <c r="D89" s="16" t="s">
         <v>106</v>
       </c>
@@ -2963,10 +3008,10 @@
       </c>
       <c r="G89" s="13"/>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="29"/>
-      <c r="B90" s="29"/>
-      <c r="C90" s="29"/>
+    <row r="90" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="34"/>
+      <c r="B90" s="34"/>
+      <c r="C90" s="34"/>
       <c r="D90" s="16" t="s">
         <v>107</v>
       </c>
@@ -2978,10 +3023,10 @@
       </c>
       <c r="G90" s="13"/>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="29"/>
-      <c r="B91" s="29"/>
-      <c r="C91" s="29"/>
+    <row r="91" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="34"/>
+      <c r="B91" s="34"/>
+      <c r="C91" s="34"/>
       <c r="D91" s="16" t="s">
         <v>108</v>
       </c>
@@ -2993,10 +3038,10 @@
       </c>
       <c r="G91" s="13"/>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="29"/>
-      <c r="B92" s="29"/>
-      <c r="C92" s="29"/>
+    <row r="92" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="34"/>
+      <c r="B92" s="34"/>
+      <c r="C92" s="34"/>
       <c r="D92" s="16" t="s">
         <v>109</v>
       </c>
@@ -3008,10 +3053,10 @@
       </c>
       <c r="G92" s="13"/>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="29"/>
-      <c r="B93" s="29"/>
-      <c r="C93" s="29"/>
+    <row r="93" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="34"/>
+      <c r="B93" s="34"/>
+      <c r="C93" s="34"/>
       <c r="D93" s="16" t="s">
         <v>110</v>
       </c>
@@ -3024,9 +3069,9 @@
       <c r="G93" s="13"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A94" s="29"/>
-      <c r="B94" s="29"/>
-      <c r="C94" s="29"/>
+      <c r="A94" s="34"/>
+      <c r="B94" s="34"/>
+      <c r="C94" s="34"/>
       <c r="D94" s="24" t="s">
         <v>111</v>
       </c>
@@ -3050,9 +3095,9 @@
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A95" s="29"/>
-      <c r="B95" s="29"/>
-      <c r="C95" s="29"/>
+      <c r="A95" s="34"/>
+      <c r="B95" s="34"/>
+      <c r="C95" s="34"/>
       <c r="D95" s="24" t="s">
         <v>112</v>
       </c>
@@ -3075,10 +3120,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="29"/>
-      <c r="B96" s="29"/>
-      <c r="C96" s="29"/>
+    <row r="96" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="34"/>
+      <c r="B96" s="34"/>
+      <c r="C96" s="34"/>
       <c r="D96" s="16" t="s">
         <v>113</v>
       </c>
@@ -3090,10 +3135,10 @@
       </c>
       <c r="G96" s="12"/>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="29"/>
-      <c r="B97" s="29"/>
-      <c r="C97" s="29"/>
+    <row r="97" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="34"/>
+      <c r="B97" s="34"/>
+      <c r="C97" s="34"/>
       <c r="D97" s="16" t="s">
         <v>114</v>
       </c>
@@ -3106,9 +3151,9 @@
       <c r="G97" s="12"/>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A98" s="29"/>
-      <c r="B98" s="29"/>
-      <c r="C98" s="29"/>
+      <c r="A98" s="34"/>
+      <c r="B98" s="34"/>
+      <c r="C98" s="34"/>
       <c r="D98" s="24" t="s">
         <v>115</v>
       </c>
@@ -3131,17 +3176,17 @@
         <v>214</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="7"/>
       <c r="F99" s="11"/>
       <c r="G99" s="11"/>
     </row>
     <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="27" t="s">
+      <c r="A100" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="B100" s="27"/>
-      <c r="C100" s="27"/>
+      <c r="B100" s="35"/>
+      <c r="C100" s="35"/>
       <c r="D100" s="16" t="s">
         <v>117</v>
       </c>
@@ -3156,9 +3201,9 @@
       </c>
     </row>
     <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="27"/>
-      <c r="B101" s="27"/>
-      <c r="C101" s="27"/>
+      <c r="A101" s="35"/>
+      <c r="B101" s="35"/>
+      <c r="C101" s="35"/>
       <c r="D101" s="16" t="s">
         <v>118</v>
       </c>
@@ -3173,9 +3218,9 @@
       </c>
     </row>
     <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="27"/>
-      <c r="B102" s="27"/>
-      <c r="C102" s="27"/>
+      <c r="A102" s="35"/>
+      <c r="B102" s="35"/>
+      <c r="C102" s="35"/>
       <c r="D102" s="16" t="s">
         <v>119</v>
       </c>
@@ -3190,9 +3235,9 @@
       </c>
     </row>
     <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="27"/>
-      <c r="B103" s="27"/>
-      <c r="C103" s="27"/>
+      <c r="A103" s="35"/>
+      <c r="B103" s="35"/>
+      <c r="C103" s="35"/>
       <c r="D103" s="16" t="s">
         <v>120</v>
       </c>
@@ -3206,10 +3251,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="29"/>
-      <c r="B104" s="27"/>
-      <c r="C104" s="27"/>
+    <row r="104" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="34"/>
+      <c r="B104" s="35"/>
+      <c r="C104" s="35"/>
       <c r="D104" s="16" t="s">
         <v>121</v>
       </c>
@@ -3221,10 +3266,10 @@
       </c>
       <c r="G104" s="12"/>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="29"/>
-      <c r="B105" s="27"/>
-      <c r="C105" s="27"/>
+    <row r="105" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="34"/>
+      <c r="B105" s="35"/>
+      <c r="C105" s="35"/>
       <c r="D105" s="16" t="s">
         <v>122</v>
       </c>
@@ -3236,10 +3281,10 @@
       </c>
       <c r="G105" s="12"/>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="29"/>
-      <c r="B106" s="27"/>
-      <c r="C106" s="27"/>
+    <row r="106" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="34"/>
+      <c r="B106" s="35"/>
+      <c r="C106" s="35"/>
       <c r="D106" s="16" t="s">
         <v>123</v>
       </c>
@@ -3251,10 +3296,10 @@
       </c>
       <c r="G106" s="12"/>
     </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="29"/>
-      <c r="B107" s="27"/>
-      <c r="C107" s="27"/>
+    <row r="107" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="34"/>
+      <c r="B107" s="35"/>
+      <c r="C107" s="35"/>
       <c r="D107" s="16" t="s">
         <v>124</v>
       </c>
@@ -3266,10 +3311,10 @@
       </c>
       <c r="G107" s="12"/>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="29"/>
-      <c r="B108" s="27"/>
-      <c r="C108" s="27"/>
+    <row r="108" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="34"/>
+      <c r="B108" s="35"/>
+      <c r="C108" s="35"/>
       <c r="D108" s="16" t="s">
         <v>125</v>
       </c>
@@ -3281,10 +3326,10 @@
       </c>
       <c r="G108" s="12"/>
     </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="29"/>
-      <c r="B109" s="27"/>
-      <c r="C109" s="27"/>
+    <row r="109" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="34"/>
+      <c r="B109" s="35"/>
+      <c r="C109" s="35"/>
       <c r="D109" s="16" t="s">
         <v>126</v>
       </c>
@@ -3296,10 +3341,10 @@
       </c>
       <c r="G109" s="12"/>
     </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="29"/>
-      <c r="B110" s="27"/>
-      <c r="C110" s="27"/>
+    <row r="110" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="34"/>
+      <c r="B110" s="35"/>
+      <c r="C110" s="35"/>
       <c r="D110" s="16" t="s">
         <v>127</v>
       </c>
@@ -3311,10 +3356,10 @@
       </c>
       <c r="G110" s="12"/>
     </row>
-    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="29"/>
-      <c r="B111" s="27"/>
-      <c r="C111" s="27"/>
+    <row r="111" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="34"/>
+      <c r="B111" s="35"/>
+      <c r="C111" s="35"/>
       <c r="D111" s="16" t="s">
         <v>128</v>
       </c>
@@ -3326,10 +3371,10 @@
       </c>
       <c r="G111" s="12"/>
     </row>
-    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="29"/>
-      <c r="B112" s="27"/>
-      <c r="C112" s="27"/>
+    <row r="112" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="34"/>
+      <c r="B112" s="35"/>
+      <c r="C112" s="35"/>
       <c r="D112" s="16" t="s">
         <v>129</v>
       </c>
@@ -3341,10 +3386,10 @@
       </c>
       <c r="G112" s="13"/>
     </row>
-    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="29"/>
-      <c r="B113" s="27"/>
-      <c r="C113" s="27"/>
+    <row r="113" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="34"/>
+      <c r="B113" s="35"/>
+      <c r="C113" s="35"/>
       <c r="D113" s="16" t="s">
         <v>130</v>
       </c>
@@ -3357,9 +3402,9 @@
       <c r="G113" s="13"/>
     </row>
     <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="27"/>
-      <c r="B114" s="27"/>
-      <c r="C114" s="27"/>
+      <c r="A114" s="35"/>
+      <c r="B114" s="35"/>
+      <c r="C114" s="35"/>
       <c r="D114" s="16" t="s">
         <v>131</v>
       </c>
@@ -3374,9 +3419,9 @@
       </c>
     </row>
     <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="27"/>
-      <c r="B115" s="27"/>
-      <c r="C115" s="27"/>
+      <c r="A115" s="35"/>
+      <c r="B115" s="35"/>
+      <c r="C115" s="35"/>
       <c r="D115" s="16" t="s">
         <v>132</v>
       </c>
@@ -3390,15 +3435,15 @@
         <v>202</v>
       </c>
     </row>
-    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="7"/>
     </row>
-    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="27" t="s">
+    <row r="117" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="B117" s="27"/>
-      <c r="C117" s="27"/>
+      <c r="B117" s="35"/>
+      <c r="C117" s="35"/>
       <c r="D117" s="16" t="s">
         <v>134</v>
       </c>
@@ -3410,10 +3455,10 @@
       </c>
       <c r="G117" s="12"/>
     </row>
-    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="27"/>
-      <c r="B118" s="27"/>
-      <c r="C118" s="27"/>
+    <row r="118" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="35"/>
+      <c r="B118" s="35"/>
+      <c r="C118" s="35"/>
       <c r="D118" s="16" t="s">
         <v>135</v>
       </c>
@@ -3425,17 +3470,17 @@
       </c>
       <c r="G118" s="12"/>
     </row>
-    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="7"/>
     </row>
     <row r="120" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="29" t="s">
+      <c r="A120" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="B120" s="27" t="s">
+      <c r="B120" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="C120" s="27"/>
+      <c r="C120" s="35"/>
       <c r="D120" s="16" t="s">
         <v>138</v>
       </c>
@@ -3450,9 +3495,9 @@
       </c>
     </row>
     <row r="121" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="29"/>
-      <c r="B121" s="27"/>
-      <c r="C121" s="27"/>
+      <c r="A121" s="34"/>
+      <c r="B121" s="35"/>
+      <c r="C121" s="35"/>
       <c r="D121" s="16" t="s">
         <v>139</v>
       </c>
@@ -3467,9 +3512,9 @@
       </c>
     </row>
     <row r="122" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="29"/>
-      <c r="B122" s="27"/>
-      <c r="C122" s="27"/>
+      <c r="A122" s="34"/>
+      <c r="B122" s="35"/>
+      <c r="C122" s="35"/>
       <c r="D122" s="16" t="s">
         <v>140</v>
       </c>
@@ -3484,9 +3529,9 @@
       </c>
     </row>
     <row r="123" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="29"/>
-      <c r="B123" s="27"/>
-      <c r="C123" s="27"/>
+      <c r="A123" s="34"/>
+      <c r="B123" s="35"/>
+      <c r="C123" s="35"/>
       <c r="D123" s="16" t="s">
         <v>141</v>
       </c>
@@ -3500,10 +3545,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="29"/>
-      <c r="B124" s="27"/>
-      <c r="C124" s="27"/>
+    <row r="124" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="34"/>
+      <c r="B124" s="35"/>
+      <c r="C124" s="35"/>
       <c r="D124" s="24" t="s">
         <v>142</v>
       </c>
@@ -3526,10 +3571,10 @@
         <v>212</v>
       </c>
     </row>
-    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="29"/>
-      <c r="B125" s="27"/>
-      <c r="C125" s="27"/>
+    <row r="125" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="34"/>
+      <c r="B125" s="35"/>
+      <c r="C125" s="35"/>
       <c r="D125" s="24" t="s">
         <v>143</v>
       </c>
@@ -3546,10 +3591,10 @@
         <v>219</v>
       </c>
     </row>
-    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="29"/>
-      <c r="B126" s="27"/>
-      <c r="C126" s="27"/>
+    <row r="126" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="34"/>
+      <c r="B126" s="35"/>
+      <c r="C126" s="35"/>
       <c r="D126" s="24" t="s">
         <v>144</v>
       </c>
@@ -3566,10 +3611,10 @@
         <v>219</v>
       </c>
     </row>
-    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="29"/>
-      <c r="B127" s="27"/>
-      <c r="C127" s="27"/>
+    <row r="127" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="34"/>
+      <c r="B127" s="35"/>
+      <c r="C127" s="35"/>
       <c r="D127" s="24" t="s">
         <v>145</v>
       </c>
@@ -3586,10 +3631,10 @@
         <v>219</v>
       </c>
     </row>
-    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="29"/>
-      <c r="B128" s="27"/>
-      <c r="C128" s="27"/>
+    <row r="128" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="34"/>
+      <c r="B128" s="35"/>
+      <c r="C128" s="35"/>
       <c r="D128" s="24" t="s">
         <v>146</v>
       </c>
@@ -3606,10 +3651,10 @@
         <v>219</v>
       </c>
     </row>
-    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="29"/>
-      <c r="B129" s="27"/>
-      <c r="C129" s="27"/>
+    <row r="129" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="34"/>
+      <c r="B129" s="35"/>
+      <c r="C129" s="35"/>
       <c r="D129" s="24" t="s">
         <v>147</v>
       </c>
@@ -3626,10 +3671,10 @@
         <v>219</v>
       </c>
     </row>
-    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="29"/>
-      <c r="B130" s="27"/>
-      <c r="C130" s="27"/>
+    <row r="130" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="34"/>
+      <c r="B130" s="35"/>
+      <c r="C130" s="35"/>
       <c r="D130" s="24" t="s">
         <v>148</v>
       </c>
@@ -3646,10 +3691,10 @@
         <v>219</v>
       </c>
     </row>
-    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="29"/>
-      <c r="B131" s="27"/>
-      <c r="C131" s="27"/>
+    <row r="131" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="34"/>
+      <c r="B131" s="35"/>
+      <c r="C131" s="35"/>
       <c r="D131" s="24" t="s">
         <v>149</v>
       </c>
@@ -3666,10 +3711,10 @@
         <v>219</v>
       </c>
     </row>
-    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="29"/>
-      <c r="B132" s="27"/>
-      <c r="C132" s="27"/>
+    <row r="132" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="34"/>
+      <c r="B132" s="35"/>
+      <c r="C132" s="35"/>
       <c r="D132" s="24" t="s">
         <v>150</v>
       </c>
@@ -3686,10 +3731,10 @@
         <v>219</v>
       </c>
     </row>
-    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="29"/>
-      <c r="B133" s="27"/>
-      <c r="C133" s="27"/>
+    <row r="133" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="34"/>
+      <c r="B133" s="35"/>
+      <c r="C133" s="35"/>
       <c r="D133" s="24" t="s">
         <v>151</v>
       </c>
@@ -3706,10 +3751,10 @@
         <v>219</v>
       </c>
     </row>
-    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="29"/>
-      <c r="B134" s="27"/>
-      <c r="C134" s="27"/>
+    <row r="134" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="34"/>
+      <c r="B134" s="35"/>
+      <c r="C134" s="35"/>
       <c r="D134" s="24" t="s">
         <v>152</v>
       </c>
@@ -3726,10 +3771,10 @@
         <v>219</v>
       </c>
     </row>
-    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="29"/>
-      <c r="B135" s="27"/>
-      <c r="C135" s="27"/>
+    <row r="135" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="34"/>
+      <c r="B135" s="35"/>
+      <c r="C135" s="35"/>
       <c r="D135" s="24" t="s">
         <v>153</v>
       </c>
@@ -3746,10 +3791,10 @@
         <v>219</v>
       </c>
     </row>
-    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="29"/>
-      <c r="B136" s="27"/>
-      <c r="C136" s="27"/>
+    <row r="136" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="34"/>
+      <c r="B136" s="35"/>
+      <c r="C136" s="35"/>
       <c r="D136" s="24" t="s">
         <v>154</v>
       </c>
@@ -3766,10 +3811,10 @@
         <v>219</v>
       </c>
     </row>
-    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="29"/>
-      <c r="B137" s="27"/>
-      <c r="C137" s="27"/>
+    <row r="137" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="34"/>
+      <c r="B137" s="35"/>
+      <c r="C137" s="35"/>
       <c r="D137" s="24" t="s">
         <v>155</v>
       </c>
@@ -3786,10 +3831,10 @@
         <v>219</v>
       </c>
     </row>
-    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="29"/>
-      <c r="B138" s="27"/>
-      <c r="C138" s="27"/>
+    <row r="138" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="34"/>
+      <c r="B138" s="35"/>
+      <c r="C138" s="35"/>
       <c r="D138" s="24" t="s">
         <v>156</v>
       </c>
@@ -3807,9 +3852,9 @@
       </c>
     </row>
     <row r="139" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="29"/>
-      <c r="B139" s="27"/>
-      <c r="C139" s="27"/>
+      <c r="A139" s="34"/>
+      <c r="B139" s="35"/>
+      <c r="C139" s="35"/>
       <c r="D139" s="16" t="s">
         <v>157</v>
       </c>
@@ -3822,9 +3867,9 @@
       <c r="G139" s="15"/>
     </row>
     <row r="140" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A140" s="29"/>
-      <c r="B140" s="27"/>
-      <c r="C140" s="27"/>
+      <c r="A140" s="34"/>
+      <c r="B140" s="35"/>
+      <c r="C140" s="35"/>
       <c r="D140" s="16" t="s">
         <v>158</v>
       </c>
@@ -3836,17 +3881,17 @@
       </c>
       <c r="G140" s="15"/>
     </row>
-    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="10"/>
       <c r="B141" s="10"/>
       <c r="C141" s="10"/>
     </row>
-    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="27" t="s">
+    <row r="142" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="B142" s="27"/>
-      <c r="C142" s="27"/>
+      <c r="B142" s="35"/>
+      <c r="C142" s="35"/>
       <c r="D142" s="16" t="s">
         <v>160</v>
       </c>
@@ -3858,10 +3903,10 @@
       </c>
       <c r="G142" s="12"/>
     </row>
-    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="27"/>
-      <c r="B143" s="27"/>
-      <c r="C143" s="27"/>
+    <row r="143" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="35"/>
+      <c r="B143" s="35"/>
+      <c r="C143" s="35"/>
       <c r="D143" s="16" t="s">
         <v>160</v>
       </c>
@@ -3873,10 +3918,10 @@
       </c>
       <c r="G143" s="12"/>
     </row>
-    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="27"/>
-      <c r="B144" s="27"/>
-      <c r="C144" s="27"/>
+    <row r="144" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="35"/>
+      <c r="B144" s="35"/>
+      <c r="C144" s="35"/>
       <c r="D144" s="16" t="s">
         <v>161</v>
       </c>
@@ -3888,10 +3933,10 @@
       </c>
       <c r="G144" s="12"/>
     </row>
-    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="27"/>
-      <c r="B145" s="27"/>
-      <c r="C145" s="27"/>
+    <row r="145" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="35"/>
+      <c r="B145" s="35"/>
+      <c r="C145" s="35"/>
       <c r="D145" s="16" t="s">
         <v>162</v>
       </c>
@@ -3903,10 +3948,10 @@
       </c>
       <c r="G145" s="13"/>
     </row>
-    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="27"/>
-      <c r="B146" s="27"/>
-      <c r="C146" s="27"/>
+    <row r="146" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="35"/>
+      <c r="B146" s="35"/>
+      <c r="C146" s="35"/>
       <c r="D146" s="16" t="s">
         <v>163</v>
       </c>
@@ -3918,10 +3963,10 @@
       </c>
       <c r="G146" s="13"/>
     </row>
-    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="7"/>
     </row>
-    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="10" t="s">
         <v>165</v>
       </c>
@@ -3935,15 +3980,15 @@
         <v>202</v>
       </c>
     </row>
-    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="7"/>
     </row>
-    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="27" t="s">
+    <row r="150" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="B150" s="27"/>
-      <c r="C150" s="27"/>
+      <c r="B150" s="35"/>
+      <c r="C150" s="35"/>
       <c r="D150" s="16" t="s">
         <v>168</v>
       </c>
@@ -3957,10 +4002,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="27"/>
-      <c r="B151" s="27"/>
-      <c r="C151" s="27"/>
+    <row r="151" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="35"/>
+      <c r="B151" s="35"/>
+      <c r="C151" s="35"/>
       <c r="D151" s="16" t="s">
         <v>169</v>
       </c>
@@ -3974,15 +4019,15 @@
         <v>200</v>
       </c>
     </row>
-    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="7"/>
     </row>
-    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="27" t="s">
+    <row r="153" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="B153" s="28"/>
-      <c r="C153" s="28"/>
+      <c r="B153" s="36"/>
+      <c r="C153" s="36"/>
       <c r="D153" s="18" t="s">
         <v>171</v>
       </c>
@@ -3994,10 +4039,10 @@
       </c>
       <c r="G153" s="2"/>
     </row>
-    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="27"/>
-      <c r="B154" s="28"/>
-      <c r="C154" s="28"/>
+    <row r="154" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="35"/>
+      <c r="B154" s="36"/>
+      <c r="C154" s="36"/>
       <c r="D154" s="18" t="s">
         <v>172</v>
       </c>
@@ -4009,10 +4054,10 @@
       </c>
       <c r="G154" s="2"/>
     </row>
-    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="27"/>
-      <c r="B155" s="28"/>
-      <c r="C155" s="28"/>
+    <row r="155" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="35"/>
+      <c r="B155" s="36"/>
+      <c r="C155" s="36"/>
       <c r="D155" s="18" t="s">
         <v>173</v>
       </c>
@@ -4024,19 +4069,19 @@
       </c>
       <c r="G155" s="2"/>
     </row>
-    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="7"/>
     </row>
-    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="27" t="s">
+    <row r="157" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="B157" s="28"/>
-      <c r="C157" s="28"/>
+      <c r="B157" s="36"/>
+      <c r="C157" s="36"/>
       <c r="D157" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="E157" s="32" t="s">
+      <c r="E157" s="29" t="s">
         <v>221</v>
       </c>
       <c r="F157" s="1" t="s">
@@ -4046,14 +4091,14 @@
         <v>200</v>
       </c>
     </row>
-    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A158" s="27"/>
-      <c r="B158" s="28"/>
-      <c r="C158" s="28"/>
+    <row r="158" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="35"/>
+      <c r="B158" s="36"/>
+      <c r="C158" s="36"/>
       <c r="D158" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="E158" s="32" t="s">
+      <c r="E158" s="29" t="s">
         <v>221</v>
       </c>
       <c r="F158" s="1" t="s">
@@ -4063,14 +4108,14 @@
         <v>200</v>
       </c>
     </row>
-    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A159" s="27"/>
-      <c r="B159" s="28"/>
-      <c r="C159" s="28"/>
+    <row r="159" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A159" s="35"/>
+      <c r="B159" s="36"/>
+      <c r="C159" s="36"/>
       <c r="D159" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="E159" s="32" t="s">
+      <c r="E159" s="29" t="s">
         <v>221</v>
       </c>
       <c r="F159" s="1" t="s">
@@ -4080,19 +4125,19 @@
         <v>200</v>
       </c>
     </row>
-    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="7"/>
     </row>
-    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="27" t="s">
+    <row r="161" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="B161" s="28"/>
-      <c r="C161" s="28"/>
+      <c r="B161" s="36"/>
+      <c r="C161" s="36"/>
       <c r="D161" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="E161" s="33" t="s">
+      <c r="E161" s="30" t="s">
         <v>223</v>
       </c>
       <c r="F161" s="2" t="s">
@@ -4100,14 +4145,14 @@
       </c>
       <c r="G161" s="2"/>
     </row>
-    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A162" s="27"/>
-      <c r="B162" s="28"/>
-      <c r="C162" s="28"/>
+    <row r="162" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="35"/>
+      <c r="B162" s="36"/>
+      <c r="C162" s="36"/>
       <c r="D162" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="E162" s="33" t="s">
+      <c r="E162" s="30" t="s">
         <v>223</v>
       </c>
       <c r="F162" s="2" t="s">
@@ -4115,14 +4160,14 @@
       </c>
       <c r="G162" s="2"/>
     </row>
-    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="27"/>
-      <c r="B163" s="28"/>
-      <c r="C163" s="28"/>
+    <row r="163" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="35"/>
+      <c r="B163" s="36"/>
+      <c r="C163" s="36"/>
       <c r="D163" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="E163" s="33" t="s">
+      <c r="E163" s="30" t="s">
         <v>221</v>
       </c>
       <c r="F163" s="2" t="s">
@@ -4130,10 +4175,10 @@
       </c>
       <c r="G163" s="2"/>
     </row>
-    <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="7"/>
     </row>
-    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="10" t="s">
         <v>198</v>
       </c>
@@ -4142,7 +4187,7 @@
       <c r="D165" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="E165" s="33" t="s">
+      <c r="E165" s="30" t="s">
         <v>221</v>
       </c>
       <c r="F165" s="1" t="s">
@@ -4152,19 +4197,19 @@
         <v>200</v>
       </c>
     </row>
-    <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="7"/>
     </row>
-    <row r="167" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A167" s="27" t="s">
+    <row r="167" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B167" s="28"/>
-      <c r="C167" s="28"/>
+      <c r="B167" s="36"/>
+      <c r="C167" s="36"/>
       <c r="D167" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="E167" s="33" t="s">
+      <c r="E167" s="30" t="s">
         <v>221</v>
       </c>
       <c r="F167" s="1" t="s">
@@ -4174,10 +4219,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="27"/>
-      <c r="B168" s="28"/>
-      <c r="C168" s="28"/>
+    <row r="168" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="35"/>
+      <c r="B168" s="36"/>
+      <c r="C168" s="36"/>
       <c r="D168" s="18" t="s">
         <v>183</v>
       </c>
@@ -4191,15 +4236,15 @@
         <v>202</v>
       </c>
     </row>
-    <row r="169" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="7"/>
     </row>
-    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A170" s="27" t="s">
+    <row r="170" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A170" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="B170" s="28"/>
-      <c r="C170" s="28"/>
+      <c r="B170" s="36"/>
+      <c r="C170" s="36"/>
       <c r="D170" s="18" t="s">
         <v>185</v>
       </c>
@@ -4213,10 +4258,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="27"/>
-      <c r="B171" s="28"/>
-      <c r="C171" s="28"/>
+    <row r="171" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="35"/>
+      <c r="B171" s="36"/>
+      <c r="C171" s="36"/>
       <c r="D171" s="18" t="s">
         <v>186</v>
       </c>
@@ -4230,10 +4275,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="27"/>
-      <c r="B172" s="28"/>
-      <c r="C172" s="28"/>
+    <row r="172" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="35"/>
+      <c r="B172" s="36"/>
+      <c r="C172" s="36"/>
       <c r="D172" s="18" t="s">
         <v>187</v>
       </c>
@@ -4245,10 +4290,10 @@
       </c>
       <c r="G172" s="3"/>
     </row>
-    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A173" s="27"/>
-      <c r="B173" s="28"/>
-      <c r="C173" s="28"/>
+    <row r="173" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A173" s="35"/>
+      <c r="B173" s="36"/>
+      <c r="C173" s="36"/>
       <c r="D173" s="18" t="s">
         <v>188</v>
       </c>
@@ -4260,15 +4305,15 @@
       </c>
       <c r="G173" s="3"/>
     </row>
-    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="7"/>
     </row>
-    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A175" s="27" t="s">
+    <row r="175" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A175" s="35" t="s">
         <v>189</v>
       </c>
-      <c r="B175" s="27"/>
-      <c r="C175" s="27"/>
+      <c r="B175" s="35"/>
+      <c r="C175" s="35"/>
       <c r="D175" s="18" t="s">
         <v>190</v>
       </c>
@@ -4280,10 +4325,10 @@
       </c>
       <c r="G175" s="2"/>
     </row>
-    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A176" s="27"/>
-      <c r="B176" s="27"/>
-      <c r="C176" s="27"/>
+    <row r="176" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="35"/>
+      <c r="B176" s="35"/>
+      <c r="C176" s="35"/>
       <c r="D176" s="18" t="s">
         <v>191</v>
       </c>
@@ -4295,10 +4340,10 @@
       </c>
       <c r="G176" s="4"/>
     </row>
-    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="27"/>
-      <c r="B177" s="27"/>
-      <c r="C177" s="27"/>
+    <row r="177" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A177" s="35"/>
+      <c r="B177" s="35"/>
+      <c r="C177" s="35"/>
       <c r="D177" s="18" t="s">
         <v>192</v>
       </c>
@@ -4310,10 +4355,10 @@
       </c>
       <c r="G177" s="3"/>
     </row>
-    <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="7"/>
     </row>
-    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="10" t="s">
         <v>193</v>
       </c>
@@ -4330,10 +4375,10 @@
       </c>
       <c r="G179" s="2"/>
     </row>
-    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="7"/>
     </row>
-    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="7"/>
       <c r="D181" s="18" t="s">
         <v>195</v>
@@ -4346,7 +4391,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="7"/>
       <c r="D182" s="18" t="s">
         <v>196</v>
@@ -4359,7 +4404,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="7"/>
       <c r="D183" s="18" t="s">
         <v>197</v>
@@ -4375,7 +4420,7 @@
   </sheetData>
   <autoFilter ref="E1:H183" xr:uid="{9EEAC858-8201-E147-9707-1E1D2225B431}">
     <filterColumn colId="0">
-      <filters>
+      <filters blank="1">
         <filter val="BB/TV"/>
         <filter val="Only TV"/>
       </filters>
@@ -4391,36 +4436,33 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <mergeCells count="71">
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="A44:A98"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="B67:B98"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="C61:C63"/>
-    <mergeCell ref="C64:C66"/>
-    <mergeCell ref="C67:C98"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="C5:C19"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="A5:A19"/>
-    <mergeCell ref="B5:B19"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B30:B33"/>
+  <mergeCells count="72">
+    <mergeCell ref="A175:A177"/>
+    <mergeCell ref="B175:B177"/>
+    <mergeCell ref="C175:C177"/>
+    <mergeCell ref="A167:A168"/>
+    <mergeCell ref="B167:B168"/>
+    <mergeCell ref="C167:C168"/>
+    <mergeCell ref="A170:A173"/>
+    <mergeCell ref="B170:B173"/>
+    <mergeCell ref="C170:C173"/>
+    <mergeCell ref="A157:A159"/>
+    <mergeCell ref="B157:B159"/>
+    <mergeCell ref="C157:C159"/>
+    <mergeCell ref="A161:A163"/>
+    <mergeCell ref="B161:B163"/>
+    <mergeCell ref="C161:C163"/>
+    <mergeCell ref="C150:C151"/>
+    <mergeCell ref="B150:B151"/>
+    <mergeCell ref="A150:A151"/>
+    <mergeCell ref="A153:A155"/>
+    <mergeCell ref="B153:B155"/>
+    <mergeCell ref="C153:C155"/>
+    <mergeCell ref="B120:B123"/>
+    <mergeCell ref="C120:C123"/>
+    <mergeCell ref="C124:C140"/>
+    <mergeCell ref="B124:B140"/>
+    <mergeCell ref="A120:A140"/>
     <mergeCell ref="C142:C146"/>
     <mergeCell ref="B142:B146"/>
     <mergeCell ref="A142:A146"/>
@@ -4437,34 +4479,39 @@
     <mergeCell ref="B61:B63"/>
     <mergeCell ref="B56:B60"/>
     <mergeCell ref="B44:B47"/>
-    <mergeCell ref="B120:B123"/>
-    <mergeCell ref="C120:C123"/>
-    <mergeCell ref="C124:C140"/>
-    <mergeCell ref="B124:B140"/>
-    <mergeCell ref="A120:A140"/>
-    <mergeCell ref="C150:C151"/>
-    <mergeCell ref="B150:B151"/>
-    <mergeCell ref="A150:A151"/>
-    <mergeCell ref="A153:A155"/>
-    <mergeCell ref="B153:B155"/>
-    <mergeCell ref="C153:C155"/>
-    <mergeCell ref="A157:A159"/>
-    <mergeCell ref="B157:B159"/>
-    <mergeCell ref="C157:C159"/>
-    <mergeCell ref="A161:A163"/>
-    <mergeCell ref="B161:B163"/>
-    <mergeCell ref="C161:C163"/>
-    <mergeCell ref="A175:A177"/>
-    <mergeCell ref="B175:B177"/>
-    <mergeCell ref="C175:C177"/>
-    <mergeCell ref="A167:A168"/>
-    <mergeCell ref="B167:B168"/>
-    <mergeCell ref="C167:C168"/>
-    <mergeCell ref="A170:A173"/>
-    <mergeCell ref="B170:B173"/>
-    <mergeCell ref="C170:C173"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="C5:C19"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A5:A19"/>
+    <mergeCell ref="B5:B19"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="L1:L1048576"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="A44:A98"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B67:B98"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="C61:C63"/>
+    <mergeCell ref="C64:C66"/>
+    <mergeCell ref="C67:C98"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B52:B53"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Collection and Environment update
</commit_message>
<xml_diff>
--- a/docs/Census_Wsc_Services.xlsx
+++ b/docs/Census_Wsc_Services.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian.catelli/Google Drive (christian.catelli@kineton.it)/Sky/Automation IT CI:CD WSC/Repository/PostmanCollection_AutomationAPI/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488686B8-735E-AC49-AA57-CB71BE74B752}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7F5E86-7DD0-2746-97A5-9CE1F5F0D7FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8656BBE8-7E17-AC42-8AF4-F6E9122F8590}"/>
   </bookViews>
@@ -964,16 +964,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1291,8 +1291,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1308,7 +1308,7 @@
     <col min="9" max="9" width="40" style="5" customWidth="1"/>
     <col min="10" max="10" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="35.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.83203125" style="33" customWidth="1"/>
+    <col min="12" max="12" width="7.83203125" style="36" customWidth="1"/>
     <col min="13" max="13" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="146" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
@@ -1349,7 +1349,7 @@
       <c r="K1" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="L1" s="36" t="s">
         <v>227</v>
       </c>
       <c r="M1" s="6" t="s">
@@ -1360,7 +1360,7 @@
       </c>
       <c r="O1" s="32"/>
     </row>
-    <row r="2" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="F2" s="10"/>
       <c r="G2" s="17"/>
@@ -1373,7 +1373,7 @@
       </c>
       <c r="O2" s="9"/>
     </row>
-    <row r="3" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -1394,18 +1394,18 @@
       </c>
       <c r="O3" s="22"/>
     </row>
-    <row r="4" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="O4" s="22"/>
     </row>
     <row r="5" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="16" t="s">
         <v>5</v>
       </c>
@@ -1421,9 +1421,9 @@
       <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
       <c r="D6" s="16" t="s">
         <v>6</v>
       </c>
@@ -1439,9 +1439,9 @@
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="16" t="s">
         <v>7</v>
       </c>
@@ -1457,9 +1457,9 @@
       <c r="O7" s="22"/>
     </row>
     <row r="8" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="16" t="s">
         <v>8</v>
       </c>
@@ -1475,9 +1475,9 @@
       <c r="O8" s="22"/>
     </row>
     <row r="9" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="16" t="s">
         <v>9</v>
       </c>
@@ -1492,9 +1492,9 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="34"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="16" t="s">
         <v>10</v>
       </c>
@@ -1509,9 +1509,9 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="34"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="16" t="s">
         <v>11</v>
       </c>
@@ -1526,9 +1526,9 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="34"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
       <c r="D12" s="16" t="s">
         <v>12</v>
       </c>
@@ -1543,9 +1543,9 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="34"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
       <c r="D13" s="16" t="s">
         <v>13</v>
       </c>
@@ -1560,9 +1560,9 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
       <c r="D14" s="16" t="s">
         <v>14</v>
       </c>
@@ -1577,9 +1577,9 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
+      <c r="A15" s="35"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
       <c r="D15" s="16" t="s">
         <v>15</v>
       </c>
@@ -1594,9 +1594,9 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="34"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="16" t="s">
         <v>16</v>
       </c>
@@ -1611,9 +1611,9 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="34"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="16" t="s">
         <v>17</v>
       </c>
@@ -1628,9 +1628,9 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
       <c r="D18" s="16" t="s">
         <v>18</v>
       </c>
@@ -1645,9 +1645,9 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
       <c r="D19" s="16" t="s">
         <v>19</v>
       </c>
@@ -1661,17 +1661,17 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
     </row>
-    <row r="21" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="34" t="s">
+    <row r="21" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="16" t="s">
         <v>21</v>
       </c>
@@ -1683,10 +1683,10 @@
       </c>
       <c r="G21" s="12"/>
     </row>
-    <row r="22" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="34"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
+    <row r="22" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="35"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
       <c r="D22" s="16" t="s">
         <v>24</v>
       </c>
@@ -1698,10 +1698,10 @@
       </c>
       <c r="G22" s="12"/>
     </row>
-    <row r="23" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="34"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
+    <row r="23" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="35"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
       <c r="D23" s="16" t="s">
         <v>25</v>
       </c>
@@ -1713,10 +1713,10 @@
       </c>
       <c r="G23" s="12"/>
     </row>
-    <row r="24" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="34"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
+    <row r="24" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="35"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
       <c r="D24" s="16" t="s">
         <v>26</v>
       </c>
@@ -1728,10 +1728,10 @@
       </c>
       <c r="G24" s="12"/>
     </row>
-    <row r="25" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="34"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
+    <row r="25" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="35"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
       <c r="D25" s="16" t="s">
         <v>27</v>
       </c>
@@ -1743,17 +1743,17 @@
       </c>
       <c r="G25" s="12"/>
     </row>
-    <row r="26" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
       <c r="D27" s="16" t="s">
         <v>30</v>
       </c>
@@ -1776,10 +1776,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="34"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
+    <row r="28" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="35"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
       <c r="D28" s="16" t="s">
         <v>31</v>
       </c>
@@ -1791,17 +1791,17 @@
       </c>
       <c r="G28" s="13"/>
     </row>
-    <row r="29" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
     </row>
     <row r="30" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
       <c r="D30" s="16" t="s">
         <v>34</v>
       </c>
@@ -1825,9 +1825,9 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="34"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
+      <c r="A31" s="35"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="35"/>
       <c r="D31" s="16" t="s">
         <v>35</v>
       </c>
@@ -1853,10 +1853,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="34"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
+    <row r="32" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="35"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
       <c r="D32" s="16" t="s">
         <v>36</v>
       </c>
@@ -1868,10 +1868,10 @@
       </c>
       <c r="G32" s="14"/>
     </row>
-    <row r="33" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="34"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
+    <row r="33" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="35"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="35"/>
       <c r="D33" s="16" t="s">
         <v>37</v>
       </c>
@@ -1883,17 +1883,17 @@
       </c>
       <c r="G33" s="14"/>
     </row>
-    <row r="34" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
     </row>
     <row r="35" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
       <c r="D35" s="16" t="s">
         <v>40</v>
       </c>
@@ -1906,9 +1906,9 @@
       <c r="G35" s="13"/>
     </row>
     <row r="36" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="34"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
+      <c r="A36" s="35"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
       <c r="D36" s="16" t="s">
         <v>41</v>
       </c>
@@ -1929,9 +1929,9 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="34"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
       <c r="D37" s="16" t="s">
         <v>42</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
@@ -1979,17 +1979,17 @@
         <v>214</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
     </row>
     <row r="41" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="34" t="s">
+      <c r="A41" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="34"/>
-      <c r="C41" s="34"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
       <c r="D41" s="16" t="s">
         <v>46</v>
       </c>
@@ -2002,9 +2002,9 @@
       <c r="G41" s="12"/>
     </row>
     <row r="42" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="34"/>
-      <c r="B42" s="34"/>
-      <c r="C42" s="34"/>
+      <c r="A42" s="35"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
       <c r="D42" s="16" t="s">
         <v>47</v>
       </c>
@@ -2016,19 +2016,19 @@
       </c>
       <c r="G42" s="12"/>
     </row>
-    <row r="43" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
     </row>
-    <row r="44" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="34" t="s">
+    <row r="44" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="34" t="s">
+      <c r="B44" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="34"/>
+      <c r="C44" s="35"/>
       <c r="D44" s="16" t="s">
         <v>51</v>
       </c>
@@ -2040,10 +2040,10 @@
       </c>
       <c r="G44" s="12"/>
     </row>
-    <row r="45" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="34"/>
-      <c r="B45" s="34"/>
-      <c r="C45" s="34"/>
+    <row r="45" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="35"/>
       <c r="D45" s="16" t="s">
         <v>52</v>
       </c>
@@ -2056,9 +2056,9 @@
       <c r="G45" s="12"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="34"/>
-      <c r="B46" s="34"/>
-      <c r="C46" s="34"/>
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="35"/>
       <c r="D46" s="16" t="s">
         <v>53</v>
       </c>
@@ -2082,9 +2082,9 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="34"/>
-      <c r="B47" s="34"/>
-      <c r="C47" s="34"/>
+      <c r="A47" s="35"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
       <c r="D47" s="16" t="s">
         <v>54</v>
       </c>
@@ -2110,12 +2110,12 @@
         <v>214</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="34"/>
-      <c r="B48" s="34" t="s">
+    <row r="48" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="35"/>
+      <c r="B48" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="C48" s="34"/>
+      <c r="C48" s="35"/>
       <c r="D48" s="16" t="s">
         <v>56</v>
       </c>
@@ -2124,10 +2124,10 @@
       </c>
       <c r="G48" s="12"/>
     </row>
-    <row r="49" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="34"/>
-      <c r="B49" s="34"/>
-      <c r="C49" s="34"/>
+    <row r="49" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="35"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="35"/>
       <c r="D49" s="16" t="s">
         <v>57</v>
       </c>
@@ -2136,12 +2136,12 @@
       </c>
       <c r="G49" s="12"/>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="34"/>
-      <c r="B50" s="34" t="s">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" s="35"/>
+      <c r="B50" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="C50" s="34"/>
+      <c r="C50" s="35"/>
       <c r="D50" s="16" t="s">
         <v>59</v>
       </c>
@@ -2155,10 +2155,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="34"/>
-      <c r="B51" s="34"/>
-      <c r="C51" s="34"/>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" s="35"/>
+      <c r="B51" s="35"/>
+      <c r="C51" s="35"/>
       <c r="D51" s="16" t="s">
         <v>60</v>
       </c>
@@ -2173,11 +2173,11 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" s="34"/>
-      <c r="B52" s="34" t="s">
+      <c r="A52" s="35"/>
+      <c r="B52" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C52" s="34"/>
+      <c r="C52" s="35"/>
       <c r="D52" s="16" t="s">
         <v>62</v>
       </c>
@@ -2201,9 +2201,9 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" s="34"/>
-      <c r="B53" s="34"/>
-      <c r="C53" s="34"/>
+      <c r="A53" s="35"/>
+      <c r="B53" s="35"/>
+      <c r="C53" s="35"/>
       <c r="D53" s="16" t="s">
         <v>63</v>
       </c>
@@ -2229,8 +2229,8 @@
         <v>212</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="34"/>
+    <row r="54" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="35"/>
       <c r="B54" s="7" t="s">
         <v>64</v>
       </c>
@@ -2244,8 +2244,8 @@
         <v>202</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="34"/>
+    <row r="55" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="35"/>
       <c r="B55" s="7" t="s">
         <v>66</v>
       </c>
@@ -2259,12 +2259,12 @@
         <v>200</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="34"/>
-      <c r="B56" s="34" t="s">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="35"/>
+      <c r="B56" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="C56" s="34" t="s">
+      <c r="C56" s="35" t="s">
         <v>68</v>
       </c>
       <c r="D56" s="16" t="s">
@@ -2280,10 +2280,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="34"/>
-      <c r="B57" s="34"/>
-      <c r="C57" s="34"/>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" s="35"/>
+      <c r="B57" s="35"/>
+      <c r="C57" s="35"/>
       <c r="D57" s="16" t="s">
         <v>70</v>
       </c>
@@ -2297,10 +2297,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="34"/>
-      <c r="B58" s="34"/>
-      <c r="C58" s="34"/>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" s="35"/>
+      <c r="B58" s="35"/>
+      <c r="C58" s="35"/>
       <c r="D58" s="16" t="s">
         <v>73</v>
       </c>
@@ -2314,10 +2314,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="34"/>
-      <c r="B59" s="34"/>
-      <c r="C59" s="34"/>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" s="35"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="35"/>
       <c r="D59" s="16" t="s">
         <v>74</v>
       </c>
@@ -2331,10 +2331,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="34"/>
-      <c r="B60" s="34"/>
-      <c r="C60" s="34"/>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="35"/>
+      <c r="B60" s="35"/>
+      <c r="C60" s="35"/>
       <c r="D60" s="16" t="s">
         <v>75</v>
       </c>
@@ -2349,11 +2349,11 @@
       </c>
     </row>
     <row r="61" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="34"/>
-      <c r="B61" s="34" t="s">
+      <c r="A61" s="35"/>
+      <c r="B61" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C61" s="34"/>
+      <c r="C61" s="35"/>
       <c r="D61" s="16" t="s">
         <v>77</v>
       </c>
@@ -2366,9 +2366,9 @@
       <c r="G61" s="12"/>
     </row>
     <row r="62" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="34"/>
-      <c r="B62" s="34"/>
-      <c r="C62" s="34"/>
+      <c r="A62" s="35"/>
+      <c r="B62" s="35"/>
+      <c r="C62" s="35"/>
       <c r="D62" s="16" t="s">
         <v>78</v>
       </c>
@@ -2381,9 +2381,9 @@
       <c r="G62" s="12"/>
     </row>
     <row r="63" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="34"/>
-      <c r="B63" s="34"/>
-      <c r="C63" s="34"/>
+      <c r="A63" s="35"/>
+      <c r="B63" s="35"/>
+      <c r="C63" s="35"/>
       <c r="D63" s="16" t="s">
         <v>79</v>
       </c>
@@ -2395,12 +2395,12 @@
       </c>
       <c r="G63" s="12"/>
     </row>
-    <row r="64" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="34"/>
-      <c r="B64" s="34" t="s">
+    <row r="64" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="35"/>
+      <c r="B64" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="C64" s="34"/>
+      <c r="C64" s="35"/>
       <c r="D64" s="16" t="s">
         <v>81</v>
       </c>
@@ -2412,10 +2412,10 @@
       </c>
       <c r="G64" s="12"/>
     </row>
-    <row r="65" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="34"/>
-      <c r="B65" s="34"/>
-      <c r="C65" s="34"/>
+    <row r="65" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="35"/>
+      <c r="B65" s="35"/>
+      <c r="C65" s="35"/>
       <c r="D65" s="16" t="s">
         <v>82</v>
       </c>
@@ -2427,10 +2427,10 @@
       </c>
       <c r="G65" s="12"/>
     </row>
-    <row r="66" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="34"/>
-      <c r="B66" s="34"/>
-      <c r="C66" s="34"/>
+    <row r="66" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="35"/>
+      <c r="B66" s="35"/>
+      <c r="C66" s="35"/>
       <c r="D66" s="16" t="s">
         <v>83</v>
       </c>
@@ -2443,9 +2443,9 @@
       <c r="G66" s="12"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A67" s="34"/>
-      <c r="B67" s="34"/>
-      <c r="C67" s="34"/>
+      <c r="A67" s="35"/>
+      <c r="B67" s="35"/>
+      <c r="C67" s="35"/>
       <c r="D67" s="16" t="s">
         <v>84</v>
       </c>
@@ -2469,9 +2469,9 @@
       </c>
     </row>
     <row r="68" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="34"/>
-      <c r="B68" s="34"/>
-      <c r="C68" s="34"/>
+      <c r="A68" s="35"/>
+      <c r="B68" s="35"/>
+      <c r="C68" s="35"/>
       <c r="D68" s="16" t="s">
         <v>85</v>
       </c>
@@ -2492,9 +2492,9 @@
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69" s="34"/>
-      <c r="B69" s="34"/>
-      <c r="C69" s="34"/>
+      <c r="A69" s="35"/>
+      <c r="B69" s="35"/>
+      <c r="C69" s="35"/>
       <c r="D69" s="16" t="s">
         <v>86</v>
       </c>
@@ -2518,9 +2518,9 @@
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A70" s="34"/>
-      <c r="B70" s="34"/>
-      <c r="C70" s="34"/>
+      <c r="A70" s="35"/>
+      <c r="B70" s="35"/>
+      <c r="C70" s="35"/>
       <c r="D70" s="16" t="s">
         <v>87</v>
       </c>
@@ -2544,9 +2544,9 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A71" s="34"/>
-      <c r="B71" s="34"/>
-      <c r="C71" s="34"/>
+      <c r="A71" s="35"/>
+      <c r="B71" s="35"/>
+      <c r="C71" s="35"/>
       <c r="D71" s="16" t="s">
         <v>88</v>
       </c>
@@ -2570,9 +2570,9 @@
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A72" s="34"/>
-      <c r="B72" s="34"/>
-      <c r="C72" s="34"/>
+      <c r="A72" s="35"/>
+      <c r="B72" s="35"/>
+      <c r="C72" s="35"/>
       <c r="D72" s="16" t="s">
         <v>89</v>
       </c>
@@ -2596,9 +2596,9 @@
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A73" s="34"/>
-      <c r="B73" s="34"/>
-      <c r="C73" s="34"/>
+      <c r="A73" s="35"/>
+      <c r="B73" s="35"/>
+      <c r="C73" s="35"/>
       <c r="D73" s="16" t="s">
         <v>90</v>
       </c>
@@ -2625,9 +2625,9 @@
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A74" s="34"/>
-      <c r="B74" s="34"/>
-      <c r="C74" s="34"/>
+      <c r="A74" s="35"/>
+      <c r="B74" s="35"/>
+      <c r="C74" s="35"/>
       <c r="D74" s="16" t="s">
         <v>91</v>
       </c>
@@ -2654,9 +2654,9 @@
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A75" s="34"/>
-      <c r="B75" s="34"/>
-      <c r="C75" s="34"/>
+      <c r="A75" s="35"/>
+      <c r="B75" s="35"/>
+      <c r="C75" s="35"/>
       <c r="D75" s="16" t="s">
         <v>92</v>
       </c>
@@ -2680,9 +2680,9 @@
       </c>
     </row>
     <row r="76" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="34"/>
-      <c r="B76" s="34"/>
-      <c r="C76" s="34"/>
+      <c r="A76" s="35"/>
+      <c r="B76" s="35"/>
+      <c r="C76" s="35"/>
       <c r="D76" s="16" t="s">
         <v>93</v>
       </c>
@@ -2706,9 +2706,9 @@
       </c>
     </row>
     <row r="77" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="34"/>
-      <c r="B77" s="34"/>
-      <c r="C77" s="34"/>
+      <c r="A77" s="35"/>
+      <c r="B77" s="35"/>
+      <c r="C77" s="35"/>
       <c r="D77" s="16" t="s">
         <v>94</v>
       </c>
@@ -2729,9 +2729,9 @@
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A78" s="34"/>
-      <c r="B78" s="34"/>
-      <c r="C78" s="34"/>
+      <c r="A78" s="35"/>
+      <c r="B78" s="35"/>
+      <c r="C78" s="35"/>
       <c r="D78" s="16" t="s">
         <v>95</v>
       </c>
@@ -2755,9 +2755,9 @@
       </c>
     </row>
     <row r="79" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="34"/>
-      <c r="B79" s="34"/>
-      <c r="C79" s="34"/>
+      <c r="A79" s="35"/>
+      <c r="B79" s="35"/>
+      <c r="C79" s="35"/>
       <c r="D79" s="24" t="s">
         <v>96</v>
       </c>
@@ -2781,9 +2781,9 @@
       </c>
     </row>
     <row r="80" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="34"/>
-      <c r="B80" s="34"/>
-      <c r="C80" s="34"/>
+      <c r="A80" s="35"/>
+      <c r="B80" s="35"/>
+      <c r="C80" s="35"/>
       <c r="D80" s="24" t="s">
         <v>97</v>
       </c>
@@ -2804,9 +2804,9 @@
       </c>
     </row>
     <row r="81" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="34"/>
-      <c r="B81" s="34"/>
-      <c r="C81" s="34"/>
+      <c r="A81" s="35"/>
+      <c r="B81" s="35"/>
+      <c r="C81" s="35"/>
       <c r="D81" s="16" t="s">
         <v>98</v>
       </c>
@@ -2819,9 +2819,9 @@
       <c r="G81" s="13"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A82" s="34"/>
-      <c r="B82" s="34"/>
-      <c r="C82" s="34"/>
+      <c r="A82" s="35"/>
+      <c r="B82" s="35"/>
+      <c r="C82" s="35"/>
       <c r="D82" s="24" t="s">
         <v>99</v>
       </c>
@@ -2848,9 +2848,9 @@
       </c>
     </row>
     <row r="83" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="34"/>
-      <c r="B83" s="34"/>
-      <c r="C83" s="34"/>
+      <c r="A83" s="35"/>
+      <c r="B83" s="35"/>
+      <c r="C83" s="35"/>
       <c r="D83" s="24" t="s">
         <v>100</v>
       </c>
@@ -2877,9 +2877,9 @@
       </c>
     </row>
     <row r="84" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="34"/>
-      <c r="B84" s="34"/>
-      <c r="C84" s="34"/>
+      <c r="A84" s="35"/>
+      <c r="B84" s="35"/>
+      <c r="C84" s="35"/>
       <c r="D84" s="24" t="s">
         <v>101</v>
       </c>
@@ -2906,9 +2906,9 @@
       </c>
     </row>
     <row r="85" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="34"/>
-      <c r="B85" s="34"/>
-      <c r="C85" s="34"/>
+      <c r="A85" s="35"/>
+      <c r="B85" s="35"/>
+      <c r="C85" s="35"/>
       <c r="D85" s="24" t="s">
         <v>102</v>
       </c>
@@ -2935,9 +2935,9 @@
       </c>
     </row>
     <row r="86" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="34"/>
-      <c r="B86" s="34"/>
-      <c r="C86" s="34"/>
+      <c r="A86" s="35"/>
+      <c r="B86" s="35"/>
+      <c r="C86" s="35"/>
       <c r="D86" s="24" t="s">
         <v>103</v>
       </c>
@@ -2963,10 +2963,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="34"/>
-      <c r="B87" s="34"/>
-      <c r="C87" s="34"/>
+    <row r="87" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="35"/>
+      <c r="B87" s="35"/>
+      <c r="C87" s="35"/>
       <c r="D87" s="16" t="s">
         <v>104</v>
       </c>
@@ -2978,10 +2978,10 @@
       </c>
       <c r="G87" s="13"/>
     </row>
-    <row r="88" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="34"/>
-      <c r="B88" s="34"/>
-      <c r="C88" s="34"/>
+    <row r="88" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="35"/>
+      <c r="B88" s="35"/>
+      <c r="C88" s="35"/>
       <c r="D88" s="16" t="s">
         <v>105</v>
       </c>
@@ -2993,10 +2993,10 @@
       </c>
       <c r="G88" s="13"/>
     </row>
-    <row r="89" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="34"/>
-      <c r="B89" s="34"/>
-      <c r="C89" s="34"/>
+    <row r="89" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="35"/>
+      <c r="B89" s="35"/>
+      <c r="C89" s="35"/>
       <c r="D89" s="16" t="s">
         <v>106</v>
       </c>
@@ -3008,10 +3008,10 @@
       </c>
       <c r="G89" s="13"/>
     </row>
-    <row r="90" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="34"/>
-      <c r="B90" s="34"/>
-      <c r="C90" s="34"/>
+    <row r="90" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="35"/>
+      <c r="B90" s="35"/>
+      <c r="C90" s="35"/>
       <c r="D90" s="16" t="s">
         <v>107</v>
       </c>
@@ -3023,10 +3023,10 @@
       </c>
       <c r="G90" s="13"/>
     </row>
-    <row r="91" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="34"/>
-      <c r="B91" s="34"/>
-      <c r="C91" s="34"/>
+    <row r="91" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="35"/>
+      <c r="B91" s="35"/>
+      <c r="C91" s="35"/>
       <c r="D91" s="16" t="s">
         <v>108</v>
       </c>
@@ -3038,10 +3038,10 @@
       </c>
       <c r="G91" s="13"/>
     </row>
-    <row r="92" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="34"/>
-      <c r="B92" s="34"/>
-      <c r="C92" s="34"/>
+    <row r="92" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="35"/>
+      <c r="B92" s="35"/>
+      <c r="C92" s="35"/>
       <c r="D92" s="16" t="s">
         <v>109</v>
       </c>
@@ -3053,10 +3053,10 @@
       </c>
       <c r="G92" s="13"/>
     </row>
-    <row r="93" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="34"/>
-      <c r="B93" s="34"/>
-      <c r="C93" s="34"/>
+    <row r="93" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="35"/>
+      <c r="B93" s="35"/>
+      <c r="C93" s="35"/>
       <c r="D93" s="16" t="s">
         <v>110</v>
       </c>
@@ -3069,9 +3069,9 @@
       <c r="G93" s="13"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A94" s="34"/>
-      <c r="B94" s="34"/>
-      <c r="C94" s="34"/>
+      <c r="A94" s="35"/>
+      <c r="B94" s="35"/>
+      <c r="C94" s="35"/>
       <c r="D94" s="24" t="s">
         <v>111</v>
       </c>
@@ -3095,9 +3095,9 @@
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A95" s="34"/>
-      <c r="B95" s="34"/>
-      <c r="C95" s="34"/>
+      <c r="A95" s="35"/>
+      <c r="B95" s="35"/>
+      <c r="C95" s="35"/>
       <c r="D95" s="24" t="s">
         <v>112</v>
       </c>
@@ -3120,10 +3120,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="34"/>
-      <c r="B96" s="34"/>
-      <c r="C96" s="34"/>
+    <row r="96" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="35"/>
+      <c r="B96" s="35"/>
+      <c r="C96" s="35"/>
       <c r="D96" s="16" t="s">
         <v>113</v>
       </c>
@@ -3135,10 +3135,10 @@
       </c>
       <c r="G96" s="12"/>
     </row>
-    <row r="97" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="34"/>
-      <c r="B97" s="34"/>
-      <c r="C97" s="34"/>
+    <row r="97" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="35"/>
+      <c r="B97" s="35"/>
+      <c r="C97" s="35"/>
       <c r="D97" s="16" t="s">
         <v>114</v>
       </c>
@@ -3151,9 +3151,9 @@
       <c r="G97" s="12"/>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A98" s="34"/>
-      <c r="B98" s="34"/>
-      <c r="C98" s="34"/>
+      <c r="A98" s="35"/>
+      <c r="B98" s="35"/>
+      <c r="C98" s="35"/>
       <c r="D98" s="24" t="s">
         <v>115</v>
       </c>
@@ -3176,17 +3176,17 @@
         <v>214</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="7"/>
       <c r="F99" s="11"/>
       <c r="G99" s="11"/>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="35" t="s">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A100" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="B100" s="35"/>
-      <c r="C100" s="35"/>
+      <c r="B100" s="33"/>
+      <c r="C100" s="33"/>
       <c r="D100" s="16" t="s">
         <v>117</v>
       </c>
@@ -3200,10 +3200,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="35"/>
-      <c r="B101" s="35"/>
-      <c r="C101" s="35"/>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A101" s="33"/>
+      <c r="B101" s="33"/>
+      <c r="C101" s="33"/>
       <c r="D101" s="16" t="s">
         <v>118</v>
       </c>
@@ -3217,10 +3217,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="35"/>
-      <c r="B102" s="35"/>
-      <c r="C102" s="35"/>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A102" s="33"/>
+      <c r="B102" s="33"/>
+      <c r="C102" s="33"/>
       <c r="D102" s="16" t="s">
         <v>119</v>
       </c>
@@ -3234,10 +3234,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="35"/>
-      <c r="B103" s="35"/>
-      <c r="C103" s="35"/>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A103" s="33"/>
+      <c r="B103" s="33"/>
+      <c r="C103" s="33"/>
       <c r="D103" s="16" t="s">
         <v>120</v>
       </c>
@@ -3251,10 +3251,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="34"/>
-      <c r="B104" s="35"/>
-      <c r="C104" s="35"/>
+    <row r="104" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="35"/>
+      <c r="B104" s="33"/>
+      <c r="C104" s="33"/>
       <c r="D104" s="16" t="s">
         <v>121</v>
       </c>
@@ -3266,10 +3266,10 @@
       </c>
       <c r="G104" s="12"/>
     </row>
-    <row r="105" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="34"/>
-      <c r="B105" s="35"/>
-      <c r="C105" s="35"/>
+    <row r="105" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="35"/>
+      <c r="B105" s="33"/>
+      <c r="C105" s="33"/>
       <c r="D105" s="16" t="s">
         <v>122</v>
       </c>
@@ -3281,10 +3281,10 @@
       </c>
       <c r="G105" s="12"/>
     </row>
-    <row r="106" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="34"/>
-      <c r="B106" s="35"/>
-      <c r="C106" s="35"/>
+    <row r="106" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="35"/>
+      <c r="B106" s="33"/>
+      <c r="C106" s="33"/>
       <c r="D106" s="16" t="s">
         <v>123</v>
       </c>
@@ -3296,10 +3296,10 @@
       </c>
       <c r="G106" s="12"/>
     </row>
-    <row r="107" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="34"/>
-      <c r="B107" s="35"/>
-      <c r="C107" s="35"/>
+    <row r="107" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="35"/>
+      <c r="B107" s="33"/>
+      <c r="C107" s="33"/>
       <c r="D107" s="16" t="s">
         <v>124</v>
       </c>
@@ -3311,10 +3311,10 @@
       </c>
       <c r="G107" s="12"/>
     </row>
-    <row r="108" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="34"/>
-      <c r="B108" s="35"/>
-      <c r="C108" s="35"/>
+    <row r="108" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="35"/>
+      <c r="B108" s="33"/>
+      <c r="C108" s="33"/>
       <c r="D108" s="16" t="s">
         <v>125</v>
       </c>
@@ -3326,10 +3326,10 @@
       </c>
       <c r="G108" s="12"/>
     </row>
-    <row r="109" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="34"/>
-      <c r="B109" s="35"/>
-      <c r="C109" s="35"/>
+    <row r="109" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="35"/>
+      <c r="B109" s="33"/>
+      <c r="C109" s="33"/>
       <c r="D109" s="16" t="s">
         <v>126</v>
       </c>
@@ -3341,10 +3341,10 @@
       </c>
       <c r="G109" s="12"/>
     </row>
-    <row r="110" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="34"/>
-      <c r="B110" s="35"/>
-      <c r="C110" s="35"/>
+    <row r="110" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="35"/>
+      <c r="B110" s="33"/>
+      <c r="C110" s="33"/>
       <c r="D110" s="16" t="s">
         <v>127</v>
       </c>
@@ -3356,10 +3356,10 @@
       </c>
       <c r="G110" s="12"/>
     </row>
-    <row r="111" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="34"/>
-      <c r="B111" s="35"/>
-      <c r="C111" s="35"/>
+    <row r="111" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="35"/>
+      <c r="B111" s="33"/>
+      <c r="C111" s="33"/>
       <c r="D111" s="16" t="s">
         <v>128</v>
       </c>
@@ -3371,10 +3371,10 @@
       </c>
       <c r="G111" s="12"/>
     </row>
-    <row r="112" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="34"/>
-      <c r="B112" s="35"/>
-      <c r="C112" s="35"/>
+    <row r="112" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="35"/>
+      <c r="B112" s="33"/>
+      <c r="C112" s="33"/>
       <c r="D112" s="16" t="s">
         <v>129</v>
       </c>
@@ -3386,10 +3386,10 @@
       </c>
       <c r="G112" s="13"/>
     </row>
-    <row r="113" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="34"/>
-      <c r="B113" s="35"/>
-      <c r="C113" s="35"/>
+    <row r="113" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="35"/>
+      <c r="B113" s="33"/>
+      <c r="C113" s="33"/>
       <c r="D113" s="16" t="s">
         <v>130</v>
       </c>
@@ -3401,10 +3401,10 @@
       </c>
       <c r="G113" s="13"/>
     </row>
-    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="35"/>
-      <c r="B114" s="35"/>
-      <c r="C114" s="35"/>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A114" s="33"/>
+      <c r="B114" s="33"/>
+      <c r="C114" s="33"/>
       <c r="D114" s="16" t="s">
         <v>131</v>
       </c>
@@ -3418,10 +3418,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="35"/>
-      <c r="B115" s="35"/>
-      <c r="C115" s="35"/>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A115" s="33"/>
+      <c r="B115" s="33"/>
+      <c r="C115" s="33"/>
       <c r="D115" s="16" t="s">
         <v>132</v>
       </c>
@@ -3435,15 +3435,15 @@
         <v>202</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="7"/>
     </row>
     <row r="117" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="35" t="s">
+      <c r="A117" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="B117" s="35"/>
-      <c r="C117" s="35"/>
+      <c r="B117" s="33"/>
+      <c r="C117" s="33"/>
       <c r="D117" s="16" t="s">
         <v>134</v>
       </c>
@@ -3456,9 +3456,9 @@
       <c r="G117" s="12"/>
     </row>
     <row r="118" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="35"/>
-      <c r="B118" s="35"/>
-      <c r="C118" s="35"/>
+      <c r="A118" s="33"/>
+      <c r="B118" s="33"/>
+      <c r="C118" s="33"/>
       <c r="D118" s="16" t="s">
         <v>135</v>
       </c>
@@ -3470,17 +3470,17 @@
       </c>
       <c r="G118" s="12"/>
     </row>
-    <row r="119" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="7"/>
     </row>
     <row r="120" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="34" t="s">
+      <c r="A120" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="B120" s="35" t="s">
+      <c r="B120" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="C120" s="35"/>
+      <c r="C120" s="33"/>
       <c r="D120" s="16" t="s">
         <v>138</v>
       </c>
@@ -3495,9 +3495,9 @@
       </c>
     </row>
     <row r="121" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="34"/>
-      <c r="B121" s="35"/>
-      <c r="C121" s="35"/>
+      <c r="A121" s="35"/>
+      <c r="B121" s="33"/>
+      <c r="C121" s="33"/>
       <c r="D121" s="16" t="s">
         <v>139</v>
       </c>
@@ -3512,9 +3512,9 @@
       </c>
     </row>
     <row r="122" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="34"/>
-      <c r="B122" s="35"/>
-      <c r="C122" s="35"/>
+      <c r="A122" s="35"/>
+      <c r="B122" s="33"/>
+      <c r="C122" s="33"/>
       <c r="D122" s="16" t="s">
         <v>140</v>
       </c>
@@ -3529,9 +3529,9 @@
       </c>
     </row>
     <row r="123" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="34"/>
-      <c r="B123" s="35"/>
-      <c r="C123" s="35"/>
+      <c r="A123" s="35"/>
+      <c r="B123" s="33"/>
+      <c r="C123" s="33"/>
       <c r="D123" s="16" t="s">
         <v>141</v>
       </c>
@@ -3546,9 +3546,9 @@
       </c>
     </row>
     <row r="124" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="34"/>
-      <c r="B124" s="35"/>
-      <c r="C124" s="35"/>
+      <c r="A124" s="35"/>
+      <c r="B124" s="33"/>
+      <c r="C124" s="33"/>
       <c r="D124" s="24" t="s">
         <v>142</v>
       </c>
@@ -3572,9 +3572,9 @@
       </c>
     </row>
     <row r="125" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="34"/>
-      <c r="B125" s="35"/>
-      <c r="C125" s="35"/>
+      <c r="A125" s="35"/>
+      <c r="B125" s="33"/>
+      <c r="C125" s="33"/>
       <c r="D125" s="24" t="s">
         <v>143</v>
       </c>
@@ -3592,9 +3592,9 @@
       </c>
     </row>
     <row r="126" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="34"/>
-      <c r="B126" s="35"/>
-      <c r="C126" s="35"/>
+      <c r="A126" s="35"/>
+      <c r="B126" s="33"/>
+      <c r="C126" s="33"/>
       <c r="D126" s="24" t="s">
         <v>144</v>
       </c>
@@ -3612,9 +3612,9 @@
       </c>
     </row>
     <row r="127" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="34"/>
-      <c r="B127" s="35"/>
-      <c r="C127" s="35"/>
+      <c r="A127" s="35"/>
+      <c r="B127" s="33"/>
+      <c r="C127" s="33"/>
       <c r="D127" s="24" t="s">
         <v>145</v>
       </c>
@@ -3632,9 +3632,9 @@
       </c>
     </row>
     <row r="128" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="34"/>
-      <c r="B128" s="35"/>
-      <c r="C128" s="35"/>
+      <c r="A128" s="35"/>
+      <c r="B128" s="33"/>
+      <c r="C128" s="33"/>
       <c r="D128" s="24" t="s">
         <v>146</v>
       </c>
@@ -3652,9 +3652,9 @@
       </c>
     </row>
     <row r="129" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="34"/>
-      <c r="B129" s="35"/>
-      <c r="C129" s="35"/>
+      <c r="A129" s="35"/>
+      <c r="B129" s="33"/>
+      <c r="C129" s="33"/>
       <c r="D129" s="24" t="s">
         <v>147</v>
       </c>
@@ -3672,9 +3672,9 @@
       </c>
     </row>
     <row r="130" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="34"/>
-      <c r="B130" s="35"/>
-      <c r="C130" s="35"/>
+      <c r="A130" s="35"/>
+      <c r="B130" s="33"/>
+      <c r="C130" s="33"/>
       <c r="D130" s="24" t="s">
         <v>148</v>
       </c>
@@ -3692,9 +3692,9 @@
       </c>
     </row>
     <row r="131" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="34"/>
-      <c r="B131" s="35"/>
-      <c r="C131" s="35"/>
+      <c r="A131" s="35"/>
+      <c r="B131" s="33"/>
+      <c r="C131" s="33"/>
       <c r="D131" s="24" t="s">
         <v>149</v>
       </c>
@@ -3712,9 +3712,9 @@
       </c>
     </row>
     <row r="132" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="34"/>
-      <c r="B132" s="35"/>
-      <c r="C132" s="35"/>
+      <c r="A132" s="35"/>
+      <c r="B132" s="33"/>
+      <c r="C132" s="33"/>
       <c r="D132" s="24" t="s">
         <v>150</v>
       </c>
@@ -3732,9 +3732,9 @@
       </c>
     </row>
     <row r="133" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="34"/>
-      <c r="B133" s="35"/>
-      <c r="C133" s="35"/>
+      <c r="A133" s="35"/>
+      <c r="B133" s="33"/>
+      <c r="C133" s="33"/>
       <c r="D133" s="24" t="s">
         <v>151</v>
       </c>
@@ -3752,9 +3752,9 @@
       </c>
     </row>
     <row r="134" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="34"/>
-      <c r="B134" s="35"/>
-      <c r="C134" s="35"/>
+      <c r="A134" s="35"/>
+      <c r="B134" s="33"/>
+      <c r="C134" s="33"/>
       <c r="D134" s="24" t="s">
         <v>152</v>
       </c>
@@ -3772,9 +3772,9 @@
       </c>
     </row>
     <row r="135" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="34"/>
-      <c r="B135" s="35"/>
-      <c r="C135" s="35"/>
+      <c r="A135" s="35"/>
+      <c r="B135" s="33"/>
+      <c r="C135" s="33"/>
       <c r="D135" s="24" t="s">
         <v>153</v>
       </c>
@@ -3792,9 +3792,9 @@
       </c>
     </row>
     <row r="136" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="34"/>
-      <c r="B136" s="35"/>
-      <c r="C136" s="35"/>
+      <c r="A136" s="35"/>
+      <c r="B136" s="33"/>
+      <c r="C136" s="33"/>
       <c r="D136" s="24" t="s">
         <v>154</v>
       </c>
@@ -3812,9 +3812,9 @@
       </c>
     </row>
     <row r="137" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="34"/>
-      <c r="B137" s="35"/>
-      <c r="C137" s="35"/>
+      <c r="A137" s="35"/>
+      <c r="B137" s="33"/>
+      <c r="C137" s="33"/>
       <c r="D137" s="24" t="s">
         <v>155</v>
       </c>
@@ -3832,9 +3832,9 @@
       </c>
     </row>
     <row r="138" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="34"/>
-      <c r="B138" s="35"/>
-      <c r="C138" s="35"/>
+      <c r="A138" s="35"/>
+      <c r="B138" s="33"/>
+      <c r="C138" s="33"/>
       <c r="D138" s="24" t="s">
         <v>156</v>
       </c>
@@ -3852,9 +3852,9 @@
       </c>
     </row>
     <row r="139" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="34"/>
-      <c r="B139" s="35"/>
-      <c r="C139" s="35"/>
+      <c r="A139" s="35"/>
+      <c r="B139" s="33"/>
+      <c r="C139" s="33"/>
       <c r="D139" s="16" t="s">
         <v>157</v>
       </c>
@@ -3867,9 +3867,9 @@
       <c r="G139" s="15"/>
     </row>
     <row r="140" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A140" s="34"/>
-      <c r="B140" s="35"/>
-      <c r="C140" s="35"/>
+      <c r="A140" s="35"/>
+      <c r="B140" s="33"/>
+      <c r="C140" s="33"/>
       <c r="D140" s="16" t="s">
         <v>158</v>
       </c>
@@ -3881,17 +3881,17 @@
       </c>
       <c r="G140" s="15"/>
     </row>
-    <row r="141" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="10"/>
       <c r="B141" s="10"/>
       <c r="C141" s="10"/>
     </row>
-    <row r="142" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="35" t="s">
+    <row r="142" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="B142" s="35"/>
-      <c r="C142" s="35"/>
+      <c r="B142" s="33"/>
+      <c r="C142" s="33"/>
       <c r="D142" s="16" t="s">
         <v>160</v>
       </c>
@@ -3903,10 +3903,10 @@
       </c>
       <c r="G142" s="12"/>
     </row>
-    <row r="143" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="35"/>
-      <c r="B143" s="35"/>
-      <c r="C143" s="35"/>
+    <row r="143" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="33"/>
+      <c r="B143" s="33"/>
+      <c r="C143" s="33"/>
       <c r="D143" s="16" t="s">
         <v>160</v>
       </c>
@@ -3918,10 +3918,10 @@
       </c>
       <c r="G143" s="12"/>
     </row>
-    <row r="144" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="35"/>
-      <c r="B144" s="35"/>
-      <c r="C144" s="35"/>
+    <row r="144" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="33"/>
+      <c r="B144" s="33"/>
+      <c r="C144" s="33"/>
       <c r="D144" s="16" t="s">
         <v>161</v>
       </c>
@@ -3933,10 +3933,10 @@
       </c>
       <c r="G144" s="12"/>
     </row>
-    <row r="145" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="35"/>
-      <c r="B145" s="35"/>
-      <c r="C145" s="35"/>
+    <row r="145" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="33"/>
+      <c r="B145" s="33"/>
+      <c r="C145" s="33"/>
       <c r="D145" s="16" t="s">
         <v>162</v>
       </c>
@@ -3948,10 +3948,10 @@
       </c>
       <c r="G145" s="13"/>
     </row>
-    <row r="146" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="35"/>
-      <c r="B146" s="35"/>
-      <c r="C146" s="35"/>
+    <row r="146" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="33"/>
+      <c r="B146" s="33"/>
+      <c r="C146" s="33"/>
       <c r="D146" s="16" t="s">
         <v>163</v>
       </c>
@@ -3963,10 +3963,10 @@
       </c>
       <c r="G146" s="13"/>
     </row>
-    <row r="147" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="7"/>
     </row>
-    <row r="148" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="10" t="s">
         <v>165</v>
       </c>
@@ -3980,15 +3980,15 @@
         <v>202</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="7"/>
     </row>
     <row r="150" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="35" t="s">
+      <c r="A150" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="B150" s="35"/>
-      <c r="C150" s="35"/>
+      <c r="B150" s="33"/>
+      <c r="C150" s="33"/>
       <c r="D150" s="16" t="s">
         <v>168</v>
       </c>
@@ -4003,9 +4003,9 @@
       </c>
     </row>
     <row r="151" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="35"/>
-      <c r="B151" s="35"/>
-      <c r="C151" s="35"/>
+      <c r="A151" s="33"/>
+      <c r="B151" s="33"/>
+      <c r="C151" s="33"/>
       <c r="D151" s="16" t="s">
         <v>169</v>
       </c>
@@ -4019,15 +4019,15 @@
         <v>200</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="7"/>
     </row>
     <row r="153" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="35" t="s">
+      <c r="A153" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="B153" s="36"/>
-      <c r="C153" s="36"/>
+      <c r="B153" s="34"/>
+      <c r="C153" s="34"/>
       <c r="D153" s="18" t="s">
         <v>171</v>
       </c>
@@ -4040,9 +4040,9 @@
       <c r="G153" s="2"/>
     </row>
     <row r="154" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="35"/>
-      <c r="B154" s="36"/>
-      <c r="C154" s="36"/>
+      <c r="A154" s="33"/>
+      <c r="B154" s="34"/>
+      <c r="C154" s="34"/>
       <c r="D154" s="18" t="s">
         <v>172</v>
       </c>
@@ -4055,9 +4055,9 @@
       <c r="G154" s="2"/>
     </row>
     <row r="155" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="35"/>
-      <c r="B155" s="36"/>
-      <c r="C155" s="36"/>
+      <c r="A155" s="33"/>
+      <c r="B155" s="34"/>
+      <c r="C155" s="34"/>
       <c r="D155" s="18" t="s">
         <v>173</v>
       </c>
@@ -4069,15 +4069,15 @@
       </c>
       <c r="G155" s="2"/>
     </row>
-    <row r="156" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="7"/>
     </row>
     <row r="157" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="35" t="s">
+      <c r="A157" s="33" t="s">
         <v>224</v>
       </c>
-      <c r="B157" s="36"/>
-      <c r="C157" s="36"/>
+      <c r="B157" s="34"/>
+      <c r="C157" s="34"/>
       <c r="D157" s="18" t="s">
         <v>174</v>
       </c>
@@ -4092,9 +4092,9 @@
       </c>
     </row>
     <row r="158" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A158" s="35"/>
-      <c r="B158" s="36"/>
-      <c r="C158" s="36"/>
+      <c r="A158" s="33"/>
+      <c r="B158" s="34"/>
+      <c r="C158" s="34"/>
       <c r="D158" s="18" t="s">
         <v>175</v>
       </c>
@@ -4109,9 +4109,9 @@
       </c>
     </row>
     <row r="159" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A159" s="35"/>
-      <c r="B159" s="36"/>
-      <c r="C159" s="36"/>
+      <c r="A159" s="33"/>
+      <c r="B159" s="34"/>
+      <c r="C159" s="34"/>
       <c r="D159" s="18" t="s">
         <v>176</v>
       </c>
@@ -4125,15 +4125,15 @@
         <v>200</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="7"/>
     </row>
-    <row r="161" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="35" t="s">
+    <row r="161" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="B161" s="36"/>
-      <c r="C161" s="36"/>
+      <c r="B161" s="34"/>
+      <c r="C161" s="34"/>
       <c r="D161" s="18" t="s">
         <v>178</v>
       </c>
@@ -4145,10 +4145,10 @@
       </c>
       <c r="G161" s="2"/>
     </row>
-    <row r="162" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A162" s="35"/>
-      <c r="B162" s="36"/>
-      <c r="C162" s="36"/>
+    <row r="162" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="33"/>
+      <c r="B162" s="34"/>
+      <c r="C162" s="34"/>
       <c r="D162" s="18" t="s">
         <v>179</v>
       </c>
@@ -4161,9 +4161,9 @@
       <c r="G162" s="2"/>
     </row>
     <row r="163" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="35"/>
-      <c r="B163" s="36"/>
-      <c r="C163" s="36"/>
+      <c r="A163" s="33"/>
+      <c r="B163" s="34"/>
+      <c r="C163" s="34"/>
       <c r="D163" s="18" t="s">
         <v>180</v>
       </c>
@@ -4175,7 +4175,7 @@
       </c>
       <c r="G163" s="2"/>
     </row>
-    <row r="164" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="7"/>
     </row>
     <row r="165" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4197,15 +4197,15 @@
         <v>200</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="7"/>
     </row>
     <row r="167" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A167" s="35" t="s">
+      <c r="A167" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="B167" s="36"/>
-      <c r="C167" s="36"/>
+      <c r="B167" s="34"/>
+      <c r="C167" s="34"/>
       <c r="D167" s="18" t="s">
         <v>182</v>
       </c>
@@ -4220,9 +4220,9 @@
       </c>
     </row>
     <row r="168" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="35"/>
-      <c r="B168" s="36"/>
-      <c r="C168" s="36"/>
+      <c r="A168" s="33"/>
+      <c r="B168" s="34"/>
+      <c r="C168" s="34"/>
       <c r="D168" s="18" t="s">
         <v>183</v>
       </c>
@@ -4236,15 +4236,15 @@
         <v>202</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="7"/>
     </row>
     <row r="170" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A170" s="35" t="s">
+      <c r="A170" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="B170" s="36"/>
-      <c r="C170" s="36"/>
+      <c r="B170" s="34"/>
+      <c r="C170" s="34"/>
       <c r="D170" s="18" t="s">
         <v>185</v>
       </c>
@@ -4259,9 +4259,9 @@
       </c>
     </row>
     <row r="171" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="35"/>
-      <c r="B171" s="36"/>
-      <c r="C171" s="36"/>
+      <c r="A171" s="33"/>
+      <c r="B171" s="34"/>
+      <c r="C171" s="34"/>
       <c r="D171" s="18" t="s">
         <v>186</v>
       </c>
@@ -4276,9 +4276,9 @@
       </c>
     </row>
     <row r="172" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="35"/>
-      <c r="B172" s="36"/>
-      <c r="C172" s="36"/>
+      <c r="A172" s="33"/>
+      <c r="B172" s="34"/>
+      <c r="C172" s="34"/>
       <c r="D172" s="18" t="s">
         <v>187</v>
       </c>
@@ -4291,9 +4291,9 @@
       <c r="G172" s="3"/>
     </row>
     <row r="173" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A173" s="35"/>
-      <c r="B173" s="36"/>
-      <c r="C173" s="36"/>
+      <c r="A173" s="33"/>
+      <c r="B173" s="34"/>
+      <c r="C173" s="34"/>
       <c r="D173" s="18" t="s">
         <v>188</v>
       </c>
@@ -4305,15 +4305,15 @@
       </c>
       <c r="G173" s="3"/>
     </row>
-    <row r="174" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="7"/>
     </row>
     <row r="175" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A175" s="35" t="s">
+      <c r="A175" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="B175" s="35"/>
-      <c r="C175" s="35"/>
+      <c r="B175" s="33"/>
+      <c r="C175" s="33"/>
       <c r="D175" s="18" t="s">
         <v>190</v>
       </c>
@@ -4326,9 +4326,9 @@
       <c r="G175" s="2"/>
     </row>
     <row r="176" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A176" s="35"/>
-      <c r="B176" s="35"/>
-      <c r="C176" s="35"/>
+      <c r="A176" s="33"/>
+      <c r="B176" s="33"/>
+      <c r="C176" s="33"/>
       <c r="D176" s="18" t="s">
         <v>191</v>
       </c>
@@ -4341,9 +4341,9 @@
       <c r="G176" s="4"/>
     </row>
     <row r="177" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="35"/>
-      <c r="B177" s="35"/>
-      <c r="C177" s="35"/>
+      <c r="A177" s="33"/>
+      <c r="B177" s="33"/>
+      <c r="C177" s="33"/>
       <c r="D177" s="18" t="s">
         <v>192</v>
       </c>
@@ -4355,10 +4355,10 @@
       </c>
       <c r="G177" s="3"/>
     </row>
-    <row r="178" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="7"/>
     </row>
-    <row r="179" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="10" t="s">
         <v>193</v>
       </c>
@@ -4375,10 +4375,10 @@
       </c>
       <c r="G179" s="2"/>
     </row>
-    <row r="180" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="7"/>
     </row>
-    <row r="181" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="7"/>
       <c r="D181" s="18" t="s">
         <v>195</v>
@@ -4391,7 +4391,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="7"/>
       <c r="D182" s="18" t="s">
         <v>196</v>
@@ -4404,7 +4404,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="7"/>
       <c r="D183" s="18" t="s">
         <v>197</v>
@@ -4425,44 +4425,38 @@
         <filter val="Only TV"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="GET"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="High"/>
-      </filters>
-    </filterColumn>
   </autoFilter>
   <mergeCells count="72">
-    <mergeCell ref="A175:A177"/>
-    <mergeCell ref="B175:B177"/>
-    <mergeCell ref="C175:C177"/>
-    <mergeCell ref="A167:A168"/>
-    <mergeCell ref="B167:B168"/>
-    <mergeCell ref="C167:C168"/>
-    <mergeCell ref="A170:A173"/>
-    <mergeCell ref="B170:B173"/>
-    <mergeCell ref="C170:C173"/>
-    <mergeCell ref="A157:A159"/>
-    <mergeCell ref="B157:B159"/>
-    <mergeCell ref="C157:C159"/>
-    <mergeCell ref="A161:A163"/>
-    <mergeCell ref="B161:B163"/>
-    <mergeCell ref="C161:C163"/>
-    <mergeCell ref="C150:C151"/>
-    <mergeCell ref="B150:B151"/>
-    <mergeCell ref="A150:A151"/>
-    <mergeCell ref="A153:A155"/>
-    <mergeCell ref="B153:B155"/>
-    <mergeCell ref="C153:C155"/>
-    <mergeCell ref="B120:B123"/>
-    <mergeCell ref="C120:C123"/>
-    <mergeCell ref="C124:C140"/>
-    <mergeCell ref="B124:B140"/>
-    <mergeCell ref="A120:A140"/>
+    <mergeCell ref="L1:L1048576"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="A44:A98"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B67:B98"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="C61:C63"/>
+    <mergeCell ref="C64:C66"/>
+    <mergeCell ref="C67:C98"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="C5:C19"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A5:A19"/>
+    <mergeCell ref="B5:B19"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="C142:C146"/>
     <mergeCell ref="B142:B146"/>
     <mergeCell ref="A142:A146"/>
@@ -4479,36 +4473,32 @@
     <mergeCell ref="B61:B63"/>
     <mergeCell ref="B56:B60"/>
     <mergeCell ref="B44:B47"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="C5:C19"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="A5:A19"/>
-    <mergeCell ref="B5:B19"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="L1:L1048576"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="A44:A98"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="B67:B98"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="C61:C63"/>
-    <mergeCell ref="C64:C66"/>
-    <mergeCell ref="C67:C98"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B120:B123"/>
+    <mergeCell ref="C120:C123"/>
+    <mergeCell ref="C124:C140"/>
+    <mergeCell ref="B124:B140"/>
+    <mergeCell ref="A120:A140"/>
+    <mergeCell ref="C150:C151"/>
+    <mergeCell ref="B150:B151"/>
+    <mergeCell ref="A150:A151"/>
+    <mergeCell ref="A153:A155"/>
+    <mergeCell ref="B153:B155"/>
+    <mergeCell ref="C153:C155"/>
+    <mergeCell ref="A157:A159"/>
+    <mergeCell ref="B157:B159"/>
+    <mergeCell ref="C157:C159"/>
+    <mergeCell ref="A161:A163"/>
+    <mergeCell ref="B161:B163"/>
+    <mergeCell ref="C161:C163"/>
+    <mergeCell ref="A175:A177"/>
+    <mergeCell ref="B175:B177"/>
+    <mergeCell ref="C175:C177"/>
+    <mergeCell ref="A167:A168"/>
+    <mergeCell ref="B167:B168"/>
+    <mergeCell ref="C167:C168"/>
+    <mergeCell ref="A170:A173"/>
+    <mergeCell ref="B170:B173"/>
+    <mergeCell ref="C170:C173"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Collection, data file and environment update
</commit_message>
<xml_diff>
--- a/docs/Census_Wsc_Services.xlsx
+++ b/docs/Census_Wsc_Services.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian.catelli/Google Drive (christian.catelli@kineton.it)/Sky/Automation IT CI:CD WSC/Repository/PostmanCollection_AutomationAPI/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7F5E86-7DD0-2746-97A5-9CE1F5F0D7FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1737396B-A34E-5C4E-99AD-E8F73702C0ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8656BBE8-7E17-AC42-8AF4-F6E9122F8590}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="233">
   <si>
     <t>Service Category</t>
   </si>
@@ -730,6 +730,9 @@
   </si>
   <si>
     <t>Attivo, Sky via Fibra in preattivazione, completo.</t>
+  </si>
+  <si>
+    <t>NOT SUPPORTED ANYMORE</t>
   </si>
 </sst>
 </file>
@@ -868,7 +871,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -964,16 +967,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1291,8 +1307,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="D53" workbookViewId="0">
+      <selection activeCell="I75" sqref="I75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1308,7 +1324,7 @@
     <col min="9" max="9" width="40" style="5" customWidth="1"/>
     <col min="10" max="10" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="35.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.83203125" style="36" customWidth="1"/>
+    <col min="12" max="12" width="7.83203125" style="33" customWidth="1"/>
     <col min="13" max="13" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="146" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
@@ -1349,7 +1365,7 @@
       <c r="K1" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="33" t="s">
         <v>227</v>
       </c>
       <c r="M1" s="6" t="s">
@@ -1401,11 +1417,11 @@
       <c r="O4" s="22"/>
     </row>
     <row r="5" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
       <c r="D5" s="16" t="s">
         <v>5</v>
       </c>
@@ -1421,9 +1437,9 @@
       <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="16" t="s">
         <v>6</v>
       </c>
@@ -1439,9 +1455,9 @@
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="35"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="16" t="s">
         <v>7</v>
       </c>
@@ -1457,9 +1473,9 @@
       <c r="O7" s="22"/>
     </row>
     <row r="8" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="35"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="16" t="s">
         <v>8</v>
       </c>
@@ -1475,9 +1491,9 @@
       <c r="O8" s="22"/>
     </row>
     <row r="9" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="16" t="s">
         <v>9</v>
       </c>
@@ -1492,9 +1508,9 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="16" t="s">
         <v>10</v>
       </c>
@@ -1509,9 +1525,9 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="35"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
       <c r="D11" s="16" t="s">
         <v>11</v>
       </c>
@@ -1526,9 +1542,9 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
       <c r="D12" s="16" t="s">
         <v>12</v>
       </c>
@@ -1543,9 +1559,9 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="16" t="s">
         <v>13</v>
       </c>
@@ -1560,9 +1576,9 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
       <c r="D14" s="16" t="s">
         <v>14</v>
       </c>
@@ -1577,9 +1593,9 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
       <c r="D15" s="16" t="s">
         <v>15</v>
       </c>
@@ -1594,9 +1610,9 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="16" t="s">
         <v>16</v>
       </c>
@@ -1611,9 +1627,9 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
       <c r="D17" s="16" t="s">
         <v>17</v>
       </c>
@@ -1628,9 +1644,9 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
       <c r="D18" s="16" t="s">
         <v>18</v>
       </c>
@@ -1645,9 +1661,9 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
       <c r="D19" s="16" t="s">
         <v>19</v>
       </c>
@@ -1667,11 +1683,11 @@
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
       <c r="D21" s="16" t="s">
         <v>21</v>
       </c>
@@ -1684,9 +1700,9 @@
       <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="35"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
       <c r="D22" s="16" t="s">
         <v>24</v>
       </c>
@@ -1699,9 +1715,9 @@
       <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="35"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
       <c r="D23" s="16" t="s">
         <v>25</v>
       </c>
@@ -1714,9 +1730,9 @@
       <c r="G23" s="12"/>
     </row>
     <row r="24" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="35"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
       <c r="D24" s="16" t="s">
         <v>26</v>
       </c>
@@ -1729,9 +1745,9 @@
       <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="35"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
       <c r="D25" s="16" t="s">
         <v>27</v>
       </c>
@@ -1749,11 +1765,11 @@
       <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
       <c r="D27" s="16" t="s">
         <v>30</v>
       </c>
@@ -1777,9 +1793,9 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="35"/>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
       <c r="D28" s="16" t="s">
         <v>31</v>
       </c>
@@ -1797,11 +1813,11 @@
       <c r="G29" s="13"/>
     </row>
     <row r="30" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
       <c r="D30" s="16" t="s">
         <v>34</v>
       </c>
@@ -1825,9 +1841,9 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="35"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="35"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
       <c r="D31" s="16" t="s">
         <v>35</v>
       </c>
@@ -1854,9 +1870,9 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="35"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="35"/>
+      <c r="A32" s="34"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
       <c r="D32" s="16" t="s">
         <v>36</v>
       </c>
@@ -1869,9 +1885,9 @@
       <c r="G32" s="14"/>
     </row>
     <row r="33" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="35"/>
-      <c r="B33" s="35"/>
-      <c r="C33" s="35"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
       <c r="D33" s="16" t="s">
         <v>37</v>
       </c>
@@ -1889,11 +1905,11 @@
       <c r="G34" s="14"/>
     </row>
     <row r="35" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="35"/>
-      <c r="C35" s="35"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
       <c r="D35" s="16" t="s">
         <v>40</v>
       </c>
@@ -1906,9 +1922,9 @@
       <c r="G35" s="13"/>
     </row>
     <row r="36" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="35"/>
-      <c r="B36" s="35"/>
-      <c r="C36" s="35"/>
+      <c r="A36" s="34"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
       <c r="D36" s="16" t="s">
         <v>41</v>
       </c>
@@ -1929,9 +1945,9 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="35"/>
-      <c r="B37" s="35"/>
-      <c r="C37" s="35"/>
+      <c r="A37" s="34"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
       <c r="D37" s="16" t="s">
         <v>42</v>
       </c>
@@ -1985,11 +2001,11 @@
       <c r="G40" s="11"/>
     </row>
     <row r="41" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="35"/>
-      <c r="C41" s="35"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
       <c r="D41" s="16" t="s">
         <v>46</v>
       </c>
@@ -2002,9 +2018,9 @@
       <c r="G41" s="12"/>
     </row>
     <row r="42" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="35"/>
-      <c r="B42" s="35"/>
-      <c r="C42" s="35"/>
+      <c r="A42" s="34"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="34"/>
       <c r="D42" s="16" t="s">
         <v>47</v>
       </c>
@@ -2022,13 +2038,13 @@
       <c r="G43" s="12"/>
     </row>
     <row r="44" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="35" t="s">
+      <c r="A44" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="35"/>
+      <c r="C44" s="34"/>
       <c r="D44" s="16" t="s">
         <v>51</v>
       </c>
@@ -2041,9 +2057,9 @@
       <c r="G44" s="12"/>
     </row>
     <row r="45" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
-      <c r="C45" s="35"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
       <c r="D45" s="16" t="s">
         <v>52</v>
       </c>
@@ -2056,9 +2072,9 @@
       <c r="G45" s="12"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="35"/>
-      <c r="B46" s="35"/>
-      <c r="C46" s="35"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="34"/>
       <c r="D46" s="16" t="s">
         <v>53</v>
       </c>
@@ -2082,9 +2098,9 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="35"/>
-      <c r="B47" s="35"/>
-      <c r="C47" s="35"/>
+      <c r="A47" s="34"/>
+      <c r="B47" s="34"/>
+      <c r="C47" s="34"/>
       <c r="D47" s="16" t="s">
         <v>54</v>
       </c>
@@ -2111,11 +2127,11 @@
       </c>
     </row>
     <row r="48" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="35"/>
-      <c r="B48" s="35" t="s">
+      <c r="A48" s="34"/>
+      <c r="B48" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="C48" s="35"/>
+      <c r="C48" s="34"/>
       <c r="D48" s="16" t="s">
         <v>56</v>
       </c>
@@ -2125,9 +2141,9 @@
       <c r="G48" s="12"/>
     </row>
     <row r="49" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="35"/>
-      <c r="B49" s="35"/>
-      <c r="C49" s="35"/>
+      <c r="A49" s="34"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="34"/>
       <c r="D49" s="16" t="s">
         <v>57</v>
       </c>
@@ -2137,11 +2153,11 @@
       <c r="G49" s="12"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="35"/>
-      <c r="B50" s="35" t="s">
+      <c r="A50" s="34"/>
+      <c r="B50" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C50" s="35"/>
+      <c r="C50" s="34"/>
       <c r="D50" s="16" t="s">
         <v>59</v>
       </c>
@@ -2156,9 +2172,9 @@
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" s="35"/>
-      <c r="B51" s="35"/>
-      <c r="C51" s="35"/>
+      <c r="A51" s="34"/>
+      <c r="B51" s="34"/>
+      <c r="C51" s="34"/>
       <c r="D51" s="16" t="s">
         <v>60</v>
       </c>
@@ -2173,11 +2189,11 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" s="35"/>
-      <c r="B52" s="35" t="s">
+      <c r="A52" s="34"/>
+      <c r="B52" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="C52" s="35"/>
+      <c r="C52" s="34"/>
       <c r="D52" s="16" t="s">
         <v>62</v>
       </c>
@@ -2201,9 +2217,9 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" s="35"/>
-      <c r="B53" s="35"/>
-      <c r="C53" s="35"/>
+      <c r="A53" s="34"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="34"/>
       <c r="D53" s="16" t="s">
         <v>63</v>
       </c>
@@ -2230,7 +2246,7 @@
       </c>
     </row>
     <row r="54" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="35"/>
+      <c r="A54" s="34"/>
       <c r="B54" s="7" t="s">
         <v>64</v>
       </c>
@@ -2245,7 +2261,7 @@
       </c>
     </row>
     <row r="55" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="35"/>
+      <c r="A55" s="34"/>
       <c r="B55" s="7" t="s">
         <v>66</v>
       </c>
@@ -2260,11 +2276,11 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A56" s="35"/>
-      <c r="B56" s="35" t="s">
+      <c r="A56" s="34"/>
+      <c r="B56" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="C56" s="35" t="s">
+      <c r="C56" s="34" t="s">
         <v>68</v>
       </c>
       <c r="D56" s="16" t="s">
@@ -2281,9 +2297,9 @@
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A57" s="35"/>
-      <c r="B57" s="35"/>
-      <c r="C57" s="35"/>
+      <c r="A57" s="34"/>
+      <c r="B57" s="34"/>
+      <c r="C57" s="34"/>
       <c r="D57" s="16" t="s">
         <v>70</v>
       </c>
@@ -2298,9 +2314,9 @@
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A58" s="35"/>
-      <c r="B58" s="35"/>
-      <c r="C58" s="35"/>
+      <c r="A58" s="34"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="34"/>
       <c r="D58" s="16" t="s">
         <v>73</v>
       </c>
@@ -2315,9 +2331,9 @@
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A59" s="35"/>
-      <c r="B59" s="35"/>
-      <c r="C59" s="35"/>
+      <c r="A59" s="34"/>
+      <c r="B59" s="34"/>
+      <c r="C59" s="34"/>
       <c r="D59" s="16" t="s">
         <v>74</v>
       </c>
@@ -2332,9 +2348,9 @@
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A60" s="35"/>
-      <c r="B60" s="35"/>
-      <c r="C60" s="35"/>
+      <c r="A60" s="34"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="34"/>
       <c r="D60" s="16" t="s">
         <v>75</v>
       </c>
@@ -2349,11 +2365,11 @@
       </c>
     </row>
     <row r="61" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="35"/>
-      <c r="B61" s="35" t="s">
+      <c r="A61" s="34"/>
+      <c r="B61" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="C61" s="35"/>
+      <c r="C61" s="34"/>
       <c r="D61" s="16" t="s">
         <v>77</v>
       </c>
@@ -2366,9 +2382,9 @@
       <c r="G61" s="12"/>
     </row>
     <row r="62" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="35"/>
-      <c r="B62" s="35"/>
-      <c r="C62" s="35"/>
+      <c r="A62" s="34"/>
+      <c r="B62" s="34"/>
+      <c r="C62" s="34"/>
       <c r="D62" s="16" t="s">
         <v>78</v>
       </c>
@@ -2381,9 +2397,9 @@
       <c r="G62" s="12"/>
     </row>
     <row r="63" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="35"/>
-      <c r="B63" s="35"/>
-      <c r="C63" s="35"/>
+      <c r="A63" s="34"/>
+      <c r="B63" s="34"/>
+      <c r="C63" s="34"/>
       <c r="D63" s="16" t="s">
         <v>79</v>
       </c>
@@ -2396,11 +2412,11 @@
       <c r="G63" s="12"/>
     </row>
     <row r="64" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="35"/>
-      <c r="B64" s="35" t="s">
+      <c r="A64" s="34"/>
+      <c r="B64" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="C64" s="35"/>
+      <c r="C64" s="34"/>
       <c r="D64" s="16" t="s">
         <v>81</v>
       </c>
@@ -2413,9 +2429,9 @@
       <c r="G64" s="12"/>
     </row>
     <row r="65" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="35"/>
-      <c r="B65" s="35"/>
-      <c r="C65" s="35"/>
+      <c r="A65" s="34"/>
+      <c r="B65" s="34"/>
+      <c r="C65" s="34"/>
       <c r="D65" s="16" t="s">
         <v>82</v>
       </c>
@@ -2428,9 +2444,9 @@
       <c r="G65" s="12"/>
     </row>
     <row r="66" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="35"/>
-      <c r="B66" s="35"/>
-      <c r="C66" s="35"/>
+      <c r="A66" s="34"/>
+      <c r="B66" s="34"/>
+      <c r="C66" s="34"/>
       <c r="D66" s="16" t="s">
         <v>83</v>
       </c>
@@ -2443,9 +2459,9 @@
       <c r="G66" s="12"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A67" s="35"/>
-      <c r="B67" s="35"/>
-      <c r="C67" s="35"/>
+      <c r="A67" s="34"/>
+      <c r="B67" s="34"/>
+      <c r="C67" s="34"/>
       <c r="D67" s="16" t="s">
         <v>84</v>
       </c>
@@ -2469,9 +2485,9 @@
       </c>
     </row>
     <row r="68" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="35"/>
-      <c r="B68" s="35"/>
-      <c r="C68" s="35"/>
+      <c r="A68" s="34"/>
+      <c r="B68" s="34"/>
+      <c r="C68" s="34"/>
       <c r="D68" s="16" t="s">
         <v>85</v>
       </c>
@@ -2492,9 +2508,9 @@
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69" s="35"/>
-      <c r="B69" s="35"/>
-      <c r="C69" s="35"/>
+      <c r="A69" s="34"/>
+      <c r="B69" s="34"/>
+      <c r="C69" s="34"/>
       <c r="D69" s="16" t="s">
         <v>86</v>
       </c>
@@ -2518,9 +2534,9 @@
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A70" s="35"/>
-      <c r="B70" s="35"/>
-      <c r="C70" s="35"/>
+      <c r="A70" s="34"/>
+      <c r="B70" s="34"/>
+      <c r="C70" s="34"/>
       <c r="D70" s="16" t="s">
         <v>87</v>
       </c>
@@ -2544,9 +2560,9 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A71" s="35"/>
-      <c r="B71" s="35"/>
-      <c r="C71" s="35"/>
+      <c r="A71" s="34"/>
+      <c r="B71" s="34"/>
+      <c r="C71" s="34"/>
       <c r="D71" s="16" t="s">
         <v>88</v>
       </c>
@@ -2570,9 +2586,9 @@
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A72" s="35"/>
-      <c r="B72" s="35"/>
-      <c r="C72" s="35"/>
+      <c r="A72" s="34"/>
+      <c r="B72" s="34"/>
+      <c r="C72" s="34"/>
       <c r="D72" s="16" t="s">
         <v>89</v>
       </c>
@@ -2596,9 +2612,9 @@
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A73" s="35"/>
-      <c r="B73" s="35"/>
-      <c r="C73" s="35"/>
+      <c r="A73" s="34"/>
+      <c r="B73" s="34"/>
+      <c r="C73" s="34"/>
       <c r="D73" s="16" t="s">
         <v>90</v>
       </c>
@@ -2625,9 +2641,9 @@
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A74" s="35"/>
-      <c r="B74" s="35"/>
-      <c r="C74" s="35"/>
+      <c r="A74" s="34"/>
+      <c r="B74" s="34"/>
+      <c r="C74" s="34"/>
       <c r="D74" s="16" t="s">
         <v>91</v>
       </c>
@@ -2654,35 +2670,34 @@
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A75" s="35"/>
-      <c r="B75" s="35"/>
-      <c r="C75" s="35"/>
-      <c r="D75" s="16" t="s">
+      <c r="A75" s="34"/>
+      <c r="B75" s="34"/>
+      <c r="C75" s="34"/>
+      <c r="D75" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="E75" s="25" t="s">
-        <v>222</v>
-      </c>
-      <c r="F75" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G75" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="H75" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="J75" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="K75" s="5" t="s">
-        <v>214</v>
-      </c>
+      <c r="E75" s="38" t="s">
+        <v>222</v>
+      </c>
+      <c r="F75" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G75" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="H75" s="38" t="s">
+        <v>207</v>
+      </c>
+      <c r="I75" s="40" t="s">
+        <v>232</v>
+      </c>
+      <c r="J75" s="41"/>
+      <c r="K75" s="40"/>
     </row>
     <row r="76" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="35"/>
-      <c r="B76" s="35"/>
-      <c r="C76" s="35"/>
+      <c r="A76" s="34"/>
+      <c r="B76" s="34"/>
+      <c r="C76" s="34"/>
       <c r="D76" s="16" t="s">
         <v>93</v>
       </c>
@@ -2706,9 +2721,9 @@
       </c>
     </row>
     <row r="77" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="35"/>
-      <c r="B77" s="35"/>
-      <c r="C77" s="35"/>
+      <c r="A77" s="34"/>
+      <c r="B77" s="34"/>
+      <c r="C77" s="34"/>
       <c r="D77" s="16" t="s">
         <v>94</v>
       </c>
@@ -2729,9 +2744,9 @@
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A78" s="35"/>
-      <c r="B78" s="35"/>
-      <c r="C78" s="35"/>
+      <c r="A78" s="34"/>
+      <c r="B78" s="34"/>
+      <c r="C78" s="34"/>
       <c r="D78" s="16" t="s">
         <v>95</v>
       </c>
@@ -2755,9 +2770,9 @@
       </c>
     </row>
     <row r="79" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="35"/>
-      <c r="B79" s="35"/>
-      <c r="C79" s="35"/>
+      <c r="A79" s="34"/>
+      <c r="B79" s="34"/>
+      <c r="C79" s="34"/>
       <c r="D79" s="24" t="s">
         <v>96</v>
       </c>
@@ -2781,9 +2796,9 @@
       </c>
     </row>
     <row r="80" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="35"/>
-      <c r="B80" s="35"/>
-      <c r="C80" s="35"/>
+      <c r="A80" s="34"/>
+      <c r="B80" s="34"/>
+      <c r="C80" s="34"/>
       <c r="D80" s="24" t="s">
         <v>97</v>
       </c>
@@ -2804,9 +2819,9 @@
       </c>
     </row>
     <row r="81" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="35"/>
-      <c r="B81" s="35"/>
-      <c r="C81" s="35"/>
+      <c r="A81" s="34"/>
+      <c r="B81" s="34"/>
+      <c r="C81" s="34"/>
       <c r="D81" s="16" t="s">
         <v>98</v>
       </c>
@@ -2819,9 +2834,9 @@
       <c r="G81" s="13"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A82" s="35"/>
-      <c r="B82" s="35"/>
-      <c r="C82" s="35"/>
+      <c r="A82" s="34"/>
+      <c r="B82" s="34"/>
+      <c r="C82" s="34"/>
       <c r="D82" s="24" t="s">
         <v>99</v>
       </c>
@@ -2848,9 +2863,9 @@
       </c>
     </row>
     <row r="83" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="35"/>
-      <c r="B83" s="35"/>
-      <c r="C83" s="35"/>
+      <c r="A83" s="34"/>
+      <c r="B83" s="34"/>
+      <c r="C83" s="34"/>
       <c r="D83" s="24" t="s">
         <v>100</v>
       </c>
@@ -2877,9 +2892,9 @@
       </c>
     </row>
     <row r="84" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="35"/>
-      <c r="B84" s="35"/>
-      <c r="C84" s="35"/>
+      <c r="A84" s="34"/>
+      <c r="B84" s="34"/>
+      <c r="C84" s="34"/>
       <c r="D84" s="24" t="s">
         <v>101</v>
       </c>
@@ -2906,9 +2921,9 @@
       </c>
     </row>
     <row r="85" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="35"/>
-      <c r="B85" s="35"/>
-      <c r="C85" s="35"/>
+      <c r="A85" s="34"/>
+      <c r="B85" s="34"/>
+      <c r="C85" s="34"/>
       <c r="D85" s="24" t="s">
         <v>102</v>
       </c>
@@ -2935,9 +2950,9 @@
       </c>
     </row>
     <row r="86" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="35"/>
-      <c r="B86" s="35"/>
-      <c r="C86" s="35"/>
+      <c r="A86" s="34"/>
+      <c r="B86" s="34"/>
+      <c r="C86" s="34"/>
       <c r="D86" s="24" t="s">
         <v>103</v>
       </c>
@@ -2964,9 +2979,9 @@
       </c>
     </row>
     <row r="87" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="35"/>
-      <c r="B87" s="35"/>
-      <c r="C87" s="35"/>
+      <c r="A87" s="34"/>
+      <c r="B87" s="34"/>
+      <c r="C87" s="34"/>
       <c r="D87" s="16" t="s">
         <v>104</v>
       </c>
@@ -2979,9 +2994,9 @@
       <c r="G87" s="13"/>
     </row>
     <row r="88" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="35"/>
-      <c r="B88" s="35"/>
-      <c r="C88" s="35"/>
+      <c r="A88" s="34"/>
+      <c r="B88" s="34"/>
+      <c r="C88" s="34"/>
       <c r="D88" s="16" t="s">
         <v>105</v>
       </c>
@@ -2994,9 +3009,9 @@
       <c r="G88" s="13"/>
     </row>
     <row r="89" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="35"/>
-      <c r="B89" s="35"/>
-      <c r="C89" s="35"/>
+      <c r="A89" s="34"/>
+      <c r="B89" s="34"/>
+      <c r="C89" s="34"/>
       <c r="D89" s="16" t="s">
         <v>106</v>
       </c>
@@ -3009,9 +3024,9 @@
       <c r="G89" s="13"/>
     </row>
     <row r="90" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="35"/>
-      <c r="B90" s="35"/>
-      <c r="C90" s="35"/>
+      <c r="A90" s="34"/>
+      <c r="B90" s="34"/>
+      <c r="C90" s="34"/>
       <c r="D90" s="16" t="s">
         <v>107</v>
       </c>
@@ -3024,9 +3039,9 @@
       <c r="G90" s="13"/>
     </row>
     <row r="91" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="35"/>
-      <c r="B91" s="35"/>
-      <c r="C91" s="35"/>
+      <c r="A91" s="34"/>
+      <c r="B91" s="34"/>
+      <c r="C91" s="34"/>
       <c r="D91" s="16" t="s">
         <v>108</v>
       </c>
@@ -3039,9 +3054,9 @@
       <c r="G91" s="13"/>
     </row>
     <row r="92" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="35"/>
-      <c r="B92" s="35"/>
-      <c r="C92" s="35"/>
+      <c r="A92" s="34"/>
+      <c r="B92" s="34"/>
+      <c r="C92" s="34"/>
       <c r="D92" s="16" t="s">
         <v>109</v>
       </c>
@@ -3054,9 +3069,9 @@
       <c r="G92" s="13"/>
     </row>
     <row r="93" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="35"/>
-      <c r="B93" s="35"/>
-      <c r="C93" s="35"/>
+      <c r="A93" s="34"/>
+      <c r="B93" s="34"/>
+      <c r="C93" s="34"/>
       <c r="D93" s="16" t="s">
         <v>110</v>
       </c>
@@ -3069,9 +3084,9 @@
       <c r="G93" s="13"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A94" s="35"/>
-      <c r="B94" s="35"/>
-      <c r="C94" s="35"/>
+      <c r="A94" s="34"/>
+      <c r="B94" s="34"/>
+      <c r="C94" s="34"/>
       <c r="D94" s="24" t="s">
         <v>111</v>
       </c>
@@ -3095,9 +3110,9 @@
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A95" s="35"/>
-      <c r="B95" s="35"/>
-      <c r="C95" s="35"/>
+      <c r="A95" s="34"/>
+      <c r="B95" s="34"/>
+      <c r="C95" s="34"/>
       <c r="D95" s="24" t="s">
         <v>112</v>
       </c>
@@ -3121,9 +3136,9 @@
       </c>
     </row>
     <row r="96" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="35"/>
-      <c r="B96" s="35"/>
-      <c r="C96" s="35"/>
+      <c r="A96" s="34"/>
+      <c r="B96" s="34"/>
+      <c r="C96" s="34"/>
       <c r="D96" s="16" t="s">
         <v>113</v>
       </c>
@@ -3136,9 +3151,9 @@
       <c r="G96" s="12"/>
     </row>
     <row r="97" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="35"/>
-      <c r="B97" s="35"/>
-      <c r="C97" s="35"/>
+      <c r="A97" s="34"/>
+      <c r="B97" s="34"/>
+      <c r="C97" s="34"/>
       <c r="D97" s="16" t="s">
         <v>114</v>
       </c>
@@ -3151,9 +3166,9 @@
       <c r="G97" s="12"/>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A98" s="35"/>
-      <c r="B98" s="35"/>
-      <c r="C98" s="35"/>
+      <c r="A98" s="34"/>
+      <c r="B98" s="34"/>
+      <c r="C98" s="34"/>
       <c r="D98" s="24" t="s">
         <v>115</v>
       </c>
@@ -3182,11 +3197,11 @@
       <c r="G99" s="11"/>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A100" s="33" t="s">
+      <c r="A100" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="B100" s="33"/>
-      <c r="C100" s="33"/>
+      <c r="B100" s="35"/>
+      <c r="C100" s="35"/>
       <c r="D100" s="16" t="s">
         <v>117</v>
       </c>
@@ -3201,9 +3216,9 @@
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A101" s="33"/>
-      <c r="B101" s="33"/>
-      <c r="C101" s="33"/>
+      <c r="A101" s="35"/>
+      <c r="B101" s="35"/>
+      <c r="C101" s="35"/>
       <c r="D101" s="16" t="s">
         <v>118</v>
       </c>
@@ -3218,9 +3233,9 @@
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A102" s="33"/>
-      <c r="B102" s="33"/>
-      <c r="C102" s="33"/>
+      <c r="A102" s="35"/>
+      <c r="B102" s="35"/>
+      <c r="C102" s="35"/>
       <c r="D102" s="16" t="s">
         <v>119</v>
       </c>
@@ -3235,9 +3250,9 @@
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A103" s="33"/>
-      <c r="B103" s="33"/>
-      <c r="C103" s="33"/>
+      <c r="A103" s="35"/>
+      <c r="B103" s="35"/>
+      <c r="C103" s="35"/>
       <c r="D103" s="16" t="s">
         <v>120</v>
       </c>
@@ -3252,9 +3267,9 @@
       </c>
     </row>
     <row r="104" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="35"/>
-      <c r="B104" s="33"/>
-      <c r="C104" s="33"/>
+      <c r="A104" s="34"/>
+      <c r="B104" s="35"/>
+      <c r="C104" s="35"/>
       <c r="D104" s="16" t="s">
         <v>121</v>
       </c>
@@ -3267,9 +3282,9 @@
       <c r="G104" s="12"/>
     </row>
     <row r="105" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="35"/>
-      <c r="B105" s="33"/>
-      <c r="C105" s="33"/>
+      <c r="A105" s="34"/>
+      <c r="B105" s="35"/>
+      <c r="C105" s="35"/>
       <c r="D105" s="16" t="s">
         <v>122</v>
       </c>
@@ -3282,9 +3297,9 @@
       <c r="G105" s="12"/>
     </row>
     <row r="106" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="35"/>
-      <c r="B106" s="33"/>
-      <c r="C106" s="33"/>
+      <c r="A106" s="34"/>
+      <c r="B106" s="35"/>
+      <c r="C106" s="35"/>
       <c r="D106" s="16" t="s">
         <v>123</v>
       </c>
@@ -3297,9 +3312,9 @@
       <c r="G106" s="12"/>
     </row>
     <row r="107" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="35"/>
-      <c r="B107" s="33"/>
-      <c r="C107" s="33"/>
+      <c r="A107" s="34"/>
+      <c r="B107" s="35"/>
+      <c r="C107" s="35"/>
       <c r="D107" s="16" t="s">
         <v>124</v>
       </c>
@@ -3312,9 +3327,9 @@
       <c r="G107" s="12"/>
     </row>
     <row r="108" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="35"/>
-      <c r="B108" s="33"/>
-      <c r="C108" s="33"/>
+      <c r="A108" s="34"/>
+      <c r="B108" s="35"/>
+      <c r="C108" s="35"/>
       <c r="D108" s="16" t="s">
         <v>125</v>
       </c>
@@ -3327,9 +3342,9 @@
       <c r="G108" s="12"/>
     </row>
     <row r="109" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="35"/>
-      <c r="B109" s="33"/>
-      <c r="C109" s="33"/>
+      <c r="A109" s="34"/>
+      <c r="B109" s="35"/>
+      <c r="C109" s="35"/>
       <c r="D109" s="16" t="s">
         <v>126</v>
       </c>
@@ -3342,9 +3357,9 @@
       <c r="G109" s="12"/>
     </row>
     <row r="110" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="35"/>
-      <c r="B110" s="33"/>
-      <c r="C110" s="33"/>
+      <c r="A110" s="34"/>
+      <c r="B110" s="35"/>
+      <c r="C110" s="35"/>
       <c r="D110" s="16" t="s">
         <v>127</v>
       </c>
@@ -3357,9 +3372,9 @@
       <c r="G110" s="12"/>
     </row>
     <row r="111" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="35"/>
-      <c r="B111" s="33"/>
-      <c r="C111" s="33"/>
+      <c r="A111" s="34"/>
+      <c r="B111" s="35"/>
+      <c r="C111" s="35"/>
       <c r="D111" s="16" t="s">
         <v>128</v>
       </c>
@@ -3372,9 +3387,9 @@
       <c r="G111" s="12"/>
     </row>
     <row r="112" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="35"/>
-      <c r="B112" s="33"/>
-      <c r="C112" s="33"/>
+      <c r="A112" s="34"/>
+      <c r="B112" s="35"/>
+      <c r="C112" s="35"/>
       <c r="D112" s="16" t="s">
         <v>129</v>
       </c>
@@ -3387,9 +3402,9 @@
       <c r="G112" s="13"/>
     </row>
     <row r="113" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="35"/>
-      <c r="B113" s="33"/>
-      <c r="C113" s="33"/>
+      <c r="A113" s="34"/>
+      <c r="B113" s="35"/>
+      <c r="C113" s="35"/>
       <c r="D113" s="16" t="s">
         <v>130</v>
       </c>
@@ -3402,9 +3417,9 @@
       <c r="G113" s="13"/>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A114" s="33"/>
-      <c r="B114" s="33"/>
-      <c r="C114" s="33"/>
+      <c r="A114" s="35"/>
+      <c r="B114" s="35"/>
+      <c r="C114" s="35"/>
       <c r="D114" s="16" t="s">
         <v>131</v>
       </c>
@@ -3419,9 +3434,9 @@
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A115" s="33"/>
-      <c r="B115" s="33"/>
-      <c r="C115" s="33"/>
+      <c r="A115" s="35"/>
+      <c r="B115" s="35"/>
+      <c r="C115" s="35"/>
       <c r="D115" s="16" t="s">
         <v>132</v>
       </c>
@@ -3439,11 +3454,11 @@
       <c r="A116" s="7"/>
     </row>
     <row r="117" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="33" t="s">
+      <c r="A117" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="B117" s="33"/>
-      <c r="C117" s="33"/>
+      <c r="B117" s="35"/>
+      <c r="C117" s="35"/>
       <c r="D117" s="16" t="s">
         <v>134</v>
       </c>
@@ -3456,9 +3471,9 @@
       <c r="G117" s="12"/>
     </row>
     <row r="118" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="33"/>
-      <c r="B118" s="33"/>
-      <c r="C118" s="33"/>
+      <c r="A118" s="35"/>
+      <c r="B118" s="35"/>
+      <c r="C118" s="35"/>
       <c r="D118" s="16" t="s">
         <v>135</v>
       </c>
@@ -3474,13 +3489,13 @@
       <c r="A119" s="7"/>
     </row>
     <row r="120" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="35" t="s">
+      <c r="A120" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="B120" s="33" t="s">
+      <c r="B120" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="C120" s="33"/>
+      <c r="C120" s="35"/>
       <c r="D120" s="16" t="s">
         <v>138</v>
       </c>
@@ -3495,9 +3510,9 @@
       </c>
     </row>
     <row r="121" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="35"/>
-      <c r="B121" s="33"/>
-      <c r="C121" s="33"/>
+      <c r="A121" s="34"/>
+      <c r="B121" s="35"/>
+      <c r="C121" s="35"/>
       <c r="D121" s="16" t="s">
         <v>139</v>
       </c>
@@ -3512,9 +3527,9 @@
       </c>
     </row>
     <row r="122" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="35"/>
-      <c r="B122" s="33"/>
-      <c r="C122" s="33"/>
+      <c r="A122" s="34"/>
+      <c r="B122" s="35"/>
+      <c r="C122" s="35"/>
       <c r="D122" s="16" t="s">
         <v>140</v>
       </c>
@@ -3529,9 +3544,9 @@
       </c>
     </row>
     <row r="123" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="35"/>
-      <c r="B123" s="33"/>
-      <c r="C123" s="33"/>
+      <c r="A123" s="34"/>
+      <c r="B123" s="35"/>
+      <c r="C123" s="35"/>
       <c r="D123" s="16" t="s">
         <v>141</v>
       </c>
@@ -3546,9 +3561,9 @@
       </c>
     </row>
     <row r="124" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="35"/>
-      <c r="B124" s="33"/>
-      <c r="C124" s="33"/>
+      <c r="A124" s="34"/>
+      <c r="B124" s="35"/>
+      <c r="C124" s="35"/>
       <c r="D124" s="24" t="s">
         <v>142</v>
       </c>
@@ -3572,9 +3587,9 @@
       </c>
     </row>
     <row r="125" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="35"/>
-      <c r="B125" s="33"/>
-      <c r="C125" s="33"/>
+      <c r="A125" s="34"/>
+      <c r="B125" s="35"/>
+      <c r="C125" s="35"/>
       <c r="D125" s="24" t="s">
         <v>143</v>
       </c>
@@ -3592,9 +3607,9 @@
       </c>
     </row>
     <row r="126" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="35"/>
-      <c r="B126" s="33"/>
-      <c r="C126" s="33"/>
+      <c r="A126" s="34"/>
+      <c r="B126" s="35"/>
+      <c r="C126" s="35"/>
       <c r="D126" s="24" t="s">
         <v>144</v>
       </c>
@@ -3612,9 +3627,9 @@
       </c>
     </row>
     <row r="127" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="35"/>
-      <c r="B127" s="33"/>
-      <c r="C127" s="33"/>
+      <c r="A127" s="34"/>
+      <c r="B127" s="35"/>
+      <c r="C127" s="35"/>
       <c r="D127" s="24" t="s">
         <v>145</v>
       </c>
@@ -3632,9 +3647,9 @@
       </c>
     </row>
     <row r="128" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="35"/>
-      <c r="B128" s="33"/>
-      <c r="C128" s="33"/>
+      <c r="A128" s="34"/>
+      <c r="B128" s="35"/>
+      <c r="C128" s="35"/>
       <c r="D128" s="24" t="s">
         <v>146</v>
       </c>
@@ -3652,9 +3667,9 @@
       </c>
     </row>
     <row r="129" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="35"/>
-      <c r="B129" s="33"/>
-      <c r="C129" s="33"/>
+      <c r="A129" s="34"/>
+      <c r="B129" s="35"/>
+      <c r="C129" s="35"/>
       <c r="D129" s="24" t="s">
         <v>147</v>
       </c>
@@ -3672,9 +3687,9 @@
       </c>
     </row>
     <row r="130" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="35"/>
-      <c r="B130" s="33"/>
-      <c r="C130" s="33"/>
+      <c r="A130" s="34"/>
+      <c r="B130" s="35"/>
+      <c r="C130" s="35"/>
       <c r="D130" s="24" t="s">
         <v>148</v>
       </c>
@@ -3692,9 +3707,9 @@
       </c>
     </row>
     <row r="131" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="35"/>
-      <c r="B131" s="33"/>
-      <c r="C131" s="33"/>
+      <c r="A131" s="34"/>
+      <c r="B131" s="35"/>
+      <c r="C131" s="35"/>
       <c r="D131" s="24" t="s">
         <v>149</v>
       </c>
@@ -3712,9 +3727,9 @@
       </c>
     </row>
     <row r="132" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="35"/>
-      <c r="B132" s="33"/>
-      <c r="C132" s="33"/>
+      <c r="A132" s="34"/>
+      <c r="B132" s="35"/>
+      <c r="C132" s="35"/>
       <c r="D132" s="24" t="s">
         <v>150</v>
       </c>
@@ -3732,9 +3747,9 @@
       </c>
     </row>
     <row r="133" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="35"/>
-      <c r="B133" s="33"/>
-      <c r="C133" s="33"/>
+      <c r="A133" s="34"/>
+      <c r="B133" s="35"/>
+      <c r="C133" s="35"/>
       <c r="D133" s="24" t="s">
         <v>151</v>
       </c>
@@ -3752,9 +3767,9 @@
       </c>
     </row>
     <row r="134" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="35"/>
-      <c r="B134" s="33"/>
-      <c r="C134" s="33"/>
+      <c r="A134" s="34"/>
+      <c r="B134" s="35"/>
+      <c r="C134" s="35"/>
       <c r="D134" s="24" t="s">
         <v>152</v>
       </c>
@@ -3772,9 +3787,9 @@
       </c>
     </row>
     <row r="135" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="35"/>
-      <c r="B135" s="33"/>
-      <c r="C135" s="33"/>
+      <c r="A135" s="34"/>
+      <c r="B135" s="35"/>
+      <c r="C135" s="35"/>
       <c r="D135" s="24" t="s">
         <v>153</v>
       </c>
@@ -3792,9 +3807,9 @@
       </c>
     </row>
     <row r="136" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="35"/>
-      <c r="B136" s="33"/>
-      <c r="C136" s="33"/>
+      <c r="A136" s="34"/>
+      <c r="B136" s="35"/>
+      <c r="C136" s="35"/>
       <c r="D136" s="24" t="s">
         <v>154</v>
       </c>
@@ -3812,9 +3827,9 @@
       </c>
     </row>
     <row r="137" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="35"/>
-      <c r="B137" s="33"/>
-      <c r="C137" s="33"/>
+      <c r="A137" s="34"/>
+      <c r="B137" s="35"/>
+      <c r="C137" s="35"/>
       <c r="D137" s="24" t="s">
         <v>155</v>
       </c>
@@ -3832,9 +3847,9 @@
       </c>
     </row>
     <row r="138" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="35"/>
-      <c r="B138" s="33"/>
-      <c r="C138" s="33"/>
+      <c r="A138" s="34"/>
+      <c r="B138" s="35"/>
+      <c r="C138" s="35"/>
       <c r="D138" s="24" t="s">
         <v>156</v>
       </c>
@@ -3852,9 +3867,9 @@
       </c>
     </row>
     <row r="139" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="35"/>
-      <c r="B139" s="33"/>
-      <c r="C139" s="33"/>
+      <c r="A139" s="34"/>
+      <c r="B139" s="35"/>
+      <c r="C139" s="35"/>
       <c r="D139" s="16" t="s">
         <v>157</v>
       </c>
@@ -3867,9 +3882,9 @@
       <c r="G139" s="15"/>
     </row>
     <row r="140" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A140" s="35"/>
-      <c r="B140" s="33"/>
-      <c r="C140" s="33"/>
+      <c r="A140" s="34"/>
+      <c r="B140" s="35"/>
+      <c r="C140" s="35"/>
       <c r="D140" s="16" t="s">
         <v>158</v>
       </c>
@@ -3887,11 +3902,11 @@
       <c r="C141" s="10"/>
     </row>
     <row r="142" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="33" t="s">
+      <c r="A142" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="B142" s="33"/>
-      <c r="C142" s="33"/>
+      <c r="B142" s="35"/>
+      <c r="C142" s="35"/>
       <c r="D142" s="16" t="s">
         <v>160</v>
       </c>
@@ -3904,9 +3919,9 @@
       <c r="G142" s="12"/>
     </row>
     <row r="143" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="33"/>
-      <c r="B143" s="33"/>
-      <c r="C143" s="33"/>
+      <c r="A143" s="35"/>
+      <c r="B143" s="35"/>
+      <c r="C143" s="35"/>
       <c r="D143" s="16" t="s">
         <v>160</v>
       </c>
@@ -3919,9 +3934,9 @@
       <c r="G143" s="12"/>
     </row>
     <row r="144" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="33"/>
-      <c r="B144" s="33"/>
-      <c r="C144" s="33"/>
+      <c r="A144" s="35"/>
+      <c r="B144" s="35"/>
+      <c r="C144" s="35"/>
       <c r="D144" s="16" t="s">
         <v>161</v>
       </c>
@@ -3934,9 +3949,9 @@
       <c r="G144" s="12"/>
     </row>
     <row r="145" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="33"/>
-      <c r="B145" s="33"/>
-      <c r="C145" s="33"/>
+      <c r="A145" s="35"/>
+      <c r="B145" s="35"/>
+      <c r="C145" s="35"/>
       <c r="D145" s="16" t="s">
         <v>162</v>
       </c>
@@ -3949,9 +3964,9 @@
       <c r="G145" s="13"/>
     </row>
     <row r="146" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="33"/>
-      <c r="B146" s="33"/>
-      <c r="C146" s="33"/>
+      <c r="A146" s="35"/>
+      <c r="B146" s="35"/>
+      <c r="C146" s="35"/>
       <c r="D146" s="16" t="s">
         <v>163</v>
       </c>
@@ -3984,11 +3999,11 @@
       <c r="A149" s="7"/>
     </row>
     <row r="150" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="33" t="s">
+      <c r="A150" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="B150" s="33"/>
-      <c r="C150" s="33"/>
+      <c r="B150" s="35"/>
+      <c r="C150" s="35"/>
       <c r="D150" s="16" t="s">
         <v>168</v>
       </c>
@@ -4003,9 +4018,9 @@
       </c>
     </row>
     <row r="151" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="33"/>
-      <c r="B151" s="33"/>
-      <c r="C151" s="33"/>
+      <c r="A151" s="35"/>
+      <c r="B151" s="35"/>
+      <c r="C151" s="35"/>
       <c r="D151" s="16" t="s">
         <v>169</v>
       </c>
@@ -4023,11 +4038,11 @@
       <c r="A152" s="7"/>
     </row>
     <row r="153" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="33" t="s">
+      <c r="A153" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="B153" s="34"/>
-      <c r="C153" s="34"/>
+      <c r="B153" s="36"/>
+      <c r="C153" s="36"/>
       <c r="D153" s="18" t="s">
         <v>171</v>
       </c>
@@ -4040,9 +4055,9 @@
       <c r="G153" s="2"/>
     </row>
     <row r="154" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="33"/>
-      <c r="B154" s="34"/>
-      <c r="C154" s="34"/>
+      <c r="A154" s="35"/>
+      <c r="B154" s="36"/>
+      <c r="C154" s="36"/>
       <c r="D154" s="18" t="s">
         <v>172</v>
       </c>
@@ -4055,9 +4070,9 @@
       <c r="G154" s="2"/>
     </row>
     <row r="155" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="33"/>
-      <c r="B155" s="34"/>
-      <c r="C155" s="34"/>
+      <c r="A155" s="35"/>
+      <c r="B155" s="36"/>
+      <c r="C155" s="36"/>
       <c r="D155" s="18" t="s">
         <v>173</v>
       </c>
@@ -4073,11 +4088,11 @@
       <c r="A156" s="7"/>
     </row>
     <row r="157" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="33" t="s">
+      <c r="A157" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="B157" s="34"/>
-      <c r="C157" s="34"/>
+      <c r="B157" s="36"/>
+      <c r="C157" s="36"/>
       <c r="D157" s="18" t="s">
         <v>174</v>
       </c>
@@ -4092,9 +4107,9 @@
       </c>
     </row>
     <row r="158" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A158" s="33"/>
-      <c r="B158" s="34"/>
-      <c r="C158" s="34"/>
+      <c r="A158" s="35"/>
+      <c r="B158" s="36"/>
+      <c r="C158" s="36"/>
       <c r="D158" s="18" t="s">
         <v>175</v>
       </c>
@@ -4109,9 +4124,9 @@
       </c>
     </row>
     <row r="159" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A159" s="33"/>
-      <c r="B159" s="34"/>
-      <c r="C159" s="34"/>
+      <c r="A159" s="35"/>
+      <c r="B159" s="36"/>
+      <c r="C159" s="36"/>
       <c r="D159" s="18" t="s">
         <v>176</v>
       </c>
@@ -4129,11 +4144,11 @@
       <c r="A160" s="7"/>
     </row>
     <row r="161" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="33" t="s">
+      <c r="A161" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="B161" s="34"/>
-      <c r="C161" s="34"/>
+      <c r="B161" s="36"/>
+      <c r="C161" s="36"/>
       <c r="D161" s="18" t="s">
         <v>178</v>
       </c>
@@ -4146,9 +4161,9 @@
       <c r="G161" s="2"/>
     </row>
     <row r="162" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A162" s="33"/>
-      <c r="B162" s="34"/>
-      <c r="C162" s="34"/>
+      <c r="A162" s="35"/>
+      <c r="B162" s="36"/>
+      <c r="C162" s="36"/>
       <c r="D162" s="18" t="s">
         <v>179</v>
       </c>
@@ -4161,9 +4176,9 @@
       <c r="G162" s="2"/>
     </row>
     <row r="163" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="33"/>
-      <c r="B163" s="34"/>
-      <c r="C163" s="34"/>
+      <c r="A163" s="35"/>
+      <c r="B163" s="36"/>
+      <c r="C163" s="36"/>
       <c r="D163" s="18" t="s">
         <v>180</v>
       </c>
@@ -4201,11 +4216,11 @@
       <c r="A166" s="7"/>
     </row>
     <row r="167" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A167" s="33" t="s">
+      <c r="A167" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B167" s="34"/>
-      <c r="C167" s="34"/>
+      <c r="B167" s="36"/>
+      <c r="C167" s="36"/>
       <c r="D167" s="18" t="s">
         <v>182</v>
       </c>
@@ -4220,9 +4235,9 @@
       </c>
     </row>
     <row r="168" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="33"/>
-      <c r="B168" s="34"/>
-      <c r="C168" s="34"/>
+      <c r="A168" s="35"/>
+      <c r="B168" s="36"/>
+      <c r="C168" s="36"/>
       <c r="D168" s="18" t="s">
         <v>183</v>
       </c>
@@ -4240,11 +4255,11 @@
       <c r="A169" s="7"/>
     </row>
     <row r="170" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A170" s="33" t="s">
+      <c r="A170" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="B170" s="34"/>
-      <c r="C170" s="34"/>
+      <c r="B170" s="36"/>
+      <c r="C170" s="36"/>
       <c r="D170" s="18" t="s">
         <v>185</v>
       </c>
@@ -4259,9 +4274,9 @@
       </c>
     </row>
     <row r="171" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="33"/>
-      <c r="B171" s="34"/>
-      <c r="C171" s="34"/>
+      <c r="A171" s="35"/>
+      <c r="B171" s="36"/>
+      <c r="C171" s="36"/>
       <c r="D171" s="18" t="s">
         <v>186</v>
       </c>
@@ -4276,9 +4291,9 @@
       </c>
     </row>
     <row r="172" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="33"/>
-      <c r="B172" s="34"/>
-      <c r="C172" s="34"/>
+      <c r="A172" s="35"/>
+      <c r="B172" s="36"/>
+      <c r="C172" s="36"/>
       <c r="D172" s="18" t="s">
         <v>187</v>
       </c>
@@ -4291,9 +4306,9 @@
       <c r="G172" s="3"/>
     </row>
     <row r="173" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A173" s="33"/>
-      <c r="B173" s="34"/>
-      <c r="C173" s="34"/>
+      <c r="A173" s="35"/>
+      <c r="B173" s="36"/>
+      <c r="C173" s="36"/>
       <c r="D173" s="18" t="s">
         <v>188</v>
       </c>
@@ -4309,11 +4324,11 @@
       <c r="A174" s="7"/>
     </row>
     <row r="175" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A175" s="33" t="s">
+      <c r="A175" s="35" t="s">
         <v>189</v>
       </c>
-      <c r="B175" s="33"/>
-      <c r="C175" s="33"/>
+      <c r="B175" s="35"/>
+      <c r="C175" s="35"/>
       <c r="D175" s="18" t="s">
         <v>190</v>
       </c>
@@ -4326,9 +4341,9 @@
       <c r="G175" s="2"/>
     </row>
     <row r="176" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A176" s="33"/>
-      <c r="B176" s="33"/>
-      <c r="C176" s="33"/>
+      <c r="A176" s="35"/>
+      <c r="B176" s="35"/>
+      <c r="C176" s="35"/>
       <c r="D176" s="18" t="s">
         <v>191</v>
       </c>
@@ -4341,9 +4356,9 @@
       <c r="G176" s="4"/>
     </row>
     <row r="177" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="33"/>
-      <c r="B177" s="33"/>
-      <c r="C177" s="33"/>
+      <c r="A177" s="35"/>
+      <c r="B177" s="35"/>
+      <c r="C177" s="35"/>
       <c r="D177" s="18" t="s">
         <v>192</v>
       </c>
@@ -4427,6 +4442,62 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="72">
+    <mergeCell ref="A175:A177"/>
+    <mergeCell ref="B175:B177"/>
+    <mergeCell ref="C175:C177"/>
+    <mergeCell ref="A167:A168"/>
+    <mergeCell ref="B167:B168"/>
+    <mergeCell ref="C167:C168"/>
+    <mergeCell ref="A170:A173"/>
+    <mergeCell ref="B170:B173"/>
+    <mergeCell ref="C170:C173"/>
+    <mergeCell ref="A157:A159"/>
+    <mergeCell ref="B157:B159"/>
+    <mergeCell ref="C157:C159"/>
+    <mergeCell ref="A161:A163"/>
+    <mergeCell ref="B161:B163"/>
+    <mergeCell ref="C161:C163"/>
+    <mergeCell ref="C150:C151"/>
+    <mergeCell ref="B150:B151"/>
+    <mergeCell ref="A150:A151"/>
+    <mergeCell ref="A153:A155"/>
+    <mergeCell ref="B153:B155"/>
+    <mergeCell ref="C153:C155"/>
+    <mergeCell ref="B120:B123"/>
+    <mergeCell ref="C120:C123"/>
+    <mergeCell ref="C124:C140"/>
+    <mergeCell ref="B124:B140"/>
+    <mergeCell ref="A120:A140"/>
+    <mergeCell ref="C142:C146"/>
+    <mergeCell ref="B142:B146"/>
+    <mergeCell ref="A142:A146"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="A100:A115"/>
+    <mergeCell ref="B100:B115"/>
+    <mergeCell ref="C100:C115"/>
+    <mergeCell ref="A117:A118"/>
+    <mergeCell ref="B117:B118"/>
+    <mergeCell ref="C117:C118"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="C5:C19"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A5:A19"/>
+    <mergeCell ref="B5:B19"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="L1:L1048576"/>
     <mergeCell ref="C50:C51"/>
     <mergeCell ref="B41:B42"/>
@@ -4443,62 +4514,6 @@
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="B50:B51"/>
     <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="C5:C19"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="A5:A19"/>
-    <mergeCell ref="B5:B19"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C142:C146"/>
-    <mergeCell ref="B142:B146"/>
-    <mergeCell ref="A142:A146"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="A100:A115"/>
-    <mergeCell ref="B100:B115"/>
-    <mergeCell ref="C100:C115"/>
-    <mergeCell ref="A117:A118"/>
-    <mergeCell ref="B117:B118"/>
-    <mergeCell ref="C117:C118"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="B120:B123"/>
-    <mergeCell ref="C120:C123"/>
-    <mergeCell ref="C124:C140"/>
-    <mergeCell ref="B124:B140"/>
-    <mergeCell ref="A120:A140"/>
-    <mergeCell ref="C150:C151"/>
-    <mergeCell ref="B150:B151"/>
-    <mergeCell ref="A150:A151"/>
-    <mergeCell ref="A153:A155"/>
-    <mergeCell ref="B153:B155"/>
-    <mergeCell ref="C153:C155"/>
-    <mergeCell ref="A157:A159"/>
-    <mergeCell ref="B157:B159"/>
-    <mergeCell ref="C157:C159"/>
-    <mergeCell ref="A161:A163"/>
-    <mergeCell ref="B161:B163"/>
-    <mergeCell ref="C161:C163"/>
-    <mergeCell ref="A175:A177"/>
-    <mergeCell ref="B175:B177"/>
-    <mergeCell ref="C175:C177"/>
-    <mergeCell ref="A167:A168"/>
-    <mergeCell ref="B167:B168"/>
-    <mergeCell ref="C167:C168"/>
-    <mergeCell ref="A170:A173"/>
-    <mergeCell ref="B170:B173"/>
-    <mergeCell ref="C170:C173"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update collection, env and data file
</commit_message>
<xml_diff>
--- a/docs/Census_Wsc_Services.xlsx
+++ b/docs/Census_Wsc_Services.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian.catelli/Google Drive (christian.catelli@kineton.it)/Sky/Automation IT CI:CD WSC/Repository/PostmanCollection_AutomationAPI/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1737396B-A34E-5C4E-99AD-E8F73702C0ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F962697D-D9FA-A646-A8BD-1ACB36EC90A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8656BBE8-7E17-AC42-8AF4-F6E9122F8590}"/>
   </bookViews>
@@ -967,16 +967,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -990,6 +980,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1307,8 +1307,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D53" workbookViewId="0">
-      <selection activeCell="I75" sqref="I75"/>
+    <sheetView tabSelected="1" topLeftCell="AU200" workbookViewId="0">
+      <selection activeCell="M75" sqref="M75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1324,7 +1324,7 @@
     <col min="9" max="9" width="40" style="5" customWidth="1"/>
     <col min="10" max="10" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="35.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.83203125" style="33" customWidth="1"/>
+    <col min="12" max="12" width="7.83203125" style="41" customWidth="1"/>
     <col min="13" max="13" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="146" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
@@ -1365,7 +1365,7 @@
       <c r="K1" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="L1" s="41" t="s">
         <v>227</v>
       </c>
       <c r="M1" s="6" t="s">
@@ -1376,7 +1376,7 @@
       </c>
       <c r="O1" s="32"/>
     </row>
-    <row r="2" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="F2" s="10"/>
       <c r="G2" s="17"/>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="O2" s="9"/>
     </row>
-    <row r="3" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -1410,18 +1410,18 @@
       </c>
       <c r="O3" s="22"/>
     </row>
-    <row r="4" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="O4" s="22"/>
     </row>
     <row r="5" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
       <c r="D5" s="16" t="s">
         <v>5</v>
       </c>
@@ -1437,9 +1437,9 @@
       <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
       <c r="D6" s="16" t="s">
         <v>6</v>
       </c>
@@ -1455,9 +1455,9 @@
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="16" t="s">
         <v>7</v>
       </c>
@@ -1473,9 +1473,9 @@
       <c r="O7" s="22"/>
     </row>
     <row r="8" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
       <c r="D8" s="16" t="s">
         <v>8</v>
       </c>
@@ -1491,9 +1491,9 @@
       <c r="O8" s="22"/>
     </row>
     <row r="9" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
       <c r="D9" s="16" t="s">
         <v>9</v>
       </c>
@@ -1508,9 +1508,9 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="34"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
       <c r="D10" s="16" t="s">
         <v>10</v>
       </c>
@@ -1525,9 +1525,9 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="34"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
       <c r="D11" s="16" t="s">
         <v>11</v>
       </c>
@@ -1542,9 +1542,9 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="34"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
       <c r="D12" s="16" t="s">
         <v>12</v>
       </c>
@@ -1559,9 +1559,9 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="34"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
+      <c r="A13" s="40"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
       <c r="D13" s="16" t="s">
         <v>13</v>
       </c>
@@ -1576,9 +1576,9 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
       <c r="D14" s="16" t="s">
         <v>14</v>
       </c>
@@ -1593,9 +1593,9 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
       <c r="D15" s="16" t="s">
         <v>15</v>
       </c>
@@ -1610,9 +1610,9 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="34"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="16" t="s">
         <v>16</v>
       </c>
@@ -1627,9 +1627,9 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="34"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
       <c r="D17" s="16" t="s">
         <v>17</v>
       </c>
@@ -1644,9 +1644,9 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
       <c r="D18" s="16" t="s">
         <v>18</v>
       </c>
@@ -1661,9 +1661,9 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
       <c r="D19" s="16" t="s">
         <v>19</v>
       </c>
@@ -1677,17 +1677,17 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
     </row>
-    <row r="21" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="34" t="s">
+    <row r="21" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="16" t="s">
         <v>21</v>
       </c>
@@ -1699,10 +1699,10 @@
       </c>
       <c r="G21" s="12"/>
     </row>
-    <row r="22" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="34"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
+    <row r="22" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="40"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
       <c r="D22" s="16" t="s">
         <v>24</v>
       </c>
@@ -1714,10 +1714,10 @@
       </c>
       <c r="G22" s="12"/>
     </row>
-    <row r="23" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="34"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
+    <row r="23" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="40"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
       <c r="D23" s="16" t="s">
         <v>25</v>
       </c>
@@ -1729,10 +1729,10 @@
       </c>
       <c r="G23" s="12"/>
     </row>
-    <row r="24" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="34"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
+    <row r="24" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
       <c r="D24" s="16" t="s">
         <v>26</v>
       </c>
@@ -1744,10 +1744,10 @@
       </c>
       <c r="G24" s="12"/>
     </row>
-    <row r="25" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="34"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
+    <row r="25" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="40"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
       <c r="D25" s="16" t="s">
         <v>27</v>
       </c>
@@ -1759,17 +1759,17 @@
       </c>
       <c r="G25" s="12"/>
     </row>
-    <row r="26" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
       <c r="D27" s="16" t="s">
         <v>30</v>
       </c>
@@ -1792,10 +1792,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="34"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
+    <row r="28" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="40"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
       <c r="D28" s="16" t="s">
         <v>31</v>
       </c>
@@ -1807,17 +1807,17 @@
       </c>
       <c r="G28" s="13"/>
     </row>
-    <row r="29" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
     </row>
     <row r="30" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
       <c r="D30" s="16" t="s">
         <v>34</v>
       </c>
@@ -1841,9 +1841,9 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="34"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
       <c r="D31" s="16" t="s">
         <v>35</v>
       </c>
@@ -1869,10 +1869,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="34"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
+    <row r="32" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="40"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
       <c r="D32" s="16" t="s">
         <v>36</v>
       </c>
@@ -1884,10 +1884,10 @@
       </c>
       <c r="G32" s="14"/>
     </row>
-    <row r="33" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="34"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
+    <row r="33" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="40"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
       <c r="D33" s="16" t="s">
         <v>37</v>
       </c>
@@ -1899,17 +1899,17 @@
       </c>
       <c r="G33" s="14"/>
     </row>
-    <row r="34" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
     </row>
     <row r="35" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
       <c r="D35" s="16" t="s">
         <v>40</v>
       </c>
@@ -1922,9 +1922,9 @@
       <c r="G35" s="13"/>
     </row>
     <row r="36" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="34"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
+      <c r="A36" s="40"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
       <c r="D36" s="16" t="s">
         <v>41</v>
       </c>
@@ -1945,9 +1945,9 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="34"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
       <c r="D37" s="16" t="s">
         <v>42</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
@@ -1995,17 +1995,17 @@
         <v>214</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
     </row>
     <row r="41" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="34" t="s">
+      <c r="A41" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="34"/>
-      <c r="C41" s="34"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="40"/>
       <c r="D41" s="16" t="s">
         <v>46</v>
       </c>
@@ -2018,9 +2018,9 @@
       <c r="G41" s="12"/>
     </row>
     <row r="42" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="34"/>
-      <c r="B42" s="34"/>
-      <c r="C42" s="34"/>
+      <c r="A42" s="40"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="40"/>
       <c r="D42" s="16" t="s">
         <v>47</v>
       </c>
@@ -2032,19 +2032,19 @@
       </c>
       <c r="G42" s="12"/>
     </row>
-    <row r="43" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
     </row>
-    <row r="44" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="34" t="s">
+    <row r="44" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="34" t="s">
+      <c r="B44" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="34"/>
+      <c r="C44" s="40"/>
       <c r="D44" s="16" t="s">
         <v>51</v>
       </c>
@@ -2056,10 +2056,10 @@
       </c>
       <c r="G44" s="12"/>
     </row>
-    <row r="45" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="34"/>
-      <c r="B45" s="34"/>
-      <c r="C45" s="34"/>
+    <row r="45" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
       <c r="D45" s="16" t="s">
         <v>52</v>
       </c>
@@ -2072,9 +2072,9 @@
       <c r="G45" s="12"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="34"/>
-      <c r="B46" s="34"/>
-      <c r="C46" s="34"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
       <c r="D46" s="16" t="s">
         <v>53</v>
       </c>
@@ -2098,9 +2098,9 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="34"/>
-      <c r="B47" s="34"/>
-      <c r="C47" s="34"/>
+      <c r="A47" s="40"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="40"/>
       <c r="D47" s="16" t="s">
         <v>54</v>
       </c>
@@ -2126,12 +2126,12 @@
         <v>214</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="34"/>
-      <c r="B48" s="34" t="s">
+    <row r="48" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="40"/>
+      <c r="B48" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="C48" s="34"/>
+      <c r="C48" s="40"/>
       <c r="D48" s="16" t="s">
         <v>56</v>
       </c>
@@ -2140,10 +2140,10 @@
       </c>
       <c r="G48" s="12"/>
     </row>
-    <row r="49" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="34"/>
-      <c r="B49" s="34"/>
-      <c r="C49" s="34"/>
+    <row r="49" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="40"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="40"/>
       <c r="D49" s="16" t="s">
         <v>57</v>
       </c>
@@ -2152,12 +2152,12 @@
       </c>
       <c r="G49" s="12"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="34"/>
-      <c r="B50" s="34" t="s">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="40"/>
+      <c r="B50" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="C50" s="34"/>
+      <c r="C50" s="40"/>
       <c r="D50" s="16" t="s">
         <v>59</v>
       </c>
@@ -2171,10 +2171,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" s="34"/>
-      <c r="B51" s="34"/>
-      <c r="C51" s="34"/>
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="40"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="40"/>
       <c r="D51" s="16" t="s">
         <v>60</v>
       </c>
@@ -2189,11 +2189,11 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" s="34"/>
-      <c r="B52" s="34" t="s">
+      <c r="A52" s="40"/>
+      <c r="B52" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C52" s="34"/>
+      <c r="C52" s="40"/>
       <c r="D52" s="16" t="s">
         <v>62</v>
       </c>
@@ -2217,9 +2217,9 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" s="34"/>
-      <c r="B53" s="34"/>
-      <c r="C53" s="34"/>
+      <c r="A53" s="40"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="40"/>
       <c r="D53" s="16" t="s">
         <v>63</v>
       </c>
@@ -2245,8 +2245,8 @@
         <v>212</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="34"/>
+    <row r="54" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="40"/>
       <c r="B54" s="7" t="s">
         <v>64</v>
       </c>
@@ -2260,8 +2260,8 @@
         <v>202</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="34"/>
+    <row r="55" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="40"/>
       <c r="B55" s="7" t="s">
         <v>66</v>
       </c>
@@ -2275,12 +2275,12 @@
         <v>200</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A56" s="34"/>
-      <c r="B56" s="34" t="s">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="40"/>
+      <c r="B56" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="C56" s="34" t="s">
+      <c r="C56" s="40" t="s">
         <v>68</v>
       </c>
       <c r="D56" s="16" t="s">
@@ -2296,10 +2296,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A57" s="34"/>
-      <c r="B57" s="34"/>
-      <c r="C57" s="34"/>
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="40"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="40"/>
       <c r="D57" s="16" t="s">
         <v>70</v>
       </c>
@@ -2313,10 +2313,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A58" s="34"/>
-      <c r="B58" s="34"/>
-      <c r="C58" s="34"/>
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="40"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="40"/>
       <c r="D58" s="16" t="s">
         <v>73</v>
       </c>
@@ -2330,10 +2330,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A59" s="34"/>
-      <c r="B59" s="34"/>
-      <c r="C59" s="34"/>
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="40"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="40"/>
       <c r="D59" s="16" t="s">
         <v>74</v>
       </c>
@@ -2347,10 +2347,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A60" s="34"/>
-      <c r="B60" s="34"/>
-      <c r="C60" s="34"/>
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="40"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="40"/>
       <c r="D60" s="16" t="s">
         <v>75</v>
       </c>
@@ -2365,11 +2365,11 @@
       </c>
     </row>
     <row r="61" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="34"/>
-      <c r="B61" s="34" t="s">
+      <c r="A61" s="40"/>
+      <c r="B61" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="C61" s="34"/>
+      <c r="C61" s="40"/>
       <c r="D61" s="16" t="s">
         <v>77</v>
       </c>
@@ -2382,9 +2382,9 @@
       <c r="G61" s="12"/>
     </row>
     <row r="62" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="34"/>
-      <c r="B62" s="34"/>
-      <c r="C62" s="34"/>
+      <c r="A62" s="40"/>
+      <c r="B62" s="40"/>
+      <c r="C62" s="40"/>
       <c r="D62" s="16" t="s">
         <v>78</v>
       </c>
@@ -2397,9 +2397,9 @@
       <c r="G62" s="12"/>
     </row>
     <row r="63" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="34"/>
-      <c r="B63" s="34"/>
-      <c r="C63" s="34"/>
+      <c r="A63" s="40"/>
+      <c r="B63" s="40"/>
+      <c r="C63" s="40"/>
       <c r="D63" s="16" t="s">
         <v>79</v>
       </c>
@@ -2411,12 +2411,12 @@
       </c>
       <c r="G63" s="12"/>
     </row>
-    <row r="64" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="34"/>
-      <c r="B64" s="34" t="s">
+    <row r="64" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="40"/>
+      <c r="B64" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="C64" s="34"/>
+      <c r="C64" s="40"/>
       <c r="D64" s="16" t="s">
         <v>81</v>
       </c>
@@ -2428,10 +2428,10 @@
       </c>
       <c r="G64" s="12"/>
     </row>
-    <row r="65" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="34"/>
-      <c r="B65" s="34"/>
-      <c r="C65" s="34"/>
+    <row r="65" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="40"/>
+      <c r="B65" s="40"/>
+      <c r="C65" s="40"/>
       <c r="D65" s="16" t="s">
         <v>82</v>
       </c>
@@ -2443,10 +2443,10 @@
       </c>
       <c r="G65" s="12"/>
     </row>
-    <row r="66" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="34"/>
-      <c r="B66" s="34"/>
-      <c r="C66" s="34"/>
+    <row r="66" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="40"/>
+      <c r="B66" s="40"/>
+      <c r="C66" s="40"/>
       <c r="D66" s="16" t="s">
         <v>83</v>
       </c>
@@ -2459,9 +2459,9 @@
       <c r="G66" s="12"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A67" s="34"/>
-      <c r="B67" s="34"/>
-      <c r="C67" s="34"/>
+      <c r="A67" s="40"/>
+      <c r="B67" s="40"/>
+      <c r="C67" s="40"/>
       <c r="D67" s="16" t="s">
         <v>84</v>
       </c>
@@ -2485,9 +2485,9 @@
       </c>
     </row>
     <row r="68" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="34"/>
-      <c r="B68" s="34"/>
-      <c r="C68" s="34"/>
+      <c r="A68" s="40"/>
+      <c r="B68" s="40"/>
+      <c r="C68" s="40"/>
       <c r="D68" s="16" t="s">
         <v>85</v>
       </c>
@@ -2508,9 +2508,9 @@
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69" s="34"/>
-      <c r="B69" s="34"/>
-      <c r="C69" s="34"/>
+      <c r="A69" s="40"/>
+      <c r="B69" s="40"/>
+      <c r="C69" s="40"/>
       <c r="D69" s="16" t="s">
         <v>86</v>
       </c>
@@ -2534,9 +2534,9 @@
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A70" s="34"/>
-      <c r="B70" s="34"/>
-      <c r="C70" s="34"/>
+      <c r="A70" s="40"/>
+      <c r="B70" s="40"/>
+      <c r="C70" s="40"/>
       <c r="D70" s="16" t="s">
         <v>87</v>
       </c>
@@ -2560,9 +2560,9 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A71" s="34"/>
-      <c r="B71" s="34"/>
-      <c r="C71" s="34"/>
+      <c r="A71" s="40"/>
+      <c r="B71" s="40"/>
+      <c r="C71" s="40"/>
       <c r="D71" s="16" t="s">
         <v>88</v>
       </c>
@@ -2586,9 +2586,9 @@
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A72" s="34"/>
-      <c r="B72" s="34"/>
-      <c r="C72" s="34"/>
+      <c r="A72" s="40"/>
+      <c r="B72" s="40"/>
+      <c r="C72" s="40"/>
       <c r="D72" s="16" t="s">
         <v>89</v>
       </c>
@@ -2612,9 +2612,9 @@
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A73" s="34"/>
-      <c r="B73" s="34"/>
-      <c r="C73" s="34"/>
+      <c r="A73" s="40"/>
+      <c r="B73" s="40"/>
+      <c r="C73" s="40"/>
       <c r="D73" s="16" t="s">
         <v>90</v>
       </c>
@@ -2641,9 +2641,9 @@
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A74" s="34"/>
-      <c r="B74" s="34"/>
-      <c r="C74" s="34"/>
+      <c r="A74" s="40"/>
+      <c r="B74" s="40"/>
+      <c r="C74" s="40"/>
       <c r="D74" s="16" t="s">
         <v>91</v>
       </c>
@@ -2670,34 +2670,34 @@
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A75" s="34"/>
-      <c r="B75" s="34"/>
-      <c r="C75" s="34"/>
-      <c r="D75" s="37" t="s">
+      <c r="A75" s="40"/>
+      <c r="B75" s="40"/>
+      <c r="C75" s="40"/>
+      <c r="D75" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="E75" s="38" t="s">
-        <v>222</v>
-      </c>
-      <c r="F75" s="39" t="s">
+      <c r="E75" s="34" t="s">
+        <v>222</v>
+      </c>
+      <c r="F75" s="35" t="s">
         <v>23</v>
       </c>
       <c r="G75" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="H75" s="38" t="s">
+      <c r="H75" s="34" t="s">
         <v>207</v>
       </c>
-      <c r="I75" s="40" t="s">
+      <c r="I75" s="36" t="s">
         <v>232</v>
       </c>
-      <c r="J75" s="41"/>
-      <c r="K75" s="40"/>
+      <c r="J75" s="37"/>
+      <c r="K75" s="36"/>
     </row>
     <row r="76" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="34"/>
-      <c r="B76" s="34"/>
-      <c r="C76" s="34"/>
+      <c r="A76" s="40"/>
+      <c r="B76" s="40"/>
+      <c r="C76" s="40"/>
       <c r="D76" s="16" t="s">
         <v>93</v>
       </c>
@@ -2721,9 +2721,9 @@
       </c>
     </row>
     <row r="77" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="34"/>
-      <c r="B77" s="34"/>
-      <c r="C77" s="34"/>
+      <c r="A77" s="40"/>
+      <c r="B77" s="40"/>
+      <c r="C77" s="40"/>
       <c r="D77" s="16" t="s">
         <v>94</v>
       </c>
@@ -2744,9 +2744,9 @@
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A78" s="34"/>
-      <c r="B78" s="34"/>
-      <c r="C78" s="34"/>
+      <c r="A78" s="40"/>
+      <c r="B78" s="40"/>
+      <c r="C78" s="40"/>
       <c r="D78" s="16" t="s">
         <v>95</v>
       </c>
@@ -2770,9 +2770,9 @@
       </c>
     </row>
     <row r="79" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="34"/>
-      <c r="B79" s="34"/>
-      <c r="C79" s="34"/>
+      <c r="A79" s="40"/>
+      <c r="B79" s="40"/>
+      <c r="C79" s="40"/>
       <c r="D79" s="24" t="s">
         <v>96</v>
       </c>
@@ -2796,9 +2796,9 @@
       </c>
     </row>
     <row r="80" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="34"/>
-      <c r="B80" s="34"/>
-      <c r="C80" s="34"/>
+      <c r="A80" s="40"/>
+      <c r="B80" s="40"/>
+      <c r="C80" s="40"/>
       <c r="D80" s="24" t="s">
         <v>97</v>
       </c>
@@ -2819,9 +2819,9 @@
       </c>
     </row>
     <row r="81" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="34"/>
-      <c r="B81" s="34"/>
-      <c r="C81" s="34"/>
+      <c r="A81" s="40"/>
+      <c r="B81" s="40"/>
+      <c r="C81" s="40"/>
       <c r="D81" s="16" t="s">
         <v>98</v>
       </c>
@@ -2834,9 +2834,9 @@
       <c r="G81" s="13"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A82" s="34"/>
-      <c r="B82" s="34"/>
-      <c r="C82" s="34"/>
+      <c r="A82" s="40"/>
+      <c r="B82" s="40"/>
+      <c r="C82" s="40"/>
       <c r="D82" s="24" t="s">
         <v>99</v>
       </c>
@@ -2863,9 +2863,9 @@
       </c>
     </row>
     <row r="83" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="34"/>
-      <c r="B83" s="34"/>
-      <c r="C83" s="34"/>
+      <c r="A83" s="40"/>
+      <c r="B83" s="40"/>
+      <c r="C83" s="40"/>
       <c r="D83" s="24" t="s">
         <v>100</v>
       </c>
@@ -2892,9 +2892,9 @@
       </c>
     </row>
     <row r="84" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="34"/>
-      <c r="B84" s="34"/>
-      <c r="C84" s="34"/>
+      <c r="A84" s="40"/>
+      <c r="B84" s="40"/>
+      <c r="C84" s="40"/>
       <c r="D84" s="24" t="s">
         <v>101</v>
       </c>
@@ -2921,9 +2921,9 @@
       </c>
     </row>
     <row r="85" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="34"/>
-      <c r="B85" s="34"/>
-      <c r="C85" s="34"/>
+      <c r="A85" s="40"/>
+      <c r="B85" s="40"/>
+      <c r="C85" s="40"/>
       <c r="D85" s="24" t="s">
         <v>102</v>
       </c>
@@ -2950,9 +2950,9 @@
       </c>
     </row>
     <row r="86" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="34"/>
-      <c r="B86" s="34"/>
-      <c r="C86" s="34"/>
+      <c r="A86" s="40"/>
+      <c r="B86" s="40"/>
+      <c r="C86" s="40"/>
       <c r="D86" s="24" t="s">
         <v>103</v>
       </c>
@@ -2978,10 +2978,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="34"/>
-      <c r="B87" s="34"/>
-      <c r="C87" s="34"/>
+    <row r="87" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="40"/>
+      <c r="B87" s="40"/>
+      <c r="C87" s="40"/>
       <c r="D87" s="16" t="s">
         <v>104</v>
       </c>
@@ -2993,10 +2993,10 @@
       </c>
       <c r="G87" s="13"/>
     </row>
-    <row r="88" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="34"/>
-      <c r="B88" s="34"/>
-      <c r="C88" s="34"/>
+    <row r="88" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="40"/>
+      <c r="B88" s="40"/>
+      <c r="C88" s="40"/>
       <c r="D88" s="16" t="s">
         <v>105</v>
       </c>
@@ -3008,10 +3008,10 @@
       </c>
       <c r="G88" s="13"/>
     </row>
-    <row r="89" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="34"/>
-      <c r="B89" s="34"/>
-      <c r="C89" s="34"/>
+    <row r="89" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="40"/>
+      <c r="B89" s="40"/>
+      <c r="C89" s="40"/>
       <c r="D89" s="16" t="s">
         <v>106</v>
       </c>
@@ -3023,10 +3023,10 @@
       </c>
       <c r="G89" s="13"/>
     </row>
-    <row r="90" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="34"/>
-      <c r="B90" s="34"/>
-      <c r="C90" s="34"/>
+    <row r="90" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="40"/>
+      <c r="B90" s="40"/>
+      <c r="C90" s="40"/>
       <c r="D90" s="16" t="s">
         <v>107</v>
       </c>
@@ -3038,10 +3038,10 @@
       </c>
       <c r="G90" s="13"/>
     </row>
-    <row r="91" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="34"/>
-      <c r="B91" s="34"/>
-      <c r="C91" s="34"/>
+    <row r="91" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="40"/>
+      <c r="B91" s="40"/>
+      <c r="C91" s="40"/>
       <c r="D91" s="16" t="s">
         <v>108</v>
       </c>
@@ -3053,10 +3053,10 @@
       </c>
       <c r="G91" s="13"/>
     </row>
-    <row r="92" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="34"/>
-      <c r="B92" s="34"/>
-      <c r="C92" s="34"/>
+    <row r="92" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="40"/>
+      <c r="B92" s="40"/>
+      <c r="C92" s="40"/>
       <c r="D92" s="16" t="s">
         <v>109</v>
       </c>
@@ -3068,10 +3068,10 @@
       </c>
       <c r="G92" s="13"/>
     </row>
-    <row r="93" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="34"/>
-      <c r="B93" s="34"/>
-      <c r="C93" s="34"/>
+    <row r="93" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="40"/>
+      <c r="B93" s="40"/>
+      <c r="C93" s="40"/>
       <c r="D93" s="16" t="s">
         <v>110</v>
       </c>
@@ -3084,9 +3084,9 @@
       <c r="G93" s="13"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A94" s="34"/>
-      <c r="B94" s="34"/>
-      <c r="C94" s="34"/>
+      <c r="A94" s="40"/>
+      <c r="B94" s="40"/>
+      <c r="C94" s="40"/>
       <c r="D94" s="24" t="s">
         <v>111</v>
       </c>
@@ -3110,9 +3110,9 @@
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A95" s="34"/>
-      <c r="B95" s="34"/>
-      <c r="C95" s="34"/>
+      <c r="A95" s="40"/>
+      <c r="B95" s="40"/>
+      <c r="C95" s="40"/>
       <c r="D95" s="24" t="s">
         <v>112</v>
       </c>
@@ -3135,10 +3135,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="34"/>
-      <c r="B96" s="34"/>
-      <c r="C96" s="34"/>
+    <row r="96" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="40"/>
+      <c r="B96" s="40"/>
+      <c r="C96" s="40"/>
       <c r="D96" s="16" t="s">
         <v>113</v>
       </c>
@@ -3150,10 +3150,10 @@
       </c>
       <c r="G96" s="12"/>
     </row>
-    <row r="97" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="34"/>
-      <c r="B97" s="34"/>
-      <c r="C97" s="34"/>
+    <row r="97" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="40"/>
+      <c r="B97" s="40"/>
+      <c r="C97" s="40"/>
       <c r="D97" s="16" t="s">
         <v>114</v>
       </c>
@@ -3166,9 +3166,9 @@
       <c r="G97" s="12"/>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A98" s="34"/>
-      <c r="B98" s="34"/>
-      <c r="C98" s="34"/>
+      <c r="A98" s="40"/>
+      <c r="B98" s="40"/>
+      <c r="C98" s="40"/>
       <c r="D98" s="24" t="s">
         <v>115</v>
       </c>
@@ -3191,17 +3191,17 @@
         <v>214</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="7"/>
       <c r="F99" s="11"/>
       <c r="G99" s="11"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A100" s="35" t="s">
+    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="B100" s="35"/>
-      <c r="C100" s="35"/>
+      <c r="B100" s="38"/>
+      <c r="C100" s="38"/>
       <c r="D100" s="16" t="s">
         <v>117</v>
       </c>
@@ -3215,10 +3215,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A101" s="35"/>
-      <c r="B101" s="35"/>
-      <c r="C101" s="35"/>
+    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="38"/>
+      <c r="B101" s="38"/>
+      <c r="C101" s="38"/>
       <c r="D101" s="16" t="s">
         <v>118</v>
       </c>
@@ -3232,10 +3232,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A102" s="35"/>
-      <c r="B102" s="35"/>
-      <c r="C102" s="35"/>
+    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="38"/>
+      <c r="B102" s="38"/>
+      <c r="C102" s="38"/>
       <c r="D102" s="16" t="s">
         <v>119</v>
       </c>
@@ -3249,10 +3249,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A103" s="35"/>
-      <c r="B103" s="35"/>
-      <c r="C103" s="35"/>
+    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="38"/>
+      <c r="B103" s="38"/>
+      <c r="C103" s="38"/>
       <c r="D103" s="16" t="s">
         <v>120</v>
       </c>
@@ -3266,10 +3266,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="34"/>
-      <c r="B104" s="35"/>
-      <c r="C104" s="35"/>
+    <row r="104" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="40"/>
+      <c r="B104" s="38"/>
+      <c r="C104" s="38"/>
       <c r="D104" s="16" t="s">
         <v>121</v>
       </c>
@@ -3281,10 +3281,10 @@
       </c>
       <c r="G104" s="12"/>
     </row>
-    <row r="105" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="34"/>
-      <c r="B105" s="35"/>
-      <c r="C105" s="35"/>
+    <row r="105" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="40"/>
+      <c r="B105" s="38"/>
+      <c r="C105" s="38"/>
       <c r="D105" s="16" t="s">
         <v>122</v>
       </c>
@@ -3296,10 +3296,10 @@
       </c>
       <c r="G105" s="12"/>
     </row>
-    <row r="106" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="34"/>
-      <c r="B106" s="35"/>
-      <c r="C106" s="35"/>
+    <row r="106" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="40"/>
+      <c r="B106" s="38"/>
+      <c r="C106" s="38"/>
       <c r="D106" s="16" t="s">
         <v>123</v>
       </c>
@@ -3311,10 +3311,10 @@
       </c>
       <c r="G106" s="12"/>
     </row>
-    <row r="107" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="34"/>
-      <c r="B107" s="35"/>
-      <c r="C107" s="35"/>
+    <row r="107" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="40"/>
+      <c r="B107" s="38"/>
+      <c r="C107" s="38"/>
       <c r="D107" s="16" t="s">
         <v>124</v>
       </c>
@@ -3326,10 +3326,10 @@
       </c>
       <c r="G107" s="12"/>
     </row>
-    <row r="108" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="34"/>
-      <c r="B108" s="35"/>
-      <c r="C108" s="35"/>
+    <row r="108" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="40"/>
+      <c r="B108" s="38"/>
+      <c r="C108" s="38"/>
       <c r="D108" s="16" t="s">
         <v>125</v>
       </c>
@@ -3341,10 +3341,10 @@
       </c>
       <c r="G108" s="12"/>
     </row>
-    <row r="109" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="34"/>
-      <c r="B109" s="35"/>
-      <c r="C109" s="35"/>
+    <row r="109" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="40"/>
+      <c r="B109" s="38"/>
+      <c r="C109" s="38"/>
       <c r="D109" s="16" t="s">
         <v>126</v>
       </c>
@@ -3356,10 +3356,10 @@
       </c>
       <c r="G109" s="12"/>
     </row>
-    <row r="110" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="34"/>
-      <c r="B110" s="35"/>
-      <c r="C110" s="35"/>
+    <row r="110" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="40"/>
+      <c r="B110" s="38"/>
+      <c r="C110" s="38"/>
       <c r="D110" s="16" t="s">
         <v>127</v>
       </c>
@@ -3371,10 +3371,10 @@
       </c>
       <c r="G110" s="12"/>
     </row>
-    <row r="111" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="34"/>
-      <c r="B111" s="35"/>
-      <c r="C111" s="35"/>
+    <row r="111" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="40"/>
+      <c r="B111" s="38"/>
+      <c r="C111" s="38"/>
       <c r="D111" s="16" t="s">
         <v>128</v>
       </c>
@@ -3386,10 +3386,10 @@
       </c>
       <c r="G111" s="12"/>
     </row>
-    <row r="112" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="34"/>
-      <c r="B112" s="35"/>
-      <c r="C112" s="35"/>
+    <row r="112" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="40"/>
+      <c r="B112" s="38"/>
+      <c r="C112" s="38"/>
       <c r="D112" s="16" t="s">
         <v>129</v>
       </c>
@@ -3401,10 +3401,10 @@
       </c>
       <c r="G112" s="13"/>
     </row>
-    <row r="113" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="34"/>
-      <c r="B113" s="35"/>
-      <c r="C113" s="35"/>
+    <row r="113" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="40"/>
+      <c r="B113" s="38"/>
+      <c r="C113" s="38"/>
       <c r="D113" s="16" t="s">
         <v>130</v>
       </c>
@@ -3416,10 +3416,10 @@
       </c>
       <c r="G113" s="13"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A114" s="35"/>
-      <c r="B114" s="35"/>
-      <c r="C114" s="35"/>
+    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="38"/>
+      <c r="B114" s="38"/>
+      <c r="C114" s="38"/>
       <c r="D114" s="16" t="s">
         <v>131</v>
       </c>
@@ -3433,10 +3433,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A115" s="35"/>
-      <c r="B115" s="35"/>
-      <c r="C115" s="35"/>
+    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="38"/>
+      <c r="B115" s="38"/>
+      <c r="C115" s="38"/>
       <c r="D115" s="16" t="s">
         <v>132</v>
       </c>
@@ -3450,15 +3450,15 @@
         <v>202</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="7"/>
     </row>
     <row r="117" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="35" t="s">
+      <c r="A117" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="B117" s="35"/>
-      <c r="C117" s="35"/>
+      <c r="B117" s="38"/>
+      <c r="C117" s="38"/>
       <c r="D117" s="16" t="s">
         <v>134</v>
       </c>
@@ -3471,9 +3471,9 @@
       <c r="G117" s="12"/>
     </row>
     <row r="118" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="35"/>
-      <c r="B118" s="35"/>
-      <c r="C118" s="35"/>
+      <c r="A118" s="38"/>
+      <c r="B118" s="38"/>
+      <c r="C118" s="38"/>
       <c r="D118" s="16" t="s">
         <v>135</v>
       </c>
@@ -3485,17 +3485,17 @@
       </c>
       <c r="G118" s="12"/>
     </row>
-    <row r="119" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="7"/>
     </row>
     <row r="120" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="34" t="s">
+      <c r="A120" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="B120" s="35" t="s">
+      <c r="B120" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="C120" s="35"/>
+      <c r="C120" s="38"/>
       <c r="D120" s="16" t="s">
         <v>138</v>
       </c>
@@ -3510,9 +3510,9 @@
       </c>
     </row>
     <row r="121" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="34"/>
-      <c r="B121" s="35"/>
-      <c r="C121" s="35"/>
+      <c r="A121" s="40"/>
+      <c r="B121" s="38"/>
+      <c r="C121" s="38"/>
       <c r="D121" s="16" t="s">
         <v>139</v>
       </c>
@@ -3527,9 +3527,9 @@
       </c>
     </row>
     <row r="122" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="34"/>
-      <c r="B122" s="35"/>
-      <c r="C122" s="35"/>
+      <c r="A122" s="40"/>
+      <c r="B122" s="38"/>
+      <c r="C122" s="38"/>
       <c r="D122" s="16" t="s">
         <v>140</v>
       </c>
@@ -3544,9 +3544,9 @@
       </c>
     </row>
     <row r="123" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="34"/>
-      <c r="B123" s="35"/>
-      <c r="C123" s="35"/>
+      <c r="A123" s="40"/>
+      <c r="B123" s="38"/>
+      <c r="C123" s="38"/>
       <c r="D123" s="16" t="s">
         <v>141</v>
       </c>
@@ -3561,9 +3561,9 @@
       </c>
     </row>
     <row r="124" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="34"/>
-      <c r="B124" s="35"/>
-      <c r="C124" s="35"/>
+      <c r="A124" s="40"/>
+      <c r="B124" s="38"/>
+      <c r="C124" s="38"/>
       <c r="D124" s="24" t="s">
         <v>142</v>
       </c>
@@ -3587,9 +3587,9 @@
       </c>
     </row>
     <row r="125" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="34"/>
-      <c r="B125" s="35"/>
-      <c r="C125" s="35"/>
+      <c r="A125" s="40"/>
+      <c r="B125" s="38"/>
+      <c r="C125" s="38"/>
       <c r="D125" s="24" t="s">
         <v>143</v>
       </c>
@@ -3607,9 +3607,9 @@
       </c>
     </row>
     <row r="126" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="34"/>
-      <c r="B126" s="35"/>
-      <c r="C126" s="35"/>
+      <c r="A126" s="40"/>
+      <c r="B126" s="38"/>
+      <c r="C126" s="38"/>
       <c r="D126" s="24" t="s">
         <v>144</v>
       </c>
@@ -3627,9 +3627,9 @@
       </c>
     </row>
     <row r="127" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="34"/>
-      <c r="B127" s="35"/>
-      <c r="C127" s="35"/>
+      <c r="A127" s="40"/>
+      <c r="B127" s="38"/>
+      <c r="C127" s="38"/>
       <c r="D127" s="24" t="s">
         <v>145</v>
       </c>
@@ -3647,9 +3647,9 @@
       </c>
     </row>
     <row r="128" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="34"/>
-      <c r="B128" s="35"/>
-      <c r="C128" s="35"/>
+      <c r="A128" s="40"/>
+      <c r="B128" s="38"/>
+      <c r="C128" s="38"/>
       <c r="D128" s="24" t="s">
         <v>146</v>
       </c>
@@ -3667,9 +3667,9 @@
       </c>
     </row>
     <row r="129" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="34"/>
-      <c r="B129" s="35"/>
-      <c r="C129" s="35"/>
+      <c r="A129" s="40"/>
+      <c r="B129" s="38"/>
+      <c r="C129" s="38"/>
       <c r="D129" s="24" t="s">
         <v>147</v>
       </c>
@@ -3687,9 +3687,9 @@
       </c>
     </row>
     <row r="130" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="34"/>
-      <c r="B130" s="35"/>
-      <c r="C130" s="35"/>
+      <c r="A130" s="40"/>
+      <c r="B130" s="38"/>
+      <c r="C130" s="38"/>
       <c r="D130" s="24" t="s">
         <v>148</v>
       </c>
@@ -3707,9 +3707,9 @@
       </c>
     </row>
     <row r="131" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="34"/>
-      <c r="B131" s="35"/>
-      <c r="C131" s="35"/>
+      <c r="A131" s="40"/>
+      <c r="B131" s="38"/>
+      <c r="C131" s="38"/>
       <c r="D131" s="24" t="s">
         <v>149</v>
       </c>
@@ -3727,9 +3727,9 @@
       </c>
     </row>
     <row r="132" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="34"/>
-      <c r="B132" s="35"/>
-      <c r="C132" s="35"/>
+      <c r="A132" s="40"/>
+      <c r="B132" s="38"/>
+      <c r="C132" s="38"/>
       <c r="D132" s="24" t="s">
         <v>150</v>
       </c>
@@ -3747,9 +3747,9 @@
       </c>
     </row>
     <row r="133" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="34"/>
-      <c r="B133" s="35"/>
-      <c r="C133" s="35"/>
+      <c r="A133" s="40"/>
+      <c r="B133" s="38"/>
+      <c r="C133" s="38"/>
       <c r="D133" s="24" t="s">
         <v>151</v>
       </c>
@@ -3767,9 +3767,9 @@
       </c>
     </row>
     <row r="134" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="34"/>
-      <c r="B134" s="35"/>
-      <c r="C134" s="35"/>
+      <c r="A134" s="40"/>
+      <c r="B134" s="38"/>
+      <c r="C134" s="38"/>
       <c r="D134" s="24" t="s">
         <v>152</v>
       </c>
@@ -3787,9 +3787,9 @@
       </c>
     </row>
     <row r="135" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="34"/>
-      <c r="B135" s="35"/>
-      <c r="C135" s="35"/>
+      <c r="A135" s="40"/>
+      <c r="B135" s="38"/>
+      <c r="C135" s="38"/>
       <c r="D135" s="24" t="s">
         <v>153</v>
       </c>
@@ -3807,9 +3807,9 @@
       </c>
     </row>
     <row r="136" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="34"/>
-      <c r="B136" s="35"/>
-      <c r="C136" s="35"/>
+      <c r="A136" s="40"/>
+      <c r="B136" s="38"/>
+      <c r="C136" s="38"/>
       <c r="D136" s="24" t="s">
         <v>154</v>
       </c>
@@ -3827,9 +3827,9 @@
       </c>
     </row>
     <row r="137" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="34"/>
-      <c r="B137" s="35"/>
-      <c r="C137" s="35"/>
+      <c r="A137" s="40"/>
+      <c r="B137" s="38"/>
+      <c r="C137" s="38"/>
       <c r="D137" s="24" t="s">
         <v>155</v>
       </c>
@@ -3847,9 +3847,9 @@
       </c>
     </row>
     <row r="138" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="34"/>
-      <c r="B138" s="35"/>
-      <c r="C138" s="35"/>
+      <c r="A138" s="40"/>
+      <c r="B138" s="38"/>
+      <c r="C138" s="38"/>
       <c r="D138" s="24" t="s">
         <v>156</v>
       </c>
@@ -3867,9 +3867,9 @@
       </c>
     </row>
     <row r="139" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="34"/>
-      <c r="B139" s="35"/>
-      <c r="C139" s="35"/>
+      <c r="A139" s="40"/>
+      <c r="B139" s="38"/>
+      <c r="C139" s="38"/>
       <c r="D139" s="16" t="s">
         <v>157</v>
       </c>
@@ -3882,9 +3882,9 @@
       <c r="G139" s="15"/>
     </row>
     <row r="140" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A140" s="34"/>
-      <c r="B140" s="35"/>
-      <c r="C140" s="35"/>
+      <c r="A140" s="40"/>
+      <c r="B140" s="38"/>
+      <c r="C140" s="38"/>
       <c r="D140" s="16" t="s">
         <v>158</v>
       </c>
@@ -3896,17 +3896,17 @@
       </c>
       <c r="G140" s="15"/>
     </row>
-    <row r="141" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="10"/>
       <c r="B141" s="10"/>
       <c r="C141" s="10"/>
     </row>
-    <row r="142" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="35" t="s">
+    <row r="142" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="B142" s="35"/>
-      <c r="C142" s="35"/>
+      <c r="B142" s="38"/>
+      <c r="C142" s="38"/>
       <c r="D142" s="16" t="s">
         <v>160</v>
       </c>
@@ -3918,10 +3918,10 @@
       </c>
       <c r="G142" s="12"/>
     </row>
-    <row r="143" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="35"/>
-      <c r="B143" s="35"/>
-      <c r="C143" s="35"/>
+    <row r="143" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="38"/>
+      <c r="B143" s="38"/>
+      <c r="C143" s="38"/>
       <c r="D143" s="16" t="s">
         <v>160</v>
       </c>
@@ -3933,10 +3933,10 @@
       </c>
       <c r="G143" s="12"/>
     </row>
-    <row r="144" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="35"/>
-      <c r="B144" s="35"/>
-      <c r="C144" s="35"/>
+    <row r="144" spans="1:9" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="38"/>
+      <c r="B144" s="38"/>
+      <c r="C144" s="38"/>
       <c r="D144" s="16" t="s">
         <v>161</v>
       </c>
@@ -3948,10 +3948,10 @@
       </c>
       <c r="G144" s="12"/>
     </row>
-    <row r="145" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="35"/>
-      <c r="B145" s="35"/>
-      <c r="C145" s="35"/>
+    <row r="145" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="38"/>
+      <c r="B145" s="38"/>
+      <c r="C145" s="38"/>
       <c r="D145" s="16" t="s">
         <v>162</v>
       </c>
@@ -3963,10 +3963,10 @@
       </c>
       <c r="G145" s="13"/>
     </row>
-    <row r="146" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="35"/>
-      <c r="B146" s="35"/>
-      <c r="C146" s="35"/>
+    <row r="146" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="38"/>
+      <c r="B146" s="38"/>
+      <c r="C146" s="38"/>
       <c r="D146" s="16" t="s">
         <v>163</v>
       </c>
@@ -3978,10 +3978,10 @@
       </c>
       <c r="G146" s="13"/>
     </row>
-    <row r="147" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="7"/>
     </row>
-    <row r="148" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="10" t="s">
         <v>165</v>
       </c>
@@ -3995,15 +3995,15 @@
         <v>202</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="7"/>
     </row>
     <row r="150" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="35" t="s">
+      <c r="A150" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="B150" s="35"/>
-      <c r="C150" s="35"/>
+      <c r="B150" s="38"/>
+      <c r="C150" s="38"/>
       <c r="D150" s="16" t="s">
         <v>168</v>
       </c>
@@ -4018,9 +4018,9 @@
       </c>
     </row>
     <row r="151" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="35"/>
-      <c r="B151" s="35"/>
-      <c r="C151" s="35"/>
+      <c r="A151" s="38"/>
+      <c r="B151" s="38"/>
+      <c r="C151" s="38"/>
       <c r="D151" s="16" t="s">
         <v>169</v>
       </c>
@@ -4034,15 +4034,15 @@
         <v>200</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="7"/>
     </row>
     <row r="153" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="35" t="s">
+      <c r="A153" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="B153" s="36"/>
-      <c r="C153" s="36"/>
+      <c r="B153" s="39"/>
+      <c r="C153" s="39"/>
       <c r="D153" s="18" t="s">
         <v>171</v>
       </c>
@@ -4055,9 +4055,9 @@
       <c r="G153" s="2"/>
     </row>
     <row r="154" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="35"/>
-      <c r="B154" s="36"/>
-      <c r="C154" s="36"/>
+      <c r="A154" s="38"/>
+      <c r="B154" s="39"/>
+      <c r="C154" s="39"/>
       <c r="D154" s="18" t="s">
         <v>172</v>
       </c>
@@ -4070,9 +4070,9 @@
       <c r="G154" s="2"/>
     </row>
     <row r="155" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="35"/>
-      <c r="B155" s="36"/>
-      <c r="C155" s="36"/>
+      <c r="A155" s="38"/>
+      <c r="B155" s="39"/>
+      <c r="C155" s="39"/>
       <c r="D155" s="18" t="s">
         <v>173</v>
       </c>
@@ -4084,15 +4084,15 @@
       </c>
       <c r="G155" s="2"/>
     </row>
-    <row r="156" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="7"/>
     </row>
     <row r="157" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="35" t="s">
+      <c r="A157" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="B157" s="36"/>
-      <c r="C157" s="36"/>
+      <c r="B157" s="39"/>
+      <c r="C157" s="39"/>
       <c r="D157" s="18" t="s">
         <v>174</v>
       </c>
@@ -4107,9 +4107,9 @@
       </c>
     </row>
     <row r="158" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A158" s="35"/>
-      <c r="B158" s="36"/>
-      <c r="C158" s="36"/>
+      <c r="A158" s="38"/>
+      <c r="B158" s="39"/>
+      <c r="C158" s="39"/>
       <c r="D158" s="18" t="s">
         <v>175</v>
       </c>
@@ -4124,9 +4124,9 @@
       </c>
     </row>
     <row r="159" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A159" s="35"/>
-      <c r="B159" s="36"/>
-      <c r="C159" s="36"/>
+      <c r="A159" s="38"/>
+      <c r="B159" s="39"/>
+      <c r="C159" s="39"/>
       <c r="D159" s="18" t="s">
         <v>176</v>
       </c>
@@ -4140,15 +4140,15 @@
         <v>200</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="7"/>
     </row>
-    <row r="161" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="35" t="s">
+    <row r="161" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="B161" s="36"/>
-      <c r="C161" s="36"/>
+      <c r="B161" s="39"/>
+      <c r="C161" s="39"/>
       <c r="D161" s="18" t="s">
         <v>178</v>
       </c>
@@ -4160,10 +4160,10 @@
       </c>
       <c r="G161" s="2"/>
     </row>
-    <row r="162" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A162" s="35"/>
-      <c r="B162" s="36"/>
-      <c r="C162" s="36"/>
+    <row r="162" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="38"/>
+      <c r="B162" s="39"/>
+      <c r="C162" s="39"/>
       <c r="D162" s="18" t="s">
         <v>179</v>
       </c>
@@ -4176,9 +4176,9 @@
       <c r="G162" s="2"/>
     </row>
     <row r="163" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="35"/>
-      <c r="B163" s="36"/>
-      <c r="C163" s="36"/>
+      <c r="A163" s="38"/>
+      <c r="B163" s="39"/>
+      <c r="C163" s="39"/>
       <c r="D163" s="18" t="s">
         <v>180</v>
       </c>
@@ -4190,7 +4190,7 @@
       </c>
       <c r="G163" s="2"/>
     </row>
-    <row r="164" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="7"/>
     </row>
     <row r="165" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4212,15 +4212,15 @@
         <v>200</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="7"/>
     </row>
     <row r="167" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A167" s="35" t="s">
+      <c r="A167" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="B167" s="36"/>
-      <c r="C167" s="36"/>
+      <c r="B167" s="39"/>
+      <c r="C167" s="39"/>
       <c r="D167" s="18" t="s">
         <v>182</v>
       </c>
@@ -4235,9 +4235,9 @@
       </c>
     </row>
     <row r="168" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="35"/>
-      <c r="B168" s="36"/>
-      <c r="C168" s="36"/>
+      <c r="A168" s="38"/>
+      <c r="B168" s="39"/>
+      <c r="C168" s="39"/>
       <c r="D168" s="18" t="s">
         <v>183</v>
       </c>
@@ -4251,15 +4251,15 @@
         <v>202</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="7"/>
     </row>
     <row r="170" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A170" s="35" t="s">
+      <c r="A170" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="B170" s="36"/>
-      <c r="C170" s="36"/>
+      <c r="B170" s="39"/>
+      <c r="C170" s="39"/>
       <c r="D170" s="18" t="s">
         <v>185</v>
       </c>
@@ -4274,9 +4274,9 @@
       </c>
     </row>
     <row r="171" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="35"/>
-      <c r="B171" s="36"/>
-      <c r="C171" s="36"/>
+      <c r="A171" s="38"/>
+      <c r="B171" s="39"/>
+      <c r="C171" s="39"/>
       <c r="D171" s="18" t="s">
         <v>186</v>
       </c>
@@ -4291,9 +4291,9 @@
       </c>
     </row>
     <row r="172" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="35"/>
-      <c r="B172" s="36"/>
-      <c r="C172" s="36"/>
+      <c r="A172" s="38"/>
+      <c r="B172" s="39"/>
+      <c r="C172" s="39"/>
       <c r="D172" s="18" t="s">
         <v>187</v>
       </c>
@@ -4306,9 +4306,9 @@
       <c r="G172" s="3"/>
     </row>
     <row r="173" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A173" s="35"/>
-      <c r="B173" s="36"/>
-      <c r="C173" s="36"/>
+      <c r="A173" s="38"/>
+      <c r="B173" s="39"/>
+      <c r="C173" s="39"/>
       <c r="D173" s="18" t="s">
         <v>188</v>
       </c>
@@ -4320,15 +4320,15 @@
       </c>
       <c r="G173" s="3"/>
     </row>
-    <row r="174" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="7"/>
     </row>
     <row r="175" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A175" s="35" t="s">
+      <c r="A175" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="B175" s="35"/>
-      <c r="C175" s="35"/>
+      <c r="B175" s="38"/>
+      <c r="C175" s="38"/>
       <c r="D175" s="18" t="s">
         <v>190</v>
       </c>
@@ -4341,9 +4341,9 @@
       <c r="G175" s="2"/>
     </row>
     <row r="176" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A176" s="35"/>
-      <c r="B176" s="35"/>
-      <c r="C176" s="35"/>
+      <c r="A176" s="38"/>
+      <c r="B176" s="38"/>
+      <c r="C176" s="38"/>
       <c r="D176" s="18" t="s">
         <v>191</v>
       </c>
@@ -4356,9 +4356,9 @@
       <c r="G176" s="4"/>
     </row>
     <row r="177" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="35"/>
-      <c r="B177" s="35"/>
-      <c r="C177" s="35"/>
+      <c r="A177" s="38"/>
+      <c r="B177" s="38"/>
+      <c r="C177" s="38"/>
       <c r="D177" s="18" t="s">
         <v>192</v>
       </c>
@@ -4370,10 +4370,10 @@
       </c>
       <c r="G177" s="3"/>
     </row>
-    <row r="178" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="7"/>
     </row>
-    <row r="179" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="10" t="s">
         <v>193</v>
       </c>
@@ -4390,10 +4390,10 @@
       </c>
       <c r="G179" s="2"/>
     </row>
-    <row r="180" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="7"/>
     </row>
-    <row r="181" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="7"/>
       <c r="D181" s="18" t="s">
         <v>195</v>
@@ -4406,7 +4406,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="7"/>
       <c r="D182" s="18" t="s">
         <v>196</v>
@@ -4419,7 +4419,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="7"/>
       <c r="D183" s="18" t="s">
         <v>197</v>
@@ -4440,34 +4440,48 @@
         <filter val="Only TV"/>
       </filters>
     </filterColumn>
+    <filterColumn colId="1">
+      <filters>
+        <filter val="GET"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="High"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <mergeCells count="72">
-    <mergeCell ref="A175:A177"/>
-    <mergeCell ref="B175:B177"/>
-    <mergeCell ref="C175:C177"/>
-    <mergeCell ref="A167:A168"/>
-    <mergeCell ref="B167:B168"/>
-    <mergeCell ref="C167:C168"/>
-    <mergeCell ref="A170:A173"/>
-    <mergeCell ref="B170:B173"/>
-    <mergeCell ref="C170:C173"/>
-    <mergeCell ref="A157:A159"/>
-    <mergeCell ref="B157:B159"/>
-    <mergeCell ref="C157:C159"/>
-    <mergeCell ref="A161:A163"/>
-    <mergeCell ref="B161:B163"/>
-    <mergeCell ref="C161:C163"/>
-    <mergeCell ref="C150:C151"/>
-    <mergeCell ref="B150:B151"/>
-    <mergeCell ref="A150:A151"/>
-    <mergeCell ref="A153:A155"/>
-    <mergeCell ref="B153:B155"/>
-    <mergeCell ref="C153:C155"/>
-    <mergeCell ref="B120:B123"/>
-    <mergeCell ref="C120:C123"/>
-    <mergeCell ref="C124:C140"/>
-    <mergeCell ref="B124:B140"/>
-    <mergeCell ref="A120:A140"/>
+    <mergeCell ref="L1:L1048576"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="A44:A98"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B67:B98"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="C61:C63"/>
+    <mergeCell ref="C64:C66"/>
+    <mergeCell ref="C67:C98"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="C5:C19"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A5:A19"/>
+    <mergeCell ref="B5:B19"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="C142:C146"/>
     <mergeCell ref="B142:B146"/>
     <mergeCell ref="A142:A146"/>
@@ -4484,36 +4498,32 @@
     <mergeCell ref="B61:B63"/>
     <mergeCell ref="B56:B60"/>
     <mergeCell ref="B44:B47"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="C5:C19"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="A5:A19"/>
-    <mergeCell ref="B5:B19"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="L1:L1048576"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="A44:A98"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="B67:B98"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="C61:C63"/>
-    <mergeCell ref="C64:C66"/>
-    <mergeCell ref="C67:C98"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B120:B123"/>
+    <mergeCell ref="C120:C123"/>
+    <mergeCell ref="C124:C140"/>
+    <mergeCell ref="B124:B140"/>
+    <mergeCell ref="A120:A140"/>
+    <mergeCell ref="C150:C151"/>
+    <mergeCell ref="B150:B151"/>
+    <mergeCell ref="A150:A151"/>
+    <mergeCell ref="A153:A155"/>
+    <mergeCell ref="B153:B155"/>
+    <mergeCell ref="C153:C155"/>
+    <mergeCell ref="A157:A159"/>
+    <mergeCell ref="B157:B159"/>
+    <mergeCell ref="C157:C159"/>
+    <mergeCell ref="A161:A163"/>
+    <mergeCell ref="B161:B163"/>
+    <mergeCell ref="C161:C163"/>
+    <mergeCell ref="A175:A177"/>
+    <mergeCell ref="B175:B177"/>
+    <mergeCell ref="C175:C177"/>
+    <mergeCell ref="A167:A168"/>
+    <mergeCell ref="B167:B168"/>
+    <mergeCell ref="C167:C168"/>
+    <mergeCell ref="A170:A173"/>
+    <mergeCell ref="B170:B173"/>
+    <mergeCell ref="C170:C173"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>